<commit_message>
AI schools & colleges worksheet checked in
AI schools & colleges worksheet checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F35F05D-1F79-4CDF-B824-891651159FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -20,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'School-Details'!$A$1:$U$122</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,13 +40,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L28" authorId="1" shapeId="0">
+    <comment ref="L28" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -88,12 +89,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -122,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="437">
   <si>
     <t>CBSE</t>
   </si>
@@ -1450,7 +1451,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1775,7 +1776,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1872,26 +1873,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1912,6 +1893,24 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2193,11 +2192,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2221,33 +2220,27 @@
     <row r="2" spans="2:18" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="54" t="s">
         <v>293</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="56"/>
       <c r="I2" s="29"/>
       <c r="K2" s="27"/>
       <c r="L2" s="28"/>
-      <c r="M2" s="49" t="s">
+      <c r="M2" s="54" t="s">
         <v>374</v>
       </c>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="51"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="56"/>
       <c r="R2" s="29"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="30"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
       <c r="I3" s="31"/>
       <c r="K3" s="30"/>
       <c r="R3" s="31"/>
@@ -2261,14 +2254,12 @@
         <f>MAX('School-Details'!A:A)</f>
         <v>235</v>
       </c>
-      <c r="E4" s="46"/>
       <c r="F4" s="21" t="s">
         <v>265</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="H4" s="46"/>
       <c r="I4" s="31"/>
       <c r="K4" s="30"/>
       <c r="L4" s="16" t="s">
@@ -2295,7 +2286,6 @@
         <f>ROUND(SUM('School-Details'!K:K)/D4,2)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="46"/>
       <c r="F5" s="14" t="s">
         <v>210</v>
       </c>
@@ -2303,7 +2293,6 @@
         <f>COUNTIF('School-Details'!M:M,F5)</f>
         <v>0</v>
       </c>
-      <c r="H5" s="46"/>
       <c r="I5" s="31"/>
       <c r="K5" s="30"/>
       <c r="L5" s="16" t="s">
@@ -2324,9 +2313,6 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
       <c r="F6" s="14" t="s">
         <v>267</v>
       </c>
@@ -2334,7 +2320,6 @@
         <f>COUNTIF('School-Details'!M:M,F6)</f>
         <v>1</v>
       </c>
-      <c r="H6" s="46"/>
       <c r="I6" s="31"/>
       <c r="K6" s="30"/>
       <c r="L6" s="16" t="s">
@@ -2342,7 +2327,7 @@
       </c>
       <c r="M6" s="16">
         <f>MAX('College-Details'!A:A)</f>
-        <v>174</v>
+        <v>53</v>
       </c>
       <c r="O6" s="14" t="s">
         <v>267</v>
@@ -2361,7 +2346,6 @@
       <c r="D7" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="E7" s="46"/>
       <c r="F7" s="14" t="s">
         <v>268</v>
       </c>
@@ -2369,7 +2353,6 @@
         <f>COUNTIF('School-Details'!M:M,F7)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="46"/>
       <c r="I7" s="31"/>
       <c r="K7" s="30"/>
       <c r="L7" s="16" t="s">
@@ -2397,7 +2380,6 @@
         <f>COUNTIF('School-Details'!U:U,C8)</f>
         <v>13</v>
       </c>
-      <c r="E8" s="46"/>
       <c r="F8" s="14" t="s">
         <v>283</v>
       </c>
@@ -2405,7 +2387,6 @@
         <f>COUNTIF('School-Details'!M:M,F8)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="46"/>
       <c r="I8" s="31"/>
       <c r="K8" s="30"/>
       <c r="O8" s="14" t="s">
@@ -2426,10 +2407,6 @@
         <f>COUNTIF('School-Details'!U:U,C9)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
       <c r="I9" s="31"/>
       <c r="K9" s="30"/>
       <c r="L9" s="21" t="s">
@@ -2456,12 +2433,11 @@
         <f>COUNTIF('School-Details'!U:U,C10)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="46"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="53" t="s">
         <v>210</v>
       </c>
-      <c r="H10" s="48"/>
+      <c r="H10" s="53"/>
       <c r="I10" s="31"/>
       <c r="K10" s="30"/>
       <c r="L10" s="14" t="s">
@@ -2482,7 +2458,6 @@
         <f>COUNTIF('School-Details'!U:U,C11)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="46"/>
       <c r="F11" s="21" t="s">
         <v>269</v>
       </c>
@@ -2502,10 +2477,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="14"/>
-      <c r="P11" s="52" t="s">
+      <c r="P11" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="Q11" s="53"/>
+      <c r="Q11" s="58"/>
       <c r="R11" s="31"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
@@ -2517,7 +2492,6 @@
         <f>COUNTIF('School-Details'!U:U,C12)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="46"/>
       <c r="F12" s="22">
         <v>45292</v>
       </c>
@@ -2556,7 +2530,6 @@
         <f>COUNTIF('School-Details'!U:U,C13)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="46"/>
       <c r="F13" s="22">
         <v>45323</v>
       </c>
@@ -2595,7 +2568,6 @@
         <f>COUNTIF('School-Details'!U:U,C14)</f>
         <v>108</v>
       </c>
-      <c r="E14" s="46"/>
       <c r="F14" s="22">
         <v>45352</v>
       </c>
@@ -2634,7 +2606,6 @@
         <f>COUNTIF('School-Details'!U:U,C15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="46"/>
       <c r="F15" s="22">
         <v>45383</v>
       </c>
@@ -2666,14 +2637,13 @@
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="30"/>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="16" t="s">
         <v>244</v>
       </c>
       <c r="D16" s="16">
         <f>SUM(D8:D15)</f>
         <v>121</v>
       </c>
-      <c r="E16" s="46"/>
       <c r="F16" s="22">
         <v>45413</v>
       </c>
@@ -2690,7 +2660,7 @@
       </c>
       <c r="M16" s="14">
         <f>COUNTIF('College-Details'!T:T,L16)</f>
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="O16" s="22">
         <v>45383</v>
@@ -2705,9 +2675,6 @@
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="30"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
       <c r="F17" s="22">
         <v>45444</v>
       </c>
@@ -2745,7 +2712,6 @@
       <c r="D18" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="E18" s="46"/>
       <c r="F18" s="22">
         <v>45474</v>
       </c>
@@ -2762,7 +2728,7 @@
       </c>
       <c r="M18" s="16">
         <f>SUM(M10:M17)</f>
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="O18" s="22">
         <v>45444</v>
@@ -2786,7 +2752,6 @@
         <f>COUNTIF('School-Details'!T:T,C19)</f>
         <v>10</v>
       </c>
-      <c r="E19" s="46"/>
       <c r="F19" s="22">
         <v>45505</v>
       </c>
@@ -2818,7 +2783,6 @@
         <f>COUNTIF('School-Details'!T:T,C20)</f>
         <v>51</v>
       </c>
-      <c r="E20" s="46"/>
       <c r="F20" s="22">
         <v>45536</v>
       </c>
@@ -2856,7 +2820,6 @@
         <f>SUM(D19:D20)</f>
         <v>61</v>
       </c>
-      <c r="E21" s="46"/>
       <c r="F21" s="22">
         <v>45566</v>
       </c>
@@ -2899,7 +2862,6 @@
         <f>COUNTIF('School-Details'!T:T,C22)</f>
         <v>50</v>
       </c>
-      <c r="E22" s="46"/>
       <c r="F22" s="22">
         <v>45597</v>
       </c>
@@ -2938,7 +2900,6 @@
         <f>SUM(D22)</f>
         <v>50</v>
       </c>
-      <c r="E23" s="46"/>
       <c r="F23" s="22">
         <v>45627</v>
       </c>
@@ -2979,7 +2940,6 @@
         <f>COUNTIF('School-Details'!T:T,C24)</f>
         <v>10</v>
       </c>
-      <c r="E24" s="46"/>
       <c r="F24" s="16" t="s">
         <v>244</v>
       </c>
@@ -3022,10 +2982,6 @@
         <f>COUNTIF('School-Details'!T:T,C25)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
       <c r="I25" s="31"/>
       <c r="K25" s="33"/>
       <c r="L25" s="14" t="s">
@@ -3057,10 +3013,6 @@
         <f>SUM(D24:D25)</f>
         <v>10</v>
       </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
       <c r="I26" s="31"/>
       <c r="K26" s="33" t="s">
         <v>273</v>
@@ -3083,10 +3035,6 @@
         <f>D21+D23+D26</f>
         <v>121</v>
       </c>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
       <c r="I27" s="31"/>
       <c r="K27" s="33"/>
       <c r="L27" s="14">
@@ -3151,7 +3099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U236"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8776,68 +8724,68 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U122"/>
+  <autoFilter ref="A1:U122" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1"/>
-    <hyperlink ref="D32" r:id="rId2"/>
-    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp"/>
-    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w"/>
-    <hyperlink ref="D22" r:id="rId5"/>
-    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com"/>
-    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in"/>
-    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com"/>
-    <hyperlink ref="D30" r:id="rId9"/>
-    <hyperlink ref="D33" r:id="rId10"/>
-    <hyperlink ref="D35" r:id="rId11"/>
-    <hyperlink ref="D37" r:id="rId12"/>
-    <hyperlink ref="D41" r:id="rId13"/>
-    <hyperlink ref="D42" r:id="rId14"/>
-    <hyperlink ref="D43" r:id="rId15"/>
-    <hyperlink ref="D47" r:id="rId16"/>
-    <hyperlink ref="D48" r:id="rId17"/>
-    <hyperlink ref="D49" r:id="rId18"/>
-    <hyperlink ref="D51" r:id="rId19"/>
-    <hyperlink ref="D52" r:id="rId20"/>
-    <hyperlink ref="D53" r:id="rId21"/>
-    <hyperlink ref="D54" r:id="rId22"/>
-    <hyperlink ref="D55" r:id="rId23"/>
-    <hyperlink ref="D56" r:id="rId24"/>
-    <hyperlink ref="D57" r:id="rId25"/>
-    <hyperlink ref="D58" r:id="rId26"/>
-    <hyperlink ref="D59" r:id="rId27"/>
-    <hyperlink ref="D60" r:id="rId28"/>
-    <hyperlink ref="D61" r:id="rId29"/>
-    <hyperlink ref="D62" r:id="rId30"/>
-    <hyperlink ref="D63" r:id="rId31"/>
-    <hyperlink ref="D64" r:id="rId32"/>
-    <hyperlink ref="D65" r:id="rId33"/>
-    <hyperlink ref="D66" r:id="rId34"/>
-    <hyperlink ref="D67" r:id="rId35"/>
-    <hyperlink ref="D68" r:id="rId36"/>
-    <hyperlink ref="D69" r:id="rId37"/>
-    <hyperlink ref="D70" r:id="rId38"/>
-    <hyperlink ref="D71" r:id="rId39"/>
-    <hyperlink ref="D72" r:id="rId40"/>
-    <hyperlink ref="D73" r:id="rId41"/>
-    <hyperlink ref="D75" r:id="rId42"/>
-    <hyperlink ref="D78" r:id="rId43"/>
-    <hyperlink ref="D79" r:id="rId44"/>
-    <hyperlink ref="D80" r:id="rId45"/>
-    <hyperlink ref="D81" r:id="rId46"/>
-    <hyperlink ref="D85" r:id="rId47"/>
-    <hyperlink ref="D88" r:id="rId48"/>
-    <hyperlink ref="D89" r:id="rId49"/>
-    <hyperlink ref="D91" r:id="rId50"/>
-    <hyperlink ref="D2" r:id="rId51"/>
-    <hyperlink ref="D28" r:id="rId52"/>
+    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D32" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D22" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="D30" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D33" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="D35" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D37" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="D41" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="D42" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="D43" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="D47" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D48" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="D49" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="D51" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="D53" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="D54" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="D55" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="D56" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="D57" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="D58" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="D59" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="D60" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="D61" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="D62" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="D63" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="D64" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="D65" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="D66" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="D67" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="D68" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="D69" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="D70" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="D71" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="D72" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="D73" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="D75" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="D78" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="D79" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="D80" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="D81" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="D85" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="D88" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="D89" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="D91" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="D2" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="D28" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId53"/>
@@ -8846,11 +8794,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9289,7 +9237,7 @@
       <c r="B11" s="38" t="s">
         <v>320</v>
       </c>
-      <c r="C11" s="58"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="39" t="s">
         <v>321</v>
       </c>
@@ -9614,7 +9562,7 @@
       <c r="B20" s="38" t="s">
         <v>335</v>
       </c>
-      <c r="C20" s="59"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="43" t="s">
         <v>336</v>
       </c>
@@ -9651,7 +9599,7 @@
       <c r="B21" s="44" t="s">
         <v>337</v>
       </c>
-      <c r="C21" s="54"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="39" t="s">
         <v>338</v>
       </c>
@@ -9724,7 +9672,7 @@
       <c r="B23" s="38" t="s">
         <v>341</v>
       </c>
-      <c r="C23" s="60"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="39" t="s">
         <v>342</v>
       </c>
@@ -9761,7 +9709,7 @@
       <c r="B24" s="38" t="s">
         <v>343</v>
       </c>
-      <c r="C24" s="57"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="39" t="s">
         <v>344</v>
       </c>
@@ -9798,7 +9746,7 @@
       <c r="B25" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="C25" s="57"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="39" t="s">
         <v>346</v>
       </c>
@@ -9835,7 +9783,7 @@
       <c r="B26" s="38" t="s">
         <v>347</v>
       </c>
-      <c r="C26" s="57"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="39" t="s">
         <v>348</v>
       </c>
@@ -9944,7 +9892,7 @@
       <c r="B29" s="38" t="s">
         <v>353</v>
       </c>
-      <c r="C29" s="54"/>
+      <c r="C29" s="46"/>
       <c r="D29" s="39" t="s">
         <v>354</v>
       </c>
@@ -9981,7 +9929,7 @@
       <c r="B30" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="C30" s="54"/>
+      <c r="C30" s="46"/>
       <c r="D30" s="39" t="s">
         <v>356</v>
       </c>
@@ -10018,7 +9966,7 @@
       <c r="B31" s="38" t="s">
         <v>357</v>
       </c>
-      <c r="C31" s="54"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="39" t="s">
         <v>358</v>
       </c>
@@ -10199,7 +10147,7 @@
       <c r="B36" s="38" t="s">
         <v>376</v>
       </c>
-      <c r="C36" s="54" t="s">
+      <c r="C36" s="46" t="s">
         <v>377</v>
       </c>
       <c r="D36" s="39" t="s">
@@ -10208,13 +10156,31 @@
       <c r="E36" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
+      <c r="M36" s="10">
+        <v>0</v>
+      </c>
+      <c r="N36" s="10">
+        <v>0</v>
+      </c>
+      <c r="O36" s="10">
+        <v>0</v>
+      </c>
+      <c r="P36" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="10">
+        <v>0</v>
+      </c>
+      <c r="R36" s="10">
+        <v>0</v>
+      </c>
+      <c r="S36" s="10">
+        <f t="shared" ref="S36:S54" si="1">ROUND(R36/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="T36" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
@@ -10223,7 +10189,7 @@
       <c r="B37" s="38" t="s">
         <v>382</v>
       </c>
-      <c r="C37" s="54" t="s">
+      <c r="C37" s="46" t="s">
         <v>381</v>
       </c>
       <c r="D37" s="39" t="s">
@@ -10232,13 +10198,31 @@
       <c r="E37" s="40" t="s">
         <v>383</v>
       </c>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
+      <c r="M37" s="10">
+        <v>0</v>
+      </c>
+      <c r="N37" s="10">
+        <v>0</v>
+      </c>
+      <c r="O37" s="10">
+        <v>0</v>
+      </c>
+      <c r="P37" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="10">
+        <v>0</v>
+      </c>
+      <c r="R37" s="10">
+        <v>0</v>
+      </c>
+      <c r="S37" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T37" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="38" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
@@ -10253,13 +10237,31 @@
       <c r="E38" s="40" t="s">
         <v>387</v>
       </c>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
+      <c r="M38" s="10">
+        <v>0</v>
+      </c>
+      <c r="N38" s="10">
+        <v>0</v>
+      </c>
+      <c r="O38" s="10">
+        <v>0</v>
+      </c>
+      <c r="P38" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="10">
+        <v>0</v>
+      </c>
+      <c r="R38" s="10">
+        <v>0</v>
+      </c>
+      <c r="S38" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T38" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="39" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
@@ -10274,13 +10276,31 @@
       <c r="E39" s="40" t="s">
         <v>389</v>
       </c>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
+      <c r="M39" s="10">
+        <v>0</v>
+      </c>
+      <c r="N39" s="10">
+        <v>0</v>
+      </c>
+      <c r="O39" s="10">
+        <v>0</v>
+      </c>
+      <c r="P39" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="10">
+        <v>0</v>
+      </c>
+      <c r="R39" s="10">
+        <v>0</v>
+      </c>
+      <c r="S39" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="40" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
@@ -10295,13 +10315,31 @@
       <c r="E40" s="40" t="s">
         <v>391</v>
       </c>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
+      <c r="M40" s="10">
+        <v>0</v>
+      </c>
+      <c r="N40" s="10">
+        <v>0</v>
+      </c>
+      <c r="O40" s="10">
+        <v>0</v>
+      </c>
+      <c r="P40" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="10">
+        <v>0</v>
+      </c>
+      <c r="R40" s="10">
+        <v>0</v>
+      </c>
+      <c r="S40" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T40" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
@@ -10310,19 +10348,37 @@
       <c r="B41" s="38" t="s">
         <v>393</v>
       </c>
-      <c r="D41" s="55" t="s">
+      <c r="D41" s="47" t="s">
         <v>394</v>
       </c>
       <c r="E41" s="40" t="s">
         <v>395</v>
       </c>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
+      <c r="M41" s="10">
+        <v>0</v>
+      </c>
+      <c r="N41" s="10">
+        <v>0</v>
+      </c>
+      <c r="O41" s="10">
+        <v>0</v>
+      </c>
+      <c r="P41" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="10">
+        <v>0</v>
+      </c>
+      <c r="R41" s="10">
+        <v>0</v>
+      </c>
+      <c r="S41" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T41" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
@@ -10337,13 +10393,31 @@
       <c r="E42" s="40" t="s">
         <v>398</v>
       </c>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="10"/>
+      <c r="M42" s="10">
+        <v>0</v>
+      </c>
+      <c r="N42" s="10">
+        <v>0</v>
+      </c>
+      <c r="O42" s="10">
+        <v>0</v>
+      </c>
+      <c r="P42" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="10">
+        <v>0</v>
+      </c>
+      <c r="R42" s="10">
+        <v>0</v>
+      </c>
+      <c r="S42" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T42" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="43" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
@@ -10352,7 +10426,7 @@
       <c r="B43" s="38" t="s">
         <v>400</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="48" t="s">
         <v>399</v>
       </c>
       <c r="D43" s="39" t="s">
@@ -10361,13 +10435,31 @@
       <c r="E43" s="40" t="s">
         <v>402</v>
       </c>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
+      <c r="M43" s="10">
+        <v>0</v>
+      </c>
+      <c r="N43" s="10">
+        <v>0</v>
+      </c>
+      <c r="O43" s="10">
+        <v>0</v>
+      </c>
+      <c r="P43" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="10">
+        <v>0</v>
+      </c>
+      <c r="R43" s="10">
+        <v>0</v>
+      </c>
+      <c r="S43" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T43" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="44" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
@@ -10382,13 +10474,31 @@
       <c r="E44" s="40" t="s">
         <v>405</v>
       </c>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
+      <c r="M44" s="10">
+        <v>0</v>
+      </c>
+      <c r="N44" s="10">
+        <v>0</v>
+      </c>
+      <c r="O44" s="10">
+        <v>0</v>
+      </c>
+      <c r="P44" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="10">
+        <v>0</v>
+      </c>
+      <c r="R44" s="10">
+        <v>0</v>
+      </c>
+      <c r="S44" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T44" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
@@ -10403,13 +10513,31 @@
       <c r="E45" s="40" t="s">
         <v>407</v>
       </c>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-      <c r="S45" s="10"/>
+      <c r="M45" s="10">
+        <v>0</v>
+      </c>
+      <c r="N45" s="10">
+        <v>0</v>
+      </c>
+      <c r="O45" s="10">
+        <v>0</v>
+      </c>
+      <c r="P45" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="10">
+        <v>0</v>
+      </c>
+      <c r="R45" s="10">
+        <v>0</v>
+      </c>
+      <c r="S45" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T45" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="46" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
@@ -10424,13 +10552,31 @@
       <c r="E46" s="40" t="s">
         <v>411</v>
       </c>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-      <c r="S46" s="10"/>
+      <c r="M46" s="10">
+        <v>0</v>
+      </c>
+      <c r="N46" s="10">
+        <v>0</v>
+      </c>
+      <c r="O46" s="10">
+        <v>0</v>
+      </c>
+      <c r="P46" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="10">
+        <v>0</v>
+      </c>
+      <c r="R46" s="10">
+        <v>0</v>
+      </c>
+      <c r="S46" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T46" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="47" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
@@ -10439,19 +10585,37 @@
       <c r="B47" s="38" t="s">
         <v>412</v>
       </c>
-      <c r="D47" s="55" t="s">
+      <c r="D47" s="47" t="s">
         <v>413</v>
       </c>
       <c r="E47" s="40" t="s">
         <v>414</v>
       </c>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="10"/>
+      <c r="M47" s="10">
+        <v>0</v>
+      </c>
+      <c r="N47" s="10">
+        <v>0</v>
+      </c>
+      <c r="O47" s="10">
+        <v>0</v>
+      </c>
+      <c r="P47" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="10">
+        <v>0</v>
+      </c>
+      <c r="R47" s="10">
+        <v>0</v>
+      </c>
+      <c r="S47" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T47" s="10" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="48" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
@@ -10466,22 +10630,40 @@
       <c r="E48" s="40" t="s">
         <v>407</v>
       </c>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10"/>
-      <c r="S48" s="10"/>
-    </row>
-    <row r="49" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M48" s="10">
+        <v>0</v>
+      </c>
+      <c r="N48" s="10">
+        <v>0</v>
+      </c>
+      <c r="O48" s="10">
+        <v>0</v>
+      </c>
+      <c r="P48" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="10">
+        <v>0</v>
+      </c>
+      <c r="R48" s="10">
+        <v>0</v>
+      </c>
+      <c r="S48" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T48" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="B49" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="C49" s="56" t="s">
+      <c r="C49" s="48" t="s">
         <v>419</v>
       </c>
       <c r="D49" s="39" t="s">
@@ -10490,15 +10672,33 @@
       <c r="E49" s="40" t="s">
         <v>422</v>
       </c>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="10"/>
-      <c r="R49" s="10"/>
-      <c r="S49" s="10"/>
-    </row>
-    <row r="50" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M49" s="10">
+        <v>0</v>
+      </c>
+      <c r="N49" s="10">
+        <v>0</v>
+      </c>
+      <c r="O49" s="10">
+        <v>0</v>
+      </c>
+      <c r="P49" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="10">
+        <v>0</v>
+      </c>
+      <c r="R49" s="10">
+        <v>0</v>
+      </c>
+      <c r="S49" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T49" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -10511,15 +10711,33 @@
       <c r="E50" s="40" t="s">
         <v>407</v>
       </c>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="10"/>
-    </row>
-    <row r="51" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="M50" s="10">
+        <v>0</v>
+      </c>
+      <c r="N50" s="10">
+        <v>0</v>
+      </c>
+      <c r="O50" s="10">
+        <v>0</v>
+      </c>
+      <c r="P50" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="10">
+        <v>0</v>
+      </c>
+      <c r="R50" s="10">
+        <v>0</v>
+      </c>
+      <c r="S50" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T50" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -10532,15 +10750,33 @@
       <c r="E51" s="40" t="s">
         <v>424</v>
       </c>
-      <c r="M51" s="10"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="10"/>
-      <c r="S51" s="10"/>
-    </row>
-    <row r="52" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="M51" s="10">
+        <v>0</v>
+      </c>
+      <c r="N51" s="10">
+        <v>0</v>
+      </c>
+      <c r="O51" s="10">
+        <v>0</v>
+      </c>
+      <c r="P51" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="10">
+        <v>0</v>
+      </c>
+      <c r="R51" s="10">
+        <v>0</v>
+      </c>
+      <c r="S51" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T51" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -10553,15 +10789,33 @@
       <c r="E52" s="40" t="s">
         <v>432</v>
       </c>
-      <c r="M52" s="10"/>
-      <c r="N52" s="10"/>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10"/>
-      <c r="Q52" s="10"/>
-      <c r="R52" s="10"/>
-      <c r="S52" s="10"/>
-    </row>
-    <row r="53" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M52" s="10">
+        <v>0</v>
+      </c>
+      <c r="N52" s="10">
+        <v>0</v>
+      </c>
+      <c r="O52" s="10">
+        <v>0</v>
+      </c>
+      <c r="P52" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="10">
+        <v>0</v>
+      </c>
+      <c r="R52" s="10">
+        <v>0</v>
+      </c>
+      <c r="S52" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T52" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -10574,15 +10828,33 @@
       <c r="E53" s="40" t="s">
         <v>424</v>
       </c>
-      <c r="M53" s="10"/>
-      <c r="N53" s="10"/>
-      <c r="O53" s="10"/>
-      <c r="P53" s="10"/>
-      <c r="Q53" s="10"/>
-      <c r="R53" s="10"/>
-      <c r="S53" s="10"/>
-    </row>
-    <row r="54" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="M53" s="10">
+        <v>0</v>
+      </c>
+      <c r="N53" s="10">
+        <v>0</v>
+      </c>
+      <c r="O53" s="10">
+        <v>0</v>
+      </c>
+      <c r="P53" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="10">
+        <v>0</v>
+      </c>
+      <c r="R53" s="10">
+        <v>0</v>
+      </c>
+      <c r="S53" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T53" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -10595,18 +10867,33 @@
       <c r="E54" s="40" t="s">
         <v>414</v>
       </c>
-      <c r="M54" s="10"/>
-      <c r="N54" s="10"/>
-      <c r="O54" s="10"/>
-      <c r="P54" s="10"/>
-      <c r="Q54" s="10"/>
-      <c r="R54" s="10"/>
-      <c r="S54" s="10"/>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>54</v>
-      </c>
+      <c r="M54" s="10">
+        <v>0</v>
+      </c>
+      <c r="N54" s="10">
+        <v>0</v>
+      </c>
+      <c r="O54" s="10">
+        <v>0</v>
+      </c>
+      <c r="P54" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="10">
+        <v>0</v>
+      </c>
+      <c r="R54" s="10">
+        <v>0</v>
+      </c>
+      <c r="S54" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T54" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M55" s="10"/>
       <c r="N55" s="10"/>
       <c r="O55" s="10"/>
@@ -10615,10 +10902,7 @@
       <c r="R55" s="10"/>
       <c r="S55" s="10"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>55</v>
-      </c>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
       <c r="O56" s="10"/>
@@ -10627,10 +10911,7 @@
       <c r="R56" s="10"/>
       <c r="S56" s="10"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>56</v>
-      </c>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M57" s="10"/>
       <c r="N57" s="10"/>
       <c r="O57" s="10"/>
@@ -10639,10 +10920,7 @@
       <c r="R57" s="10"/>
       <c r="S57" s="10"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>57</v>
-      </c>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M58" s="10"/>
       <c r="N58" s="10"/>
       <c r="O58" s="10"/>
@@ -10651,10 +10929,7 @@
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>58</v>
-      </c>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M59" s="10"/>
       <c r="N59" s="10"/>
       <c r="O59" s="10"/>
@@ -10663,10 +10938,7 @@
       <c r="R59" s="10"/>
       <c r="S59" s="10"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>59</v>
-      </c>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M60" s="10"/>
       <c r="N60" s="10"/>
       <c r="O60" s="10"/>
@@ -10675,10 +10947,7 @@
       <c r="R60" s="10"/>
       <c r="S60" s="10"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>60</v>
-      </c>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M61" s="10"/>
       <c r="N61" s="10"/>
       <c r="O61" s="10"/>
@@ -10687,10 +10956,7 @@
       <c r="R61" s="10"/>
       <c r="S61" s="10"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>61</v>
-      </c>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M62" s="10"/>
       <c r="N62" s="10"/>
       <c r="O62" s="10"/>
@@ -10699,10 +10965,7 @@
       <c r="R62" s="10"/>
       <c r="S62" s="10"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
-        <v>62</v>
-      </c>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M63" s="10"/>
       <c r="N63" s="10"/>
       <c r="O63" s="10"/>
@@ -10711,10 +10974,7 @@
       <c r="R63" s="10"/>
       <c r="S63" s="10"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
-        <v>63</v>
-      </c>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
       <c r="O64" s="10"/>
@@ -10723,10 +10983,7 @@
       <c r="R64" s="10"/>
       <c r="S64" s="10"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
-        <v>64</v>
-      </c>
+    <row r="65" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
       <c r="O65" s="10"/>
@@ -10735,10 +10992,7 @@
       <c r="R65" s="10"/>
       <c r="S65" s="10"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
-        <v>65</v>
-      </c>
+    <row r="66" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M66" s="10"/>
       <c r="N66" s="10"/>
       <c r="O66" s="10"/>
@@ -10747,10 +11001,7 @@
       <c r="R66" s="10"/>
       <c r="S66" s="10"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>66</v>
-      </c>
+    <row r="67" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
       <c r="O67" s="10"/>
@@ -10759,10 +11010,7 @@
       <c r="R67" s="10"/>
       <c r="S67" s="10"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
-        <v>67</v>
-      </c>
+    <row r="68" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M68" s="10"/>
       <c r="N68" s="10"/>
       <c r="O68" s="10"/>
@@ -10771,10 +11019,7 @@
       <c r="R68" s="10"/>
       <c r="S68" s="10"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>68</v>
-      </c>
+    <row r="69" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M69" s="10"/>
       <c r="N69" s="10"/>
       <c r="O69" s="10"/>
@@ -10783,10 +11028,7 @@
       <c r="R69" s="10"/>
       <c r="S69" s="10"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
-        <v>69</v>
-      </c>
+    <row r="70" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M70" s="10"/>
       <c r="N70" s="10"/>
       <c r="O70" s="10"/>
@@ -10795,10 +11037,7 @@
       <c r="R70" s="10"/>
       <c r="S70" s="10"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
-        <v>70</v>
-      </c>
+    <row r="71" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M71" s="10"/>
       <c r="N71" s="10"/>
       <c r="O71" s="10"/>
@@ -10807,10 +11046,7 @@
       <c r="R71" s="10"/>
       <c r="S71" s="10"/>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
-        <v>71</v>
-      </c>
+    <row r="72" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M72" s="10"/>
       <c r="N72" s="10"/>
       <c r="O72" s="10"/>
@@ -10819,10 +11055,7 @@
       <c r="R72" s="10"/>
       <c r="S72" s="10"/>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A73" s="2">
-        <v>72</v>
-      </c>
+    <row r="73" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M73" s="10"/>
       <c r="N73" s="10"/>
       <c r="O73" s="10"/>
@@ -10831,10 +11064,7 @@
       <c r="R73" s="10"/>
       <c r="S73" s="10"/>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A74" s="2">
-        <v>73</v>
-      </c>
+    <row r="74" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M74" s="10"/>
       <c r="N74" s="10"/>
       <c r="O74" s="10"/>
@@ -10843,10 +11073,7 @@
       <c r="R74" s="10"/>
       <c r="S74" s="10"/>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
-        <v>74</v>
-      </c>
+    <row r="75" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M75" s="10"/>
       <c r="N75" s="10"/>
       <c r="O75" s="10"/>
@@ -10855,10 +11082,7 @@
       <c r="R75" s="10"/>
       <c r="S75" s="10"/>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
-        <v>75</v>
-      </c>
+    <row r="76" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M76" s="10"/>
       <c r="N76" s="10"/>
       <c r="O76" s="10"/>
@@ -10867,10 +11091,7 @@
       <c r="R76" s="10"/>
       <c r="S76" s="10"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
-        <v>76</v>
-      </c>
+    <row r="77" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M77" s="10"/>
       <c r="N77" s="10"/>
       <c r="O77" s="10"/>
@@ -10879,10 +11100,7 @@
       <c r="R77" s="10"/>
       <c r="S77" s="10"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
-        <v>77</v>
-      </c>
+    <row r="78" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M78" s="10"/>
       <c r="N78" s="10"/>
       <c r="O78" s="10"/>
@@ -10891,10 +11109,7 @@
       <c r="R78" s="10"/>
       <c r="S78" s="10"/>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <v>78</v>
-      </c>
+    <row r="79" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M79" s="10"/>
       <c r="N79" s="10"/>
       <c r="O79" s="10"/>
@@ -10903,10 +11118,7 @@
       <c r="R79" s="10"/>
       <c r="S79" s="10"/>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>79</v>
-      </c>
+    <row r="80" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M80" s="10"/>
       <c r="N80" s="10"/>
       <c r="O80" s="10"/>
@@ -10915,10 +11127,7 @@
       <c r="R80" s="10"/>
       <c r="S80" s="10"/>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>80</v>
-      </c>
+    <row r="81" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M81" s="10"/>
       <c r="N81" s="10"/>
       <c r="O81" s="10"/>
@@ -10927,10 +11136,7 @@
       <c r="R81" s="10"/>
       <c r="S81" s="10"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A82" s="2">
-        <v>81</v>
-      </c>
+    <row r="82" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M82" s="10"/>
       <c r="N82" s="10"/>
       <c r="O82" s="10"/>
@@ -10939,10 +11145,7 @@
       <c r="R82" s="10"/>
       <c r="S82" s="10"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A83" s="2">
-        <v>82</v>
-      </c>
+    <row r="83" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M83" s="10"/>
       <c r="N83" s="10"/>
       <c r="O83" s="10"/>
@@ -10951,10 +11154,7 @@
       <c r="R83" s="10"/>
       <c r="S83" s="10"/>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A84" s="2">
-        <v>83</v>
-      </c>
+    <row r="84" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M84" s="10"/>
       <c r="N84" s="10"/>
       <c r="O84" s="10"/>
@@ -10963,10 +11163,7 @@
       <c r="R84" s="10"/>
       <c r="S84" s="10"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A85" s="2">
-        <v>84</v>
-      </c>
+    <row r="85" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M85" s="10"/>
       <c r="N85" s="10"/>
       <c r="O85" s="10"/>
@@ -10975,10 +11172,7 @@
       <c r="R85" s="10"/>
       <c r="S85" s="10"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
-        <v>85</v>
-      </c>
+    <row r="86" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M86" s="10"/>
       <c r="N86" s="10"/>
       <c r="O86" s="10"/>
@@ -10987,10 +11181,7 @@
       <c r="R86" s="10"/>
       <c r="S86" s="10"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A87" s="2">
-        <v>86</v>
-      </c>
+    <row r="87" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M87" s="10"/>
       <c r="N87" s="10"/>
       <c r="O87" s="10"/>
@@ -10999,10 +11190,7 @@
       <c r="R87" s="10"/>
       <c r="S87" s="10"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A88" s="2">
-        <v>87</v>
-      </c>
+    <row r="88" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M88" s="10"/>
       <c r="N88" s="10"/>
       <c r="O88" s="10"/>
@@ -11011,10 +11199,7 @@
       <c r="R88" s="10"/>
       <c r="S88" s="10"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A89" s="2">
-        <v>88</v>
-      </c>
+    <row r="89" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M89" s="10"/>
       <c r="N89" s="10"/>
       <c r="O89" s="10"/>
@@ -11023,10 +11208,7 @@
       <c r="R89" s="10"/>
       <c r="S89" s="10"/>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A90" s="2">
-        <v>89</v>
-      </c>
+    <row r="90" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M90" s="10"/>
       <c r="N90" s="10"/>
       <c r="O90" s="10"/>
@@ -11035,10 +11217,7 @@
       <c r="R90" s="10"/>
       <c r="S90" s="10"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A91" s="2">
-        <v>90</v>
-      </c>
+    <row r="91" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M91" s="10"/>
       <c r="N91" s="10"/>
       <c r="O91" s="10"/>
@@ -11047,10 +11226,7 @@
       <c r="R91" s="10"/>
       <c r="S91" s="10"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A92" s="2">
-        <v>91</v>
-      </c>
+    <row r="92" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M92" s="10"/>
       <c r="N92" s="10"/>
       <c r="O92" s="10"/>
@@ -11059,10 +11235,7 @@
       <c r="R92" s="10"/>
       <c r="S92" s="10"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A93" s="2">
-        <v>92</v>
-      </c>
+    <row r="93" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M93" s="10"/>
       <c r="N93" s="10"/>
       <c r="O93" s="10"/>
@@ -11071,10 +11244,7 @@
       <c r="R93" s="10"/>
       <c r="S93" s="10"/>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A94" s="2">
-        <v>93</v>
-      </c>
+    <row r="94" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M94" s="10"/>
       <c r="N94" s="10"/>
       <c r="O94" s="10"/>
@@ -11083,10 +11253,7 @@
       <c r="R94" s="10"/>
       <c r="S94" s="10"/>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A95" s="2">
-        <v>94</v>
-      </c>
+    <row r="95" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M95" s="10"/>
       <c r="N95" s="10"/>
       <c r="O95" s="10"/>
@@ -11095,10 +11262,7 @@
       <c r="R95" s="10"/>
       <c r="S95" s="10"/>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A96" s="2">
-        <v>95</v>
-      </c>
+    <row r="96" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M96" s="10"/>
       <c r="N96" s="10"/>
       <c r="O96" s="10"/>
@@ -11107,10 +11271,7 @@
       <c r="R96" s="10"/>
       <c r="S96" s="10"/>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A97" s="2">
-        <v>96</v>
-      </c>
+    <row r="97" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M97" s="10"/>
       <c r="N97" s="10"/>
       <c r="O97" s="10"/>
@@ -11119,10 +11280,7 @@
       <c r="R97" s="10"/>
       <c r="S97" s="10"/>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A98" s="2">
-        <v>97</v>
-      </c>
+    <row r="98" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M98" s="10"/>
       <c r="N98" s="10"/>
       <c r="O98" s="10"/>
@@ -11131,10 +11289,7 @@
       <c r="R98" s="10"/>
       <c r="S98" s="10"/>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A99" s="2">
-        <v>98</v>
-      </c>
+    <row r="99" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M99" s="10"/>
       <c r="N99" s="10"/>
       <c r="O99" s="10"/>
@@ -11143,10 +11298,7 @@
       <c r="R99" s="10"/>
       <c r="S99" s="10"/>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A100" s="2">
-        <v>99</v>
-      </c>
+    <row r="100" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M100" s="10"/>
       <c r="N100" s="10"/>
       <c r="O100" s="10"/>
@@ -11155,10 +11307,7 @@
       <c r="R100" s="10"/>
       <c r="S100" s="10"/>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A101" s="2">
-        <v>100</v>
-      </c>
+    <row r="101" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M101" s="10"/>
       <c r="N101" s="10"/>
       <c r="O101" s="10"/>
@@ -11167,10 +11316,7 @@
       <c r="R101" s="10"/>
       <c r="S101" s="10"/>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A102" s="2">
-        <v>101</v>
-      </c>
+    <row r="102" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M102" s="10"/>
       <c r="N102" s="10"/>
       <c r="O102" s="10"/>
@@ -11179,10 +11325,7 @@
       <c r="R102" s="10"/>
       <c r="S102" s="10"/>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A103" s="2">
-        <v>102</v>
-      </c>
+    <row r="103" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M103" s="10"/>
       <c r="N103" s="10"/>
       <c r="O103" s="10"/>
@@ -11191,10 +11334,7 @@
       <c r="R103" s="10"/>
       <c r="S103" s="10"/>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A104" s="2">
-        <v>103</v>
-      </c>
+    <row r="104" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M104" s="10"/>
       <c r="N104" s="10"/>
       <c r="O104" s="10"/>
@@ -11203,10 +11343,7 @@
       <c r="R104" s="10"/>
       <c r="S104" s="10"/>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A105" s="2">
-        <v>104</v>
-      </c>
+    <row r="105" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M105" s="10"/>
       <c r="N105" s="10"/>
       <c r="O105" s="10"/>
@@ -11215,10 +11352,7 @@
       <c r="R105" s="10"/>
       <c r="S105" s="10"/>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A106" s="2">
-        <v>105</v>
-      </c>
+    <row r="106" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M106" s="10"/>
       <c r="N106" s="10"/>
       <c r="O106" s="10"/>
@@ -11227,10 +11361,7 @@
       <c r="R106" s="10"/>
       <c r="S106" s="10"/>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A107" s="2">
-        <v>106</v>
-      </c>
+    <row r="107" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M107" s="10"/>
       <c r="N107" s="10"/>
       <c r="O107" s="10"/>
@@ -11239,10 +11370,7 @@
       <c r="R107" s="10"/>
       <c r="S107" s="10"/>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A108" s="2">
-        <v>107</v>
-      </c>
+    <row r="108" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M108" s="10"/>
       <c r="N108" s="10"/>
       <c r="O108" s="10"/>
@@ -11251,10 +11379,7 @@
       <c r="R108" s="10"/>
       <c r="S108" s="10"/>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A109" s="2">
-        <v>108</v>
-      </c>
+    <row r="109" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M109" s="10"/>
       <c r="N109" s="10"/>
       <c r="O109" s="10"/>
@@ -11263,10 +11388,7 @@
       <c r="R109" s="10"/>
       <c r="S109" s="10"/>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A110" s="2">
-        <v>109</v>
-      </c>
+    <row r="110" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M110" s="10"/>
       <c r="N110" s="10"/>
       <c r="O110" s="10"/>
@@ -11275,10 +11397,7 @@
       <c r="R110" s="10"/>
       <c r="S110" s="10"/>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A111" s="2">
-        <v>110</v>
-      </c>
+    <row r="111" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M111" s="10"/>
       <c r="N111" s="10"/>
       <c r="O111" s="10"/>
@@ -11287,10 +11406,7 @@
       <c r="R111" s="10"/>
       <c r="S111" s="10"/>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A112" s="2">
-        <v>111</v>
-      </c>
+    <row r="112" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M112" s="10"/>
       <c r="N112" s="10"/>
       <c r="O112" s="10"/>
@@ -11299,10 +11415,7 @@
       <c r="R112" s="10"/>
       <c r="S112" s="10"/>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A113" s="2">
-        <v>112</v>
-      </c>
+    <row r="113" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M113" s="10"/>
       <c r="N113" s="10"/>
       <c r="O113" s="10"/>
@@ -11311,10 +11424,7 @@
       <c r="R113" s="10"/>
       <c r="S113" s="10"/>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A114" s="2">
-        <v>113</v>
-      </c>
+    <row r="114" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M114" s="10"/>
       <c r="N114" s="10"/>
       <c r="O114" s="10"/>
@@ -11323,10 +11433,7 @@
       <c r="R114" s="10"/>
       <c r="S114" s="10"/>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A115" s="2">
-        <v>114</v>
-      </c>
+    <row r="115" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M115" s="10"/>
       <c r="N115" s="10"/>
       <c r="O115" s="10"/>
@@ -11335,10 +11442,7 @@
       <c r="R115" s="10"/>
       <c r="S115" s="10"/>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A116" s="2">
-        <v>115</v>
-      </c>
+    <row r="116" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M116" s="10"/>
       <c r="N116" s="10"/>
       <c r="O116" s="10"/>
@@ -11347,10 +11451,7 @@
       <c r="R116" s="10"/>
       <c r="S116" s="10"/>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A117" s="2">
-        <v>116</v>
-      </c>
+    <row r="117" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M117" s="10"/>
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
@@ -11359,10 +11460,7 @@
       <c r="R117" s="10"/>
       <c r="S117" s="10"/>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A118" s="2">
-        <v>117</v>
-      </c>
+    <row r="118" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M118" s="10"/>
       <c r="N118" s="10"/>
       <c r="O118" s="10"/>
@@ -11371,10 +11469,7 @@
       <c r="R118" s="10"/>
       <c r="S118" s="10"/>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A119" s="2">
-        <v>118</v>
-      </c>
+    <row r="119" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M119" s="10"/>
       <c r="N119" s="10"/>
       <c r="O119" s="10"/>
@@ -11383,10 +11478,7 @@
       <c r="R119" s="10"/>
       <c r="S119" s="10"/>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A120" s="2">
-        <v>119</v>
-      </c>
+    <row r="120" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M120" s="10"/>
       <c r="N120" s="10"/>
       <c r="O120" s="10"/>
@@ -11395,10 +11487,7 @@
       <c r="R120" s="10"/>
       <c r="S120" s="10"/>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A121" s="2">
-        <v>120</v>
-      </c>
+    <row r="121" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M121" s="10"/>
       <c r="N121" s="10"/>
       <c r="O121" s="10"/>
@@ -11407,10 +11496,7 @@
       <c r="R121" s="10"/>
       <c r="S121" s="10"/>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A122" s="2">
-        <v>121</v>
-      </c>
+    <row r="122" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M122" s="10"/>
       <c r="N122" s="10"/>
       <c r="O122" s="10"/>
@@ -11419,10 +11505,7 @@
       <c r="R122" s="10"/>
       <c r="S122" s="10"/>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A123" s="2">
-        <v>122</v>
-      </c>
+    <row r="123" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M123" s="10"/>
       <c r="N123" s="10"/>
       <c r="O123" s="10"/>
@@ -11431,10 +11514,7 @@
       <c r="R123" s="10"/>
       <c r="S123" s="10"/>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A124" s="2">
-        <v>123</v>
-      </c>
+    <row r="124" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M124" s="10"/>
       <c r="N124" s="10"/>
       <c r="O124" s="10"/>
@@ -11443,10 +11523,7 @@
       <c r="R124" s="10"/>
       <c r="S124" s="10"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A125" s="2">
-        <v>124</v>
-      </c>
+    <row r="125" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M125" s="10"/>
       <c r="N125" s="10"/>
       <c r="O125" s="10"/>
@@ -11455,10 +11532,7 @@
       <c r="R125" s="10"/>
       <c r="S125" s="10"/>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A126" s="2">
-        <v>125</v>
-      </c>
+    <row r="126" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M126" s="10"/>
       <c r="N126" s="10"/>
       <c r="O126" s="10"/>
@@ -11467,10 +11541,7 @@
       <c r="R126" s="10"/>
       <c r="S126" s="10"/>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A127" s="2">
-        <v>126</v>
-      </c>
+    <row r="127" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M127" s="10"/>
       <c r="N127" s="10"/>
       <c r="O127" s="10"/>
@@ -11479,10 +11550,7 @@
       <c r="R127" s="10"/>
       <c r="S127" s="10"/>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A128" s="2">
-        <v>127</v>
-      </c>
+    <row r="128" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M128" s="10"/>
       <c r="N128" s="10"/>
       <c r="O128" s="10"/>
@@ -11491,10 +11559,7 @@
       <c r="R128" s="10"/>
       <c r="S128" s="10"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A129" s="2">
-        <v>128</v>
-      </c>
+    <row r="129" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M129" s="10"/>
       <c r="N129" s="10"/>
       <c r="O129" s="10"/>
@@ -11503,10 +11568,7 @@
       <c r="R129" s="10"/>
       <c r="S129" s="10"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A130" s="2">
-        <v>129</v>
-      </c>
+    <row r="130" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M130" s="10"/>
       <c r="N130" s="10"/>
       <c r="O130" s="10"/>
@@ -11515,10 +11577,7 @@
       <c r="R130" s="10"/>
       <c r="S130" s="10"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A131" s="2">
-        <v>130</v>
-      </c>
+    <row r="131" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M131" s="10"/>
       <c r="N131" s="10"/>
       <c r="O131" s="10"/>
@@ -11527,10 +11586,7 @@
       <c r="R131" s="10"/>
       <c r="S131" s="10"/>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A132" s="2">
-        <v>131</v>
-      </c>
+    <row r="132" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M132" s="10"/>
       <c r="N132" s="10"/>
       <c r="O132" s="10"/>
@@ -11539,10 +11595,7 @@
       <c r="R132" s="10"/>
       <c r="S132" s="10"/>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A133" s="2">
-        <v>132</v>
-      </c>
+    <row r="133" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M133" s="10"/>
       <c r="N133" s="10"/>
       <c r="O133" s="10"/>
@@ -11551,10 +11604,7 @@
       <c r="R133" s="10"/>
       <c r="S133" s="10"/>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A134" s="2">
-        <v>133</v>
-      </c>
+    <row r="134" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M134" s="10"/>
       <c r="N134" s="10"/>
       <c r="O134" s="10"/>
@@ -11563,10 +11613,7 @@
       <c r="R134" s="10"/>
       <c r="S134" s="10"/>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A135" s="2">
-        <v>134</v>
-      </c>
+    <row r="135" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M135" s="10"/>
       <c r="N135" s="10"/>
       <c r="O135" s="10"/>
@@ -11575,10 +11622,7 @@
       <c r="R135" s="10"/>
       <c r="S135" s="10"/>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A136" s="2">
-        <v>135</v>
-      </c>
+    <row r="136" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M136" s="10"/>
       <c r="N136" s="10"/>
       <c r="O136" s="10"/>
@@ -11587,10 +11631,7 @@
       <c r="R136" s="10"/>
       <c r="S136" s="10"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A137" s="2">
-        <v>136</v>
-      </c>
+    <row r="137" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M137" s="10"/>
       <c r="N137" s="10"/>
       <c r="O137" s="10"/>
@@ -11599,10 +11640,7 @@
       <c r="R137" s="10"/>
       <c r="S137" s="10"/>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A138" s="2">
-        <v>137</v>
-      </c>
+    <row r="138" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M138" s="10"/>
       <c r="N138" s="10"/>
       <c r="O138" s="10"/>
@@ -11611,10 +11649,7 @@
       <c r="R138" s="10"/>
       <c r="S138" s="10"/>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A139" s="2">
-        <v>138</v>
-      </c>
+    <row r="139" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M139" s="10"/>
       <c r="N139" s="10"/>
       <c r="O139" s="10"/>
@@ -11623,10 +11658,7 @@
       <c r="R139" s="10"/>
       <c r="S139" s="10"/>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A140" s="2">
-        <v>139</v>
-      </c>
+    <row r="140" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M140" s="10"/>
       <c r="N140" s="10"/>
       <c r="O140" s="10"/>
@@ -11635,10 +11667,7 @@
       <c r="R140" s="10"/>
       <c r="S140" s="10"/>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A141" s="2">
-        <v>140</v>
-      </c>
+    <row r="141" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M141" s="10"/>
       <c r="N141" s="10"/>
       <c r="O141" s="10"/>
@@ -11647,10 +11676,7 @@
       <c r="R141" s="10"/>
       <c r="S141" s="10"/>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A142" s="2">
-        <v>141</v>
-      </c>
+    <row r="142" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M142" s="10"/>
       <c r="N142" s="10"/>
       <c r="O142" s="10"/>
@@ -11659,10 +11685,7 @@
       <c r="R142" s="10"/>
       <c r="S142" s="10"/>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A143" s="2">
-        <v>142</v>
-      </c>
+    <row r="143" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M143" s="10"/>
       <c r="N143" s="10"/>
       <c r="O143" s="10"/>
@@ -11671,10 +11694,7 @@
       <c r="R143" s="10"/>
       <c r="S143" s="10"/>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A144" s="2">
-        <v>143</v>
-      </c>
+    <row r="144" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M144" s="10"/>
       <c r="N144" s="10"/>
       <c r="O144" s="10"/>
@@ -11683,10 +11703,7 @@
       <c r="R144" s="10"/>
       <c r="S144" s="10"/>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A145" s="2">
-        <v>144</v>
-      </c>
+    <row r="145" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M145" s="10"/>
       <c r="N145" s="10"/>
       <c r="O145" s="10"/>
@@ -11695,10 +11712,7 @@
       <c r="R145" s="10"/>
       <c r="S145" s="10"/>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A146" s="2">
-        <v>145</v>
-      </c>
+    <row r="146" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M146" s="10"/>
       <c r="N146" s="10"/>
       <c r="O146" s="10"/>
@@ -11707,10 +11721,7 @@
       <c r="R146" s="10"/>
       <c r="S146" s="10"/>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A147" s="2">
-        <v>146</v>
-      </c>
+    <row r="147" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M147" s="10"/>
       <c r="N147" s="10"/>
       <c r="O147" s="10"/>
@@ -11719,10 +11730,7 @@
       <c r="R147" s="10"/>
       <c r="S147" s="10"/>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A148" s="2">
-        <v>147</v>
-      </c>
+    <row r="148" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M148" s="10"/>
       <c r="N148" s="10"/>
       <c r="O148" s="10"/>
@@ -11731,10 +11739,7 @@
       <c r="R148" s="10"/>
       <c r="S148" s="10"/>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A149" s="2">
-        <v>148</v>
-      </c>
+    <row r="149" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M149" s="10"/>
       <c r="N149" s="10"/>
       <c r="O149" s="10"/>
@@ -11743,10 +11748,7 @@
       <c r="R149" s="10"/>
       <c r="S149" s="10"/>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A150" s="2">
-        <v>149</v>
-      </c>
+    <row r="150" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M150" s="10"/>
       <c r="N150" s="10"/>
       <c r="O150" s="10"/>
@@ -11755,10 +11757,7 @@
       <c r="R150" s="10"/>
       <c r="S150" s="10"/>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A151" s="2">
-        <v>150</v>
-      </c>
+    <row r="151" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M151" s="10"/>
       <c r="N151" s="10"/>
       <c r="O151" s="10"/>
@@ -11767,10 +11766,7 @@
       <c r="R151" s="10"/>
       <c r="S151" s="10"/>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A152" s="2">
-        <v>151</v>
-      </c>
+    <row r="152" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M152" s="10"/>
       <c r="N152" s="10"/>
       <c r="O152" s="10"/>
@@ -11779,10 +11775,7 @@
       <c r="R152" s="10"/>
       <c r="S152" s="10"/>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A153" s="2">
-        <v>152</v>
-      </c>
+    <row r="153" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M153" s="10"/>
       <c r="N153" s="10"/>
       <c r="O153" s="10"/>
@@ -11791,10 +11784,7 @@
       <c r="R153" s="10"/>
       <c r="S153" s="10"/>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A154" s="2">
-        <v>153</v>
-      </c>
+    <row r="154" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M154" s="10"/>
       <c r="N154" s="10"/>
       <c r="O154" s="10"/>
@@ -11803,10 +11793,7 @@
       <c r="R154" s="10"/>
       <c r="S154" s="10"/>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A155" s="2">
-        <v>154</v>
-      </c>
+    <row r="155" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M155" s="10"/>
       <c r="N155" s="10"/>
       <c r="O155" s="10"/>
@@ -11815,10 +11802,7 @@
       <c r="R155" s="10"/>
       <c r="S155" s="10"/>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A156" s="2">
-        <v>155</v>
-      </c>
+    <row r="156" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M156" s="10"/>
       <c r="N156" s="10"/>
       <c r="O156" s="10"/>
@@ -11827,10 +11811,7 @@
       <c r="R156" s="10"/>
       <c r="S156" s="10"/>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A157" s="2">
-        <v>156</v>
-      </c>
+    <row r="157" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M157" s="10"/>
       <c r="N157" s="10"/>
       <c r="O157" s="10"/>
@@ -11839,10 +11820,7 @@
       <c r="R157" s="10"/>
       <c r="S157" s="10"/>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A158" s="2">
-        <v>157</v>
-      </c>
+    <row r="158" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M158" s="10"/>
       <c r="N158" s="10"/>
       <c r="O158" s="10"/>
@@ -11851,10 +11829,7 @@
       <c r="R158" s="10"/>
       <c r="S158" s="10"/>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A159" s="2">
-        <v>158</v>
-      </c>
+    <row r="159" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M159" s="10"/>
       <c r="N159" s="10"/>
       <c r="O159" s="10"/>
@@ -11863,10 +11838,7 @@
       <c r="R159" s="10"/>
       <c r="S159" s="10"/>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A160" s="2">
-        <v>159</v>
-      </c>
+    <row r="160" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M160" s="10"/>
       <c r="N160" s="10"/>
       <c r="O160" s="10"/>
@@ -11875,10 +11847,7 @@
       <c r="R160" s="10"/>
       <c r="S160" s="10"/>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A161" s="2">
-        <v>160</v>
-      </c>
+    <row r="161" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M161" s="10"/>
       <c r="N161" s="10"/>
       <c r="O161" s="10"/>
@@ -11887,10 +11856,7 @@
       <c r="R161" s="10"/>
       <c r="S161" s="10"/>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A162" s="2">
-        <v>161</v>
-      </c>
+    <row r="162" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M162" s="10"/>
       <c r="N162" s="10"/>
       <c r="O162" s="10"/>
@@ -11899,10 +11865,7 @@
       <c r="R162" s="10"/>
       <c r="S162" s="10"/>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A163" s="2">
-        <v>162</v>
-      </c>
+    <row r="163" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M163" s="10"/>
       <c r="N163" s="10"/>
       <c r="O163" s="10"/>
@@ -11911,10 +11874,7 @@
       <c r="R163" s="10"/>
       <c r="S163" s="10"/>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A164" s="2">
-        <v>163</v>
-      </c>
+    <row r="164" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M164" s="10"/>
       <c r="N164" s="10"/>
       <c r="O164" s="10"/>
@@ -11923,10 +11883,7 @@
       <c r="R164" s="10"/>
       <c r="S164" s="10"/>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A165" s="2">
-        <v>164</v>
-      </c>
+    <row r="165" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M165" s="10"/>
       <c r="N165" s="10"/>
       <c r="O165" s="10"/>
@@ -11935,10 +11892,7 @@
       <c r="R165" s="10"/>
       <c r="S165" s="10"/>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A166" s="2">
-        <v>165</v>
-      </c>
+    <row r="166" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M166" s="10"/>
       <c r="N166" s="10"/>
       <c r="O166" s="10"/>
@@ -11947,10 +11901,7 @@
       <c r="R166" s="10"/>
       <c r="S166" s="10"/>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A167" s="2">
-        <v>166</v>
-      </c>
+    <row r="167" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M167" s="10"/>
       <c r="N167" s="10"/>
       <c r="O167" s="10"/>
@@ -11959,10 +11910,7 @@
       <c r="R167" s="10"/>
       <c r="S167" s="10"/>
     </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A168" s="2">
-        <v>167</v>
-      </c>
+    <row r="168" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M168" s="10"/>
       <c r="N168" s="10"/>
       <c r="O168" s="10"/>
@@ -11971,10 +11919,7 @@
       <c r="R168" s="10"/>
       <c r="S168" s="10"/>
     </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A169" s="2">
-        <v>168</v>
-      </c>
+    <row r="169" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M169" s="10"/>
       <c r="N169" s="10"/>
       <c r="O169" s="10"/>
@@ -11983,10 +11928,7 @@
       <c r="R169" s="10"/>
       <c r="S169" s="10"/>
     </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A170" s="2">
-        <v>169</v>
-      </c>
+    <row r="170" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M170" s="10"/>
       <c r="N170" s="10"/>
       <c r="O170" s="10"/>
@@ -11995,10 +11937,7 @@
       <c r="R170" s="10"/>
       <c r="S170" s="10"/>
     </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A171" s="2">
-        <v>170</v>
-      </c>
+    <row r="171" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M171" s="10"/>
       <c r="N171" s="10"/>
       <c r="O171" s="10"/>
@@ -12007,10 +11946,7 @@
       <c r="R171" s="10"/>
       <c r="S171" s="10"/>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A172" s="2">
-        <v>171</v>
-      </c>
+    <row r="172" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M172" s="10"/>
       <c r="N172" s="10"/>
       <c r="O172" s="10"/>
@@ -12019,10 +11955,7 @@
       <c r="R172" s="10"/>
       <c r="S172" s="10"/>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A173" s="2">
-        <v>172</v>
-      </c>
+    <row r="173" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M173" s="10"/>
       <c r="N173" s="10"/>
       <c r="O173" s="10"/>
@@ -12031,10 +11964,7 @@
       <c r="R173" s="10"/>
       <c r="S173" s="10"/>
     </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A174" s="2">
-        <v>173</v>
-      </c>
+    <row r="174" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M174" s="10"/>
       <c r="N174" s="10"/>
       <c r="O174" s="10"/>
@@ -12043,10 +11973,7 @@
       <c r="R174" s="10"/>
       <c r="S174" s="10"/>
     </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A175" s="2">
-        <v>174</v>
-      </c>
+    <row r="175" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M175" s="10"/>
       <c r="N175" s="10"/>
       <c r="O175" s="10"/>
@@ -12055,7 +11982,7 @@
       <c r="R175" s="10"/>
       <c r="S175" s="10"/>
     </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="176" spans="13:19" x14ac:dyDescent="0.3">
       <c r="M176" s="10"/>
       <c r="N176" s="10"/>
       <c r="O176" s="10"/>
@@ -12093,23 +12020,23 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C36" r:id="rId1"/>
-    <hyperlink ref="C37" r:id="rId2"/>
-    <hyperlink ref="D41" r:id="rId3" display="https://www.google.com/search?sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;tbs=lf:1,lf_ui:2&amp;tbm=lcl&amp;sxsrf=ACQVn0-yjBygfThguW8-plBveMrMzDiPGw:1704870884151&amp;q=engineering+colleges+in+south+calcutta&amp;rflfq=1&amp;num=10&amp;sa=X&amp;ved=2ahUKEwjQ47_7otKDAxUve2wGHY_pCzEQjGp6BAgXEAE&amp;biw=1536&amp;bih=730&amp;dpr=1.25"/>
-    <hyperlink ref="C43" r:id="rId4"/>
-    <hyperlink ref="D47" r:id="rId5" display="https://www.google.com/search?q=engineering+colleges+kolkata&amp;sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;biw=1536&amp;bih=730&amp;tbm=lcl&amp;sxsrf=ACQVn09cs4SfDApVNizAZQHyNbKrHkG1kw%3A1704870889163&amp;ei=6UOeZYunCcqWseMP2bOt0A4&amp;ved=0ahUKEwjLv_H9otKDAxVKS2wGHdlZC-oQ4dUDCAk&amp;uact=5&amp;oq=engineering+colleges+kolkata&amp;gs_lp=Eg1nd3Mtd2l6LWxvY2FsIhxlbmdpbmVlcmluZyBjb2xsZWdlcyBrb2xrYXRhMgUQABiABDIGEAAYFhgeMgYQABgWGB4yCBAAGBYYHhgPMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeSPErUNUEWOgmcAF4AJABAZgBqwGgAb0XqgEEMC4yM7gBA8gBAPgBAcICCxAAGIAEGIoFGIYDwgIEECMYJ8ICCxAAGIAEGIoFGJECwgIKEAAYgAQYFBiHAsICDhAAGIAEGIoFGJECGMkDiAYB&amp;sclient=gws-wiz-local"/>
-    <hyperlink ref="C49" r:id="rId6"/>
+    <hyperlink ref="C36" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C37" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D41" r:id="rId3" display="https://www.google.com/search?sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;tbs=lf:1,lf_ui:2&amp;tbm=lcl&amp;sxsrf=ACQVn0-yjBygfThguW8-plBveMrMzDiPGw:1704870884151&amp;q=engineering+colleges+in+south+calcutta&amp;rflfq=1&amp;num=10&amp;sa=X&amp;ved=2ahUKEwjQ47_7otKDAxUve2wGHY_pCzEQjGp6BAgXEAE&amp;biw=1536&amp;bih=730&amp;dpr=1.25" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C43" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D47" r:id="rId5" display="https://www.google.com/search?q=engineering+colleges+kolkata&amp;sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;biw=1536&amp;bih=730&amp;tbm=lcl&amp;sxsrf=ACQVn09cs4SfDApVNizAZQHyNbKrHkG1kw%3A1704870889163&amp;ei=6UOeZYunCcqWseMP2bOt0A4&amp;ved=0ahUKEwjLv_H9otKDAxVKS2wGHdlZC-oQ4dUDCAk&amp;uact=5&amp;oq=engineering+colleges+kolkata&amp;gs_lp=Eg1nd3Mtd2l6LWxvY2FsIhxlbmdpbmVlcmluZyBjb2xsZWdlcyBrb2xrYXRhMgUQABiABDIGEAAYFhgeMgYQABgWGB4yCBAAGBYYHhgPMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeSPErUNUEWOgmcAF4AJABAZgBqwGgAb0XqgEEMC4yM7gBA8gBAPgBAcICCxAAGIAEGIoFGIYDwgIEECMYJ8ICCxAAGIAEGIoFGJECwgIKEAAYgAQYFBiHAsICDhAAGIAEGIoFGJECGMkDiAYB&amp;sclient=gws-wiz-local" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="C49" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -12118,7 +12045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update AI Workshop Schools-Colleges.xlsx
updated
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F35F05D-1F79-4CDF-B824-891651159FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -21,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'School-Details'!$A$1:$U$122</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,13 +39,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>del</author>
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L28" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="L28" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,12 +88,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>del</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="437">
   <si>
     <t>CBSE</t>
   </si>
@@ -1415,13 +1414,6 @@
     <t>8981510888 9007720041 9831071659</t>
   </si>
   <si>
-    <t xml:space="preserve">
-IEM PUBLIC SCHOOL</t>
-  </si>
-  <si>
-    <t>IEM PUBLIC SCHOOL</t>
-  </si>
-  <si>
     <t>+9147059775
 +9147059774
   9831071659</t>
@@ -1446,12 +1438,19 @@
   </si>
   <si>
     <t xml:space="preserve"> 033 6627 0502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+IEM PUBLIC SCHOOL, Salt Lake</t>
+  </si>
+  <si>
+    <t>IEM PUBLIC SCHOOL, new town</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2192,10 +2191,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -2252,7 +2251,7 @@
       </c>
       <c r="D4" s="16">
         <f>MAX('School-Details'!A:A)</f>
-        <v>235</v>
+        <v>123</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>265</v>
@@ -2284,7 +2283,7 @@
       </c>
       <c r="D5" s="16">
         <f>ROUND(SUM('School-Details'!K:K)/D4,2)</f>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>210</v>
@@ -2566,7 +2565,7 @@
       </c>
       <c r="D14" s="14">
         <f>COUNTIF('School-Details'!U:U,C14)</f>
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F14" s="22">
         <v>45352</v>
@@ -2642,7 +2641,7 @@
       </c>
       <c r="D16" s="16">
         <f>SUM(D8:D15)</f>
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F16" s="22">
         <v>45413</v>
@@ -2781,7 +2780,7 @@
       </c>
       <c r="D20" s="14">
         <f>COUNTIF('School-Details'!T:T,C20)</f>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F20" s="22">
         <v>45536</v>
@@ -2818,7 +2817,7 @@
       </c>
       <c r="D21" s="14">
         <f>SUM(D19:D20)</f>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F21" s="22">
         <v>45566</v>
@@ -3033,7 +3032,7 @@
       </c>
       <c r="D27" s="16">
         <f>D21+D23+D26</f>
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I27" s="31"/>
       <c r="K27" s="33"/>
@@ -3099,14 +3098,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U236"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D117" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="F23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H114" sqref="H114"/>
+      <selection pane="bottomRight" activeCell="W128" sqref="W128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5939,7 +5938,7 @@
         <v>4</v>
       </c>
       <c r="S67" s="10">
-        <f t="shared" ref="S67:S122" si="2">SUM(N67:R67)</f>
+        <f t="shared" ref="S67:S124" si="2">SUM(N67:R67)</f>
         <v>22</v>
       </c>
       <c r="T67" s="10">
@@ -5987,7 +5986,7 @@
         <v>20</v>
       </c>
       <c r="T68" s="10">
-        <f t="shared" ref="T68:T122" si="3">ROUND(S68/5,0)</f>
+        <f t="shared" ref="T68:T124" si="3">ROUND(S68/5,0)</f>
         <v>4</v>
       </c>
       <c r="U68" s="10" t="s">
@@ -8134,7 +8133,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="17" t="s">
-        <v>427</v>
+        <v>435</v>
       </c>
       <c r="C123" s="40" t="s">
         <v>25</v>
@@ -8144,6 +8143,32 @@
       </c>
       <c r="G123" s="40" t="s">
         <v>310</v>
+      </c>
+      <c r="N123" s="1">
+        <v>2</v>
+      </c>
+      <c r="O123" s="1">
+        <v>5</v>
+      </c>
+      <c r="P123" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q123" s="1">
+        <v>4</v>
+      </c>
+      <c r="R123" s="1">
+        <v>4</v>
+      </c>
+      <c r="S123" s="10">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="T123" s="10">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U123" s="10" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="124" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -8151,641 +8176,107 @@
         <v>123</v>
       </c>
       <c r="B124" s="17" t="s">
-        <v>428</v>
+        <v>436</v>
       </c>
       <c r="C124" s="40" t="s">
         <v>25</v>
       </c>
       <c r="F124" s="7" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G124" s="40" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A125" s="2">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A126" s="2">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A127" s="2">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A128" s="2">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" s="2">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="2">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" s="2">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" s="2">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" s="2">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" s="2">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" s="2">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" s="2">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" s="2">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" s="2">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" s="2">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" s="2">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" s="2">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" s="2">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" s="2">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" s="2">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" s="2">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" s="2">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" s="2">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" s="2">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150" s="2">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152" s="2">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153" s="2">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154" s="2">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155" s="2">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156" s="2">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157" s="2">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158" s="2">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A159" s="2">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A160" s="2">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A161" s="2">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A162" s="2">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A163" s="2">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A164" s="2">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A165" s="2">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A166" s="2">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A167" s="2">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A168" s="2">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A169" s="2">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A170" s="2">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A171" s="2">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A172" s="2">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A173" s="2">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A174" s="2">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A175" s="2">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A176" s="2">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A177" s="2">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A178" s="2">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A179" s="2">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A180" s="2">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A181" s="2">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A182" s="2">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A183" s="2">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A184" s="2">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A185" s="2">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A186" s="2">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A187" s="2">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A188" s="2">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A189" s="2">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A190" s="2">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A191" s="2">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A192" s="2">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A193" s="2">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A194" s="2">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A195" s="2">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A196" s="2">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A197" s="2">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A198" s="2">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A199" s="2">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A200" s="2">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A201" s="2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A202" s="2">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A203" s="2">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A204" s="2">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A205" s="2">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A206" s="2">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A207" s="2">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A208" s="2">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A209" s="2">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A210" s="2">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A211" s="2">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A212" s="2">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A213" s="2">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A214" s="2">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A215" s="2">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A216" s="2">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A217" s="2">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A218" s="2">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A219" s="2">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A220" s="2">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A221" s="2">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A222" s="2">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A223" s="2">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A224" s="2">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A225" s="2">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A226" s="2">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A227" s="2">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A228" s="2">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A229" s="2">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A230" s="2">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A231" s="2">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A232" s="2">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A233" s="2">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A234" s="2">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A235" s="2">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A236" s="2">
-        <v>235</v>
+      <c r="N124" s="1">
+        <v>2</v>
+      </c>
+      <c r="O124" s="1">
+        <v>5</v>
+      </c>
+      <c r="P124" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q124" s="1">
+        <v>4</v>
+      </c>
+      <c r="R124" s="1">
+        <v>4</v>
+      </c>
+      <c r="S124" s="10">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="T124" s="10">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U124" s="10" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U122" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:U122"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576">
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D32" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="D22" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="D30" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="D33" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="D35" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="D37" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="D41" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="D42" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="D43" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="D47" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="D48" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="D49" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="D51" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="D53" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="D54" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="D55" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="D56" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="D57" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="D58" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="D59" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="D60" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="D61" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="D62" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="D63" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="D64" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="D65" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="D66" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="D67" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="D68" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="D69" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="D70" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="D71" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="D72" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="D73" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="D75" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="D78" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="D79" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="D80" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="D81" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="D85" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="D88" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="D89" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="D91" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="D2" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="D28" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="D31" r:id="rId1"/>
+    <hyperlink ref="D32" r:id="rId2"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp"/>
+    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w"/>
+    <hyperlink ref="D22" r:id="rId5"/>
+    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com"/>
+    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in"/>
+    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com"/>
+    <hyperlink ref="D30" r:id="rId9"/>
+    <hyperlink ref="D33" r:id="rId10"/>
+    <hyperlink ref="D35" r:id="rId11"/>
+    <hyperlink ref="D37" r:id="rId12"/>
+    <hyperlink ref="D41" r:id="rId13"/>
+    <hyperlink ref="D42" r:id="rId14"/>
+    <hyperlink ref="D43" r:id="rId15"/>
+    <hyperlink ref="D47" r:id="rId16"/>
+    <hyperlink ref="D48" r:id="rId17"/>
+    <hyperlink ref="D49" r:id="rId18"/>
+    <hyperlink ref="D51" r:id="rId19"/>
+    <hyperlink ref="D52" r:id="rId20"/>
+    <hyperlink ref="D53" r:id="rId21"/>
+    <hyperlink ref="D54" r:id="rId22"/>
+    <hyperlink ref="D55" r:id="rId23"/>
+    <hyperlink ref="D56" r:id="rId24"/>
+    <hyperlink ref="D57" r:id="rId25"/>
+    <hyperlink ref="D58" r:id="rId26"/>
+    <hyperlink ref="D59" r:id="rId27"/>
+    <hyperlink ref="D60" r:id="rId28"/>
+    <hyperlink ref="D61" r:id="rId29"/>
+    <hyperlink ref="D62" r:id="rId30"/>
+    <hyperlink ref="D63" r:id="rId31"/>
+    <hyperlink ref="D64" r:id="rId32"/>
+    <hyperlink ref="D65" r:id="rId33"/>
+    <hyperlink ref="D66" r:id="rId34"/>
+    <hyperlink ref="D67" r:id="rId35"/>
+    <hyperlink ref="D68" r:id="rId36"/>
+    <hyperlink ref="D69" r:id="rId37"/>
+    <hyperlink ref="D70" r:id="rId38"/>
+    <hyperlink ref="D71" r:id="rId39"/>
+    <hyperlink ref="D72" r:id="rId40"/>
+    <hyperlink ref="D73" r:id="rId41"/>
+    <hyperlink ref="D75" r:id="rId42"/>
+    <hyperlink ref="D78" r:id="rId43"/>
+    <hyperlink ref="D79" r:id="rId44"/>
+    <hyperlink ref="D80" r:id="rId45"/>
+    <hyperlink ref="D81" r:id="rId46"/>
+    <hyperlink ref="D85" r:id="rId47"/>
+    <hyperlink ref="D88" r:id="rId48"/>
+    <hyperlink ref="D89" r:id="rId49"/>
+    <hyperlink ref="D91" r:id="rId50"/>
+    <hyperlink ref="D2" r:id="rId51"/>
+    <hyperlink ref="D28" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId53"/>
@@ -8794,10 +8285,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D49" workbookViewId="0">
       <selection activeCell="R56" sqref="R56"/>
     </sheetView>
   </sheetViews>
@@ -10781,13 +10272,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="38" t="s">
+        <v>428</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>429</v>
+      </c>
+      <c r="E52" s="40" t="s">
         <v>430</v>
-      </c>
-      <c r="D52" s="39" t="s">
-        <v>431</v>
-      </c>
-      <c r="E52" s="40" t="s">
-        <v>432</v>
       </c>
       <c r="M52" s="10">
         <v>0</v>
@@ -10820,10 +10311,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D53" s="39" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E53" s="40" t="s">
         <v>424</v>
@@ -10859,10 +10350,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D54" s="39" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E54" s="40" t="s">
         <v>414</v>
@@ -12020,23 +11511,23 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576">
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C36" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="C37" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D41" r:id="rId3" display="https://www.google.com/search?sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;tbs=lf:1,lf_ui:2&amp;tbm=lcl&amp;sxsrf=ACQVn0-yjBygfThguW8-plBveMrMzDiPGw:1704870884151&amp;q=engineering+colleges+in+south+calcutta&amp;rflfq=1&amp;num=10&amp;sa=X&amp;ved=2ahUKEwjQ47_7otKDAxUve2wGHY_pCzEQjGp6BAgXEAE&amp;biw=1536&amp;bih=730&amp;dpr=1.25" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="C43" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="D47" r:id="rId5" display="https://www.google.com/search?q=engineering+colleges+kolkata&amp;sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;biw=1536&amp;bih=730&amp;tbm=lcl&amp;sxsrf=ACQVn09cs4SfDApVNizAZQHyNbKrHkG1kw%3A1704870889163&amp;ei=6UOeZYunCcqWseMP2bOt0A4&amp;ved=0ahUKEwjLv_H9otKDAxVKS2wGHdlZC-oQ4dUDCAk&amp;uact=5&amp;oq=engineering+colleges+kolkata&amp;gs_lp=Eg1nd3Mtd2l6LWxvY2FsIhxlbmdpbmVlcmluZyBjb2xsZWdlcyBrb2xrYXRhMgUQABiABDIGEAAYFhgeMgYQABgWGB4yCBAAGBYYHhgPMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeSPErUNUEWOgmcAF4AJABAZgBqwGgAb0XqgEEMC4yM7gBA8gBAPgBAcICCxAAGIAEGIoFGIYDwgIEECMYJ8ICCxAAGIAEGIoFGJECwgIKEAAYgAQYFBiHAsICDhAAGIAEGIoFGJECGMkDiAYB&amp;sclient=gws-wiz-local" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="C49" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="C36" r:id="rId1"/>
+    <hyperlink ref="C37" r:id="rId2"/>
+    <hyperlink ref="D41" r:id="rId3" display="https://www.google.com/search?sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;tbs=lf:1,lf_ui:2&amp;tbm=lcl&amp;sxsrf=ACQVn0-yjBygfThguW8-plBveMrMzDiPGw:1704870884151&amp;q=engineering+colleges+in+south+calcutta&amp;rflfq=1&amp;num=10&amp;sa=X&amp;ved=2ahUKEwjQ47_7otKDAxUve2wGHY_pCzEQjGp6BAgXEAE&amp;biw=1536&amp;bih=730&amp;dpr=1.25"/>
+    <hyperlink ref="C43" r:id="rId4"/>
+    <hyperlink ref="D47" r:id="rId5" display="https://www.google.com/search?q=engineering+colleges+kolkata&amp;sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;biw=1536&amp;bih=730&amp;tbm=lcl&amp;sxsrf=ACQVn09cs4SfDApVNizAZQHyNbKrHkG1kw%3A1704870889163&amp;ei=6UOeZYunCcqWseMP2bOt0A4&amp;ved=0ahUKEwjLv_H9otKDAxVKS2wGHdlZC-oQ4dUDCAk&amp;uact=5&amp;oq=engineering+colleges+kolkata&amp;gs_lp=Eg1nd3Mtd2l6LWxvY2FsIhxlbmdpbmVlcmluZyBjb2xsZWdlcyBrb2xrYXRhMgUQABiABDIGEAAYFhgeMgYQABgWGB4yCBAAGBYYHhgPMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeSPErUNUEWOgmcAF4AJABAZgBqwGgAb0XqgEEMC4yM7gBA8gBAPgBAcICCxAAGIAEGIoFGIYDwgIEECMYJ8ICCxAAGIAEGIoFGJECwgIKEAAYgAQYFBiHAsICDhAAGIAEGIoFGJECGMkDiAYB&amp;sclient=gws-wiz-local"/>
+    <hyperlink ref="C49" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -12045,7 +11536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Updated workshop for schools & colleges
Updated workshop for schools & colleges
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02AF92B-0BDE-40DF-B3F0-A7769EFBDDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14036C25-A8DE-44D0-B206-D38F233B8F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="440">
   <si>
     <t>CBSE</t>
   </si>
@@ -1599,7 +1599,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1611,32 +1611,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1747,43 +1721,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1855,12 +1792,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1920,16 +1894,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1978,6 +1952,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1990,24 +1968,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2291,10 +2259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R31"/>
+  <dimension ref="B1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,280 +2273,308 @@
     <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" customWidth="1"/>
-    <col min="10" max="10" width="5.77734375" customWidth="1"/>
+    <col min="9" max="9" width="2.6640625" customWidth="1"/>
+    <col min="10" max="10" width="4.109375" customWidth="1"/>
     <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:18" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="64" t="s">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:18" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="58" t="s">
         <v>293</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="29"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="54" t="s">
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="29"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="62" t="s">
         <v>374</v>
       </c>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="29"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="29"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="31"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="30"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
+      <c r="C4" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="16">
+        <f>MAX('School-Details'!A:A)</f>
+        <v>123</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>266</v>
+      </c>
       <c r="I4" s="31"/>
       <c r="K4" s="30"/>
+      <c r="L4" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="M4" s="16">
+        <f>COUNTIF('College-Details'!J:J,L4)</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="61"/>
+      <c r="O4" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q4" s="61"/>
       <c r="R4" s="31"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="30"/>
       <c r="C5" s="16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D5" s="16">
-        <f>MAX('School-Details'!A:A)</f>
-        <v>123</v>
-      </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>266</v>
-      </c>
-      <c r="H5" s="59"/>
+        <f>ROUND(SUM('School-Details'!K:K)/D4,2)</f>
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G5" s="14">
+        <f>COUNTIF('School-Details'!M:M,F5)</f>
+        <v>0</v>
+      </c>
       <c r="I5" s="31"/>
       <c r="K5" s="30"/>
       <c r="L5" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="M5" s="14">
+        <v>367</v>
+      </c>
+      <c r="M5" s="16">
         <f>COUNTIF('College-Details'!J:J,L5)</f>
         <v>0</v>
       </c>
-      <c r="O5" s="21" t="s">
-        <v>265</v>
-      </c>
-      <c r="P5" s="21" t="s">
-        <v>266</v>
-      </c>
+      <c r="N5" s="61"/>
+      <c r="O5" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="P5" s="14">
+        <f>COUNTIF('College-Details'!L:L,O5)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="61"/>
       <c r="R5" s="31"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="30"/>
       <c r="C6" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="D6" s="16">
-        <f>ROUND(SUM('School-Details'!K:K)/D5,2)</f>
-        <v>0.01</v>
-      </c>
-      <c r="E6" s="59"/>
+        <v>437</v>
+      </c>
+      <c r="D6" s="53">
+        <v>45299</v>
+      </c>
       <c r="F6" s="14" t="s">
-        <v>210</v>
+        <v>267</v>
       </c>
       <c r="G6" s="14">
         <f>COUNTIF('School-Details'!M:M,F6)</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="59"/>
+        <v>1</v>
+      </c>
       <c r="I6" s="31"/>
       <c r="K6" s="30"/>
       <c r="L6" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="M6" s="14">
-        <f>COUNTIF('College-Details'!J:J,L6)</f>
-        <v>0</v>
-      </c>
+        <v>368</v>
+      </c>
+      <c r="M6" s="16">
+        <f>MAX('College-Details'!A:A)</f>
+        <v>53</v>
+      </c>
+      <c r="N6" s="61"/>
       <c r="O6" s="14" t="s">
-        <v>210</v>
+        <v>267</v>
       </c>
       <c r="P6" s="14">
         <f>COUNTIF('College-Details'!L:L,O6)</f>
         <v>0</v>
       </c>
+      <c r="Q6" s="61"/>
       <c r="R6" s="31"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="30"/>
       <c r="C7" s="16" t="s">
-        <v>437</v>
-      </c>
-      <c r="D7" s="60">
-        <v>45299</v>
-      </c>
-      <c r="E7" s="59"/>
+        <v>439</v>
+      </c>
+      <c r="D7" s="53">
+        <f ca="1">TODAY()</f>
+        <v>45301</v>
+      </c>
       <c r="F7" s="14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G7" s="14">
         <f>COUNTIF('School-Details'!M:M,F7)</f>
-        <v>1</v>
-      </c>
-      <c r="H7" s="59"/>
+        <v>0</v>
+      </c>
       <c r="I7" s="31"/>
       <c r="K7" s="30"/>
       <c r="L7" s="16" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="M7" s="16">
-        <f>MAX('College-Details'!A:A)</f>
-        <v>53</v>
-      </c>
+        <f>SUM('College-Details'!I:I)/M6</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="61"/>
       <c r="O7" s="14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="P7" s="14">
         <f>COUNTIF('College-Details'!L:L,O7)</f>
         <v>0</v>
       </c>
+      <c r="Q7" s="61"/>
       <c r="R7" s="31"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="30"/>
       <c r="C8" s="16" t="s">
-        <v>439</v>
-      </c>
-      <c r="D8" s="60">
-        <f ca="1">TODAY()</f>
-        <v>45301</v>
-      </c>
-      <c r="E8" s="59"/>
+        <v>438</v>
+      </c>
+      <c r="D8" s="54">
+        <f ca="1">ROUND(D11/(D7-D6+1),0)</f>
+        <v>4</v>
+      </c>
       <c r="F8" s="14" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="G8" s="14">
         <f>COUNTIF('School-Details'!M:M,F8)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="59"/>
       <c r="I8" s="31"/>
       <c r="K8" s="30"/>
       <c r="L8" s="16" t="s">
-        <v>369</v>
-      </c>
-      <c r="M8" s="16">
-        <f>SUM('College-Details'!I:I)/M7</f>
-        <v>0</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="M8" s="53"/>
+      <c r="N8" s="61"/>
       <c r="O8" s="14" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="P8" s="14">
         <f>COUNTIF('College-Details'!L:L,O8)</f>
         <v>0</v>
       </c>
+      <c r="Q8" s="61"/>
       <c r="R8" s="31"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="30"/>
-      <c r="C9" s="16" t="s">
-        <v>438</v>
-      </c>
-      <c r="D9" s="61">
-        <f ca="1">ROUND(D12/(D8-D7+1),0)</f>
-        <v>4</v>
-      </c>
-      <c r="E9" s="59"/>
-      <c r="F9" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="G9" s="14">
-        <f>COUNTIF('School-Details'!M:M,F9)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="59"/>
+      <c r="F9" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="G9" s="16">
+        <f>SUM(G5:G8)</f>
+        <v>1</v>
+      </c>
       <c r="I9" s="31"/>
       <c r="K9" s="30"/>
-      <c r="O9" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="P9" s="14">
-        <f>COUNTIF('College-Details'!L:L,O9)</f>
-        <v>0</v>
-      </c>
+      <c r="L9" s="16" t="s">
+        <v>439</v>
+      </c>
+      <c r="M9" s="53"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="P9" s="16">
+        <f>SUM(P5:P8)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="61"/>
       <c r="R9" s="31"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="30"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
+      <c r="C10" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>264</v>
+      </c>
       <c r="I10" s="31"/>
       <c r="K10" s="30"/>
-      <c r="L10" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="P10" s="16">
-        <f>SUM(P6:P9)</f>
-        <v>0</v>
-      </c>
+      <c r="L10" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="M10" s="54">
+        <f>ROUND(M14/(M9-M8+1),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="61"/>
       <c r="R10" s="31"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="30"/>
-      <c r="C11" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="59"/>
+      <c r="C11" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="D11" s="14">
+        <f>COUNTIF('School-Details'!U:U,C11)</f>
+        <v>13</v>
+      </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="H11" s="53"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="31"/>
       <c r="K11" s="30"/>
-      <c r="L11" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="M11" s="14">
-        <f>COUNTIF('College-Details'!T:T,L11)</f>
-        <v>0</v>
-      </c>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="57" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q11" s="57"/>
       <c r="R11" s="31"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="30"/>
       <c r="C12" s="14" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D12" s="14">
         <f>COUNTIF('School-Details'!U:U,C12)</f>
-        <v>13</v>
-      </c>
-      <c r="E12" s="59"/>
+        <v>0</v>
+      </c>
       <c r="F12" s="21" t="s">
         <v>269</v>
       </c>
@@ -2590,30 +2586,33 @@
       </c>
       <c r="I12" s="31"/>
       <c r="K12" s="30"/>
-      <c r="L12" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="M12" s="14">
-        <f>COUNTIF('College-Details'!T:T,L12)</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="14"/>
-      <c r="P12" s="57" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q12" s="58"/>
+      <c r="L12" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="N12" s="61"/>
+      <c r="O12" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>271</v>
+      </c>
       <c r="R12" s="31"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="30"/>
       <c r="C13" s="14" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D13" s="14">
         <f>COUNTIF('School-Details'!U:U,C13)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="59"/>
       <c r="F13" s="22">
         <v>45292</v>
       </c>
@@ -2626,33 +2625,33 @@
       <c r="I13" s="31"/>
       <c r="K13" s="30"/>
       <c r="L13" s="14" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="M13" s="14">
         <f>COUNTIF('College-Details'!T:T,L13)</f>
         <v>0</v>
       </c>
-      <c r="O13" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="P13" s="21" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q13" s="21" t="s">
-        <v>271</v>
+      <c r="N13" s="61"/>
+      <c r="O13" s="22">
+        <v>45292</v>
+      </c>
+      <c r="P13" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>0</v>
       </c>
       <c r="R13" s="31"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="30"/>
       <c r="C14" s="14" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D14" s="14">
         <f>COUNTIF('School-Details'!U:U,C14)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="59"/>
       <c r="F14" s="22">
         <v>45323</v>
       </c>
@@ -2665,14 +2664,15 @@
       <c r="I14" s="31"/>
       <c r="K14" s="30"/>
       <c r="L14" s="14" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="M14" s="14">
         <f>COUNTIF('College-Details'!T:T,L14)</f>
         <v>0</v>
       </c>
+      <c r="N14" s="61"/>
       <c r="O14" s="22">
-        <v>45292</v>
+        <v>45323</v>
       </c>
       <c r="P14" s="14">
         <v>0</v>
@@ -2685,13 +2685,12 @@
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="30"/>
       <c r="C15" s="14" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D15" s="14">
         <f>COUNTIF('School-Details'!U:U,C15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="59"/>
       <c r="F15" s="22">
         <v>45352</v>
       </c>
@@ -2704,14 +2703,15 @@
       <c r="I15" s="31"/>
       <c r="K15" s="30"/>
       <c r="L15" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="M15" s="14">
         <f>COUNTIF('College-Details'!T:T,L15)</f>
         <v>0</v>
       </c>
+      <c r="N15" s="61"/>
       <c r="O15" s="22">
-        <v>45323</v>
+        <v>45352</v>
       </c>
       <c r="P15" s="14">
         <v>0</v>
@@ -2724,13 +2724,12 @@
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="30"/>
       <c r="C16" s="14" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D16" s="14">
         <f>COUNTIF('School-Details'!U:U,C16)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="59"/>
       <c r="F16" s="22">
         <v>45383</v>
       </c>
@@ -2743,14 +2742,15 @@
       <c r="I16" s="31"/>
       <c r="K16" s="30"/>
       <c r="L16" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="M16" s="14">
         <f>COUNTIF('College-Details'!T:T,L16)</f>
         <v>0</v>
       </c>
+      <c r="N16" s="61"/>
       <c r="O16" s="22">
-        <v>45352</v>
+        <v>45383</v>
       </c>
       <c r="P16" s="14">
         <v>0</v>
@@ -2763,13 +2763,12 @@
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="30"/>
       <c r="C17" s="14" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D17" s="14">
         <f>COUNTIF('School-Details'!U:U,C17)</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="59"/>
+        <v>110</v>
+      </c>
       <c r="F17" s="22">
         <v>45413</v>
       </c>
@@ -2782,14 +2781,15 @@
       <c r="I17" s="31"/>
       <c r="K17" s="30"/>
       <c r="L17" s="14" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="M17" s="14">
         <f>COUNTIF('College-Details'!T:T,L17)</f>
-        <v>53</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N17" s="61"/>
       <c r="O17" s="22">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="P17" s="14">
         <v>0</v>
@@ -2802,13 +2802,12 @@
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="30"/>
       <c r="C18" s="14" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="D18" s="14">
         <f>COUNTIF('School-Details'!U:U,C18)</f>
-        <v>110</v>
-      </c>
-      <c r="E18" s="59"/>
+        <v>0</v>
+      </c>
       <c r="F18" s="22">
         <v>45444</v>
       </c>
@@ -2821,14 +2820,15 @@
       <c r="I18" s="31"/>
       <c r="K18" s="30"/>
       <c r="L18" s="14" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="M18" s="14">
         <f>COUNTIF('College-Details'!T:T,L18)</f>
         <v>0</v>
       </c>
+      <c r="N18" s="61"/>
       <c r="O18" s="22">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="P18" s="14">
         <v>0</v>
@@ -2840,14 +2840,13 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="30"/>
-      <c r="C19" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="D19" s="14">
-        <f>COUNTIF('School-Details'!U:U,C19)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="59"/>
+      <c r="C19" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D19" s="16">
+        <f>SUM(D11:D18)</f>
+        <v>123</v>
+      </c>
       <c r="F19" s="22">
         <v>45474</v>
       </c>
@@ -2859,15 +2858,16 @@
       </c>
       <c r="I19" s="31"/>
       <c r="K19" s="30"/>
-      <c r="L19" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="M19" s="16">
-        <f>SUM(M11:M18)</f>
+      <c r="L19" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="M19" s="14">
+        <f>COUNTIF('College-Details'!T:T,L19)</f>
         <v>53</v>
       </c>
+      <c r="N19" s="61"/>
       <c r="O19" s="22">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="P19" s="14">
         <v>0</v>
@@ -2879,14 +2879,6 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="30"/>
-      <c r="C20" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="D20" s="16">
-        <f>SUM(D12:D19)</f>
-        <v>123</v>
-      </c>
-      <c r="E20" s="59"/>
       <c r="F20" s="22">
         <v>45505</v>
       </c>
@@ -2898,8 +2890,16 @@
       </c>
       <c r="I20" s="31"/>
       <c r="K20" s="30"/>
+      <c r="L20" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="M20" s="14">
+        <f>COUNTIF('College-Details'!T:T,L20)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="61"/>
       <c r="O20" s="22">
-        <v>45474</v>
+        <v>45505</v>
       </c>
       <c r="P20" s="14">
         <v>0</v>
@@ -2910,10 +2910,13 @@
       <c r="R20" s="31"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="30"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>264</v>
+      </c>
       <c r="F21" s="22">
         <v>45536</v>
       </c>
@@ -2924,15 +2927,17 @@
         <v>0</v>
       </c>
       <c r="I21" s="31"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="21" t="s">
-        <v>370</v>
-      </c>
-      <c r="M21" s="21" t="s">
-        <v>264</v>
-      </c>
+      <c r="K21" s="30"/>
+      <c r="L21" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="M21" s="16">
+        <f>SUM(M13:M20)</f>
+        <v>53</v>
+      </c>
+      <c r="N21" s="61"/>
       <c r="O21" s="22">
-        <v>45505</v>
+        <v>45536</v>
       </c>
       <c r="P21" s="14">
         <v>0</v>
@@ -2943,14 +2948,16 @@
       <c r="R21" s="31"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="32"/>
-      <c r="C22" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="E22" s="59"/>
+      <c r="B22" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22" s="14">
+        <v>5</v>
+      </c>
+      <c r="D22" s="14">
+        <f>COUNTIF('School-Details'!T:T,C22)</f>
+        <v>10</v>
+      </c>
       <c r="F22" s="22">
         <v>45566</v>
       </c>
@@ -2961,18 +2968,12 @@
         <v>0</v>
       </c>
       <c r="I22" s="31"/>
-      <c r="K22" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="L22" s="14">
-        <v>5</v>
-      </c>
-      <c r="M22" s="14">
-        <f>COUNTIF('College-Details'!S:S,L22)</f>
-        <v>0</v>
-      </c>
+      <c r="K22" s="30"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
       <c r="O22" s="22">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="P22" s="14">
         <v>0</v>
@@ -2983,17 +2984,14 @@
       <c r="R22" s="31"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="33" t="s">
-        <v>272</v>
-      </c>
+      <c r="B23" s="33"/>
       <c r="C23" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="14">
         <f>COUNTIF('School-Details'!T:T,C23)</f>
-        <v>10</v>
-      </c>
-      <c r="E23" s="59"/>
+        <v>53</v>
+      </c>
       <c r="F23" s="22">
         <v>45597</v>
       </c>
@@ -3004,16 +3002,16 @@
         <v>0</v>
       </c>
       <c r="I23" s="31"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="14">
-        <v>4</v>
-      </c>
-      <c r="M23" s="14">
-        <f>COUNTIF('College-Details'!S:S,L23)</f>
-        <v>0</v>
-      </c>
+      <c r="K23" s="32"/>
+      <c r="L23" s="21" t="s">
+        <v>370</v>
+      </c>
+      <c r="M23" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="N23" s="61"/>
       <c r="O23" s="22">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="P23" s="14">
         <v>0</v>
@@ -3025,14 +3023,13 @@
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="33"/>
-      <c r="C24" s="14">
-        <v>4</v>
+      <c r="C24" s="14" t="s">
+        <v>275</v>
       </c>
       <c r="D24" s="14">
-        <f>COUNTIF('School-Details'!T:T,C24)</f>
-        <v>53</v>
-      </c>
-      <c r="E24" s="59"/>
+        <f>SUM(D22:D23)</f>
+        <v>63</v>
+      </c>
       <c r="F24" s="22">
         <v>45627</v>
       </c>
@@ -3043,16 +3040,19 @@
         <v>0</v>
       </c>
       <c r="I24" s="31"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="14" t="s">
-        <v>371</v>
+      <c r="K24" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="L24" s="14">
+        <v>5</v>
       </c>
       <c r="M24" s="14">
-        <f>SUM(M22:M23)</f>
-        <v>0</v>
-      </c>
+        <f>COUNTIF('College-Details'!S:S,L24)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="61"/>
       <c r="O24" s="22">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="P24" s="14">
         <v>0</v>
@@ -3063,15 +3063,16 @@
       <c r="R24" s="31"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" s="33"/>
-      <c r="C25" s="14" t="s">
-        <v>275</v>
+      <c r="B25" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="C25" s="14">
+        <v>3</v>
       </c>
       <c r="D25" s="14">
-        <f>SUM(D23:D24)</f>
-        <v>63</v>
-      </c>
-      <c r="E25" s="59"/>
+        <f>COUNTIF('School-Details'!T:T,C25)</f>
+        <v>50</v>
+      </c>
       <c r="F25" s="16" t="s">
         <v>244</v>
       </c>
@@ -3084,193 +3085,204 @@
         <v>0</v>
       </c>
       <c r="I25" s="31"/>
-      <c r="K25" s="33" t="s">
-        <v>278</v>
-      </c>
+      <c r="K25" s="33"/>
       <c r="L25" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M25" s="14">
         <f>COUNTIF('College-Details'!S:S,L25)</f>
         <v>0</v>
       </c>
-      <c r="O25" s="22">
-        <v>45627</v>
-      </c>
-      <c r="P25" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="14">
+      <c r="N25" s="61"/>
+      <c r="O25" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="P25" s="16">
+        <f>SUM(P13:P24)</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="16">
+        <f>SUM(Q13:Q24)</f>
         <v>0</v>
       </c>
       <c r="R25" s="31"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="C26" s="14">
-        <v>3</v>
+      <c r="B26" s="33"/>
+      <c r="C26" s="14" t="s">
+        <v>277</v>
       </c>
       <c r="D26" s="14">
-        <f>COUNTIF('School-Details'!T:T,C26)</f>
+        <f>SUM(D25)</f>
         <v>50</v>
       </c>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
       <c r="I26" s="31"/>
       <c r="K26" s="33"/>
       <c r="L26" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M26" s="14">
-        <f>SUM(M25)</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="P26" s="16">
-        <f>SUM(P14:P25)</f>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="16">
-        <f>SUM(Q14:Q25)</f>
-        <v>0</v>
-      </c>
+        <f>SUM(M24:M25)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="61"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="61"/>
+      <c r="Q26" s="61"/>
       <c r="R26" s="31"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="33"/>
-      <c r="C27" s="14" t="s">
-        <v>277</v>
+      <c r="B27" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="C27" s="14">
+        <v>2</v>
       </c>
       <c r="D27" s="14">
-        <f>SUM(D26)</f>
-        <v>50</v>
-      </c>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
+        <f>COUNTIF('School-Details'!T:T,C27)</f>
+        <v>10</v>
+      </c>
       <c r="I27" s="31"/>
       <c r="K27" s="33" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="L27" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M27" s="14">
         <f>COUNTIF('College-Details'!S:S,L27)</f>
         <v>0</v>
       </c>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
       <c r="R27" s="31"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" s="33" t="s">
-        <v>273</v>
-      </c>
+      <c r="B28" s="33"/>
       <c r="C28" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="14">
         <f>COUNTIF('School-Details'!T:T,C28)</f>
-        <v>10</v>
-      </c>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
+        <v>0</v>
+      </c>
       <c r="I28" s="31"/>
       <c r="K28" s="33"/>
-      <c r="L28" s="14">
-        <v>1</v>
+      <c r="L28" s="14" t="s">
+        <v>372</v>
       </c>
       <c r="M28" s="14">
-        <f>COUNTIF('College-Details'!S:S,L28)</f>
-        <v>0</v>
-      </c>
+        <f>SUM(M27)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="61"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="61"/>
       <c r="R28" s="31"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="33"/>
-      <c r="C29" s="14">
+      <c r="C29" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D29" s="14">
+        <f>SUM(D27:D28)</f>
+        <v>10</v>
+      </c>
+      <c r="I29" s="31"/>
+      <c r="K29" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="L29" s="14">
+        <v>2</v>
+      </c>
+      <c r="M29" s="14">
+        <f>COUNTIF('College-Details'!S:S,L29)</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="61"/>
+      <c r="O29" s="61"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="61"/>
+      <c r="R29" s="31"/>
+    </row>
+    <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="55"/>
+      <c r="C30" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="D30" s="56">
+        <f>D24+D26+D29</f>
+        <v>123</v>
+      </c>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="36"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="14">
         <v>1</v>
       </c>
-      <c r="D29" s="14">
-        <f>COUNTIF('School-Details'!T:T,C29)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="31"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="14" t="s">
+      <c r="M30" s="14">
+        <f>COUNTIF('College-Details'!S:S,L30)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="61"/>
+      <c r="O30" s="61"/>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="61"/>
+      <c r="R30" s="31"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="K31" s="33"/>
+      <c r="L31" s="14" t="s">
         <v>373</v>
       </c>
-      <c r="M29" s="14">
-        <f>SUM(M27:M28)</f>
-        <v>0</v>
-      </c>
-      <c r="R29" s="31"/>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B30" s="33"/>
-      <c r="C30" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="D30" s="14">
-        <f>SUM(D28:D29)</f>
-        <v>10</v>
-      </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="31"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="16" t="s">
+      <c r="M31" s="14">
+        <f>SUM(M29:M30)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="61"/>
+      <c r="O31" s="61"/>
+      <c r="P31" s="61"/>
+      <c r="Q31" s="61"/>
+      <c r="R31" s="31"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="K32" s="33"/>
+      <c r="L32" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="M30" s="16">
-        <f>M24+M26+M29</f>
-        <v>0</v>
-      </c>
-      <c r="R30" s="31"/>
-    </row>
-    <row r="31" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="62"/>
-      <c r="C31" s="63" t="s">
-        <v>244</v>
-      </c>
-      <c r="D31" s="63">
-        <f>D25+D27+D30</f>
-        <v>123</v>
-      </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="36"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="36"/>
+      <c r="M32" s="16">
+        <f>M26+M28+M31</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
+      <c r="P32" s="61"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="31"/>
+    </row>
+    <row r="33" spans="11:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K33" s="34"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="M2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated AI workshop for schools & colleges
Updated AI workshop for schools & colleges
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC592C92-F0F2-4034-88DE-AFAFD16052A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
     <sheet name="School-Details" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId3"/>
+    <sheet name="Rahul-Calls" sheetId="11" r:id="rId3"/>
     <sheet name="College-Details" sheetId="10" r:id="rId4"/>
     <sheet name="Notes" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'School-Details'!$A$1:$U$124</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,13 +41,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L28" authorId="1" shapeId="0">
+    <comment ref="L28" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -89,12 +90,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1460,7 +1461,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1834,7 +1835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1956,7 +1957,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1977,6 +1977,15 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2258,11 +2267,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2286,35 +2295,29 @@
     <row r="2" spans="2:18" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="58" t="s">
         <v>293</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="61"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="29"/>
       <c r="K2" s="27"/>
       <c r="L2" s="28"/>
-      <c r="M2" s="62" t="s">
+      <c r="M2" s="61" t="s">
         <v>374</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="64"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="63"/>
       <c r="R2" s="29"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="30"/>
       <c r="I3" s="31"/>
       <c r="K3" s="30"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
       <c r="R3" s="31"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
@@ -2341,14 +2344,12 @@
         <f>COUNTIF('College-Details'!J:J,L4)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="57"/>
       <c r="O4" s="21" t="s">
         <v>265</v>
       </c>
       <c r="P4" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="Q4" s="57"/>
       <c r="R4" s="31"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
@@ -2376,7 +2377,6 @@
         <f>COUNTIF('College-Details'!J:J,L5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="57"/>
       <c r="O5" s="14" t="s">
         <v>210</v>
       </c>
@@ -2384,7 +2384,6 @@
         <f>COUNTIF('College-Details'!L:L,O5)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="57"/>
       <c r="R5" s="31"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
@@ -2411,7 +2410,6 @@
         <f>MAX('College-Details'!A:A)</f>
         <v>53</v>
       </c>
-      <c r="N6" s="57"/>
       <c r="O6" s="14" t="s">
         <v>267</v>
       </c>
@@ -2419,7 +2417,6 @@
         <f>COUNTIF('College-Details'!L:L,O6)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="57"/>
       <c r="R6" s="31"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
@@ -2447,7 +2444,6 @@
         <f>SUM('College-Details'!I:I)/M6</f>
         <v>0</v>
       </c>
-      <c r="N7" s="57"/>
       <c r="O7" s="14" t="s">
         <v>268</v>
       </c>
@@ -2455,7 +2451,6 @@
         <f>COUNTIF('College-Details'!L:L,O7)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="57"/>
       <c r="R7" s="31"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
@@ -2480,7 +2475,6 @@
         <v>437</v>
       </c>
       <c r="M8" s="53"/>
-      <c r="N8" s="57"/>
       <c r="O8" s="14" t="s">
         <v>283</v>
       </c>
@@ -2488,7 +2482,6 @@
         <f>COUNTIF('College-Details'!L:L,O8)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="57"/>
       <c r="R8" s="31"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
@@ -2505,8 +2498,10 @@
       <c r="L9" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="M9" s="53"/>
-      <c r="N9" s="57"/>
+      <c r="M9" s="53">
+        <f ca="1">TODAY()</f>
+        <v>45302</v>
+      </c>
       <c r="O9" s="16" t="s">
         <v>244</v>
       </c>
@@ -2514,7 +2509,6 @@
         <f>SUM(P5:P8)</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="57"/>
       <c r="R9" s="31"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
@@ -2531,13 +2525,9 @@
         <v>438</v>
       </c>
       <c r="M10" s="54">
-        <f>ROUND(M14/(M9-M8+1),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="57"/>
+        <f ca="1">ROUND(M14/(M9-M8+1),0)</f>
+        <v>0</v>
+      </c>
       <c r="R10" s="31"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
@@ -2550,20 +2540,17 @@
         <v>13</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="H11" s="58"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="31"/>
       <c r="K11" s="30"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="57"/>
-      <c r="N11" s="57"/>
       <c r="O11" s="14"/>
-      <c r="P11" s="58" t="s">
+      <c r="P11" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="Q11" s="58"/>
+      <c r="Q11" s="57"/>
       <c r="R11" s="31"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
@@ -2592,7 +2579,6 @@
       <c r="M12" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="N12" s="57"/>
       <c r="O12" s="21" t="s">
         <v>269</v>
       </c>
@@ -2631,7 +2617,6 @@
         <f>COUNTIF('College-Details'!T:T,L13)</f>
         <v>0</v>
       </c>
-      <c r="N13" s="57"/>
       <c r="O13" s="22">
         <v>45292</v>
       </c>
@@ -2670,7 +2655,6 @@
         <f>COUNTIF('College-Details'!T:T,L14)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="57"/>
       <c r="O14" s="22">
         <v>45323</v>
       </c>
@@ -2709,7 +2693,6 @@
         <f>COUNTIF('College-Details'!T:T,L15)</f>
         <v>0</v>
       </c>
-      <c r="N15" s="57"/>
       <c r="O15" s="22">
         <v>45352</v>
       </c>
@@ -2748,7 +2731,6 @@
         <f>COUNTIF('College-Details'!T:T,L16)</f>
         <v>0</v>
       </c>
-      <c r="N16" s="57"/>
       <c r="O16" s="22">
         <v>45383</v>
       </c>
@@ -2787,7 +2769,6 @@
         <f>COUNTIF('College-Details'!T:T,L17)</f>
         <v>0</v>
       </c>
-      <c r="N17" s="57"/>
       <c r="O17" s="22">
         <v>45413</v>
       </c>
@@ -2826,7 +2807,6 @@
         <f>COUNTIF('College-Details'!T:T,L18)</f>
         <v>0</v>
       </c>
-      <c r="N18" s="57"/>
       <c r="O18" s="22">
         <v>45444</v>
       </c>
@@ -2865,7 +2845,6 @@
         <f>COUNTIF('College-Details'!T:T,L19)</f>
         <v>53</v>
       </c>
-      <c r="N19" s="57"/>
       <c r="O19" s="22">
         <v>45474</v>
       </c>
@@ -2897,7 +2876,6 @@
         <f>COUNTIF('College-Details'!T:T,L20)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="57"/>
       <c r="O20" s="22">
         <v>45505</v>
       </c>
@@ -2935,7 +2913,6 @@
         <f>SUM(M13:M20)</f>
         <v>53</v>
       </c>
-      <c r="N21" s="57"/>
       <c r="O21" s="22">
         <v>45536</v>
       </c>
@@ -2969,9 +2946,6 @@
       </c>
       <c r="I22" s="31"/>
       <c r="K22" s="30"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57"/>
       <c r="O22" s="22">
         <v>45566</v>
       </c>
@@ -3009,7 +2983,6 @@
       <c r="M23" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="N23" s="57"/>
       <c r="O23" s="22">
         <v>45597</v>
       </c>
@@ -3050,7 +3023,6 @@
         <f>COUNTIF('College-Details'!S:S,L24)</f>
         <v>0</v>
       </c>
-      <c r="N24" s="57"/>
       <c r="O24" s="22">
         <v>45627</v>
       </c>
@@ -3093,7 +3065,6 @@
         <f>COUNTIF('College-Details'!S:S,L25)</f>
         <v>0</v>
       </c>
-      <c r="N25" s="57"/>
       <c r="O25" s="16" t="s">
         <v>244</v>
       </c>
@@ -3125,10 +3096,6 @@
         <f>SUM(M24:M25)</f>
         <v>0</v>
       </c>
-      <c r="N26" s="57"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="57"/>
-      <c r="Q26" s="57"/>
       <c r="R26" s="31"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
@@ -3153,10 +3120,6 @@
         <f>COUNTIF('College-Details'!S:S,L27)</f>
         <v>0</v>
       </c>
-      <c r="N27" s="57"/>
-      <c r="O27" s="57"/>
-      <c r="P27" s="57"/>
-      <c r="Q27" s="57"/>
       <c r="R27" s="31"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
@@ -3177,10 +3140,6 @@
         <f>SUM(M27)</f>
         <v>0</v>
       </c>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
       <c r="R28" s="31"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
@@ -3203,10 +3162,6 @@
         <f>COUNTIF('College-Details'!S:S,L29)</f>
         <v>0</v>
       </c>
-      <c r="N29" s="57"/>
-      <c r="O29" s="57"/>
-      <c r="P29" s="57"/>
-      <c r="Q29" s="57"/>
       <c r="R29" s="31"/>
     </row>
     <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3231,10 +3186,6 @@
         <f>COUNTIF('College-Details'!S:S,L30)</f>
         <v>0</v>
       </c>
-      <c r="N30" s="57"/>
-      <c r="O30" s="57"/>
-      <c r="P30" s="57"/>
-      <c r="Q30" s="57"/>
       <c r="R30" s="31"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.3">
@@ -3246,10 +3197,6 @@
         <f>SUM(M29:M30)</f>
         <v>0</v>
       </c>
-      <c r="N31" s="57"/>
-      <c r="O31" s="57"/>
-      <c r="P31" s="57"/>
-      <c r="Q31" s="57"/>
       <c r="R31" s="31"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.3">
@@ -3261,10 +3208,6 @@
         <f>M26+M28+M31</f>
         <v>0</v>
       </c>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
       <c r="R32" s="31"/>
     </row>
     <row r="33" spans="11:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3290,7 +3233,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U124"/>
   <sheetViews>
@@ -8408,7 +8351,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U124">
+  <autoFilter ref="A1:U124" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="20">
       <filters>
         <filter val="Not-Contacted"/>
@@ -8416,66 +8359,66 @@
     </filterColumn>
   </autoFilter>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1"/>
-    <hyperlink ref="D32" r:id="rId2"/>
-    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp"/>
-    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w"/>
-    <hyperlink ref="D22" r:id="rId5"/>
-    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com"/>
-    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in"/>
-    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com"/>
-    <hyperlink ref="D30" r:id="rId9"/>
-    <hyperlink ref="D33" r:id="rId10"/>
-    <hyperlink ref="D35" r:id="rId11"/>
-    <hyperlink ref="D37" r:id="rId12"/>
-    <hyperlink ref="D41" r:id="rId13"/>
-    <hyperlink ref="D42" r:id="rId14"/>
-    <hyperlink ref="D43" r:id="rId15"/>
-    <hyperlink ref="D47" r:id="rId16"/>
-    <hyperlink ref="D48" r:id="rId17"/>
-    <hyperlink ref="D49" r:id="rId18"/>
-    <hyperlink ref="D51" r:id="rId19"/>
-    <hyperlink ref="D52" r:id="rId20"/>
-    <hyperlink ref="D53" r:id="rId21"/>
-    <hyperlink ref="D54" r:id="rId22"/>
-    <hyperlink ref="D55" r:id="rId23"/>
-    <hyperlink ref="D56" r:id="rId24"/>
-    <hyperlink ref="D57" r:id="rId25"/>
-    <hyperlink ref="D58" r:id="rId26"/>
-    <hyperlink ref="D59" r:id="rId27"/>
-    <hyperlink ref="D60" r:id="rId28"/>
-    <hyperlink ref="D61" r:id="rId29"/>
-    <hyperlink ref="D62" r:id="rId30"/>
-    <hyperlink ref="D63" r:id="rId31"/>
-    <hyperlink ref="D64" r:id="rId32"/>
-    <hyperlink ref="D65" r:id="rId33"/>
-    <hyperlink ref="D66" r:id="rId34"/>
-    <hyperlink ref="D67" r:id="rId35"/>
-    <hyperlink ref="D68" r:id="rId36"/>
-    <hyperlink ref="D69" r:id="rId37"/>
-    <hyperlink ref="D70" r:id="rId38"/>
-    <hyperlink ref="D71" r:id="rId39"/>
-    <hyperlink ref="D72" r:id="rId40"/>
-    <hyperlink ref="D73" r:id="rId41"/>
-    <hyperlink ref="D75" r:id="rId42"/>
-    <hyperlink ref="D78" r:id="rId43"/>
-    <hyperlink ref="D79" r:id="rId44"/>
-    <hyperlink ref="D80" r:id="rId45"/>
-    <hyperlink ref="D81" r:id="rId46"/>
-    <hyperlink ref="D85" r:id="rId47"/>
-    <hyperlink ref="D88" r:id="rId48"/>
-    <hyperlink ref="D89" r:id="rId49"/>
-    <hyperlink ref="D91" r:id="rId50"/>
-    <hyperlink ref="D2" r:id="rId51"/>
-    <hyperlink ref="D28" r:id="rId52"/>
+    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D32" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D22" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="D30" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D33" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="D35" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D37" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="D41" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="D42" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="D43" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="D47" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D48" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="D49" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="D51" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="D53" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="D54" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="D55" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="D56" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="D57" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="D58" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="D59" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="D60" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="D61" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="D62" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="D63" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="D64" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="D65" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="D66" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="D67" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="D68" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="D69" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="D70" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="D71" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="D72" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="D73" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="D75" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="D78" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="D79" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="D80" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="D81" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="D85" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="D88" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="D89" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="D91" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="D2" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="D28" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId53"/>
@@ -8484,18 +8427,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.44140625" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -8506,42 +8452,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>2</v>
+    <row r="2" spans="1:3" s="65" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38">
+        <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="64" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>4</v>
+    <row r="3" spans="1:3" s="65" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38">
+        <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="64" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>5</v>
+    <row r="4" spans="1:3" s="65" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="38">
+        <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="66" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>6</v>
+    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="38">
+        <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>13</v>
@@ -8550,9 +8496,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>7</v>
+    <row r="6" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="38">
+        <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>14</v>
@@ -8561,9 +8507,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>8</v>
+    <row r="7" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="38">
+        <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>15</v>
@@ -8572,9 +8518,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>9</v>
+    <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38">
+        <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>16</v>
@@ -8583,9 +8529,9 @@
         <v>9051770999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>10</v>
+    <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="38">
+        <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>17</v>
@@ -8594,9 +8540,9 @@
         <v>9903606575</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>11</v>
+    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="38">
+        <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>18</v>
@@ -8605,9 +8551,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>12</v>
+    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>19</v>
@@ -8616,9 +8562,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>15</v>
+    <row r="12" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="38">
+        <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>20</v>
@@ -8627,9 +8573,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
-        <v>19</v>
+    <row r="13" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="38">
+        <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>24</v>
@@ -8638,9 +8584,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>20</v>
+    <row r="14" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="38">
+        <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>26</v>
@@ -8649,9 +8595,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>23</v>
+    <row r="15" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38">
+        <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>29</v>
@@ -8660,9 +8606,9 @@
         <v>8961111167</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>24</v>
+    <row r="16" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="38">
+        <v>15</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>30</v>
@@ -8671,9 +8617,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>25</v>
+    <row r="17" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="38">
+        <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>31</v>
@@ -8682,9 +8628,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>26</v>
+    <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="38">
+        <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>32</v>
@@ -8693,9 +8639,9 @@
         <v>7044096127</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
-        <v>28</v>
+    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38">
+        <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>72</v>
@@ -8704,9 +8650,9 @@
         <v>9831274629</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
-        <v>29</v>
+    <row r="20" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="38">
+        <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
         <v>34</v>
@@ -8715,9 +8661,9 @@
         <v>8777257554</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
-        <v>32</v>
+    <row r="21" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38">
+        <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>76</v>
@@ -8726,9 +8672,9 @@
         <v>3322651531</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
-        <v>33</v>
+    <row r="22" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="38">
+        <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>79</v>
@@ -8737,9 +8683,9 @@
         <v>3324753015</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>35</v>
+    <row r="23" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="38">
+        <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
         <v>82</v>
@@ -8748,9 +8694,9 @@
         <v>3324753765</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
-        <v>36</v>
+    <row r="24" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="38">
+        <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>85</v>
@@ -8759,9 +8705,9 @@
         <v>3324286903</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
-        <v>37</v>
+    <row r="25" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="38">
+        <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>87</v>
@@ -8770,9 +8716,9 @@
         <v>8902488077</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
-        <v>38</v>
+    <row r="26" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="38">
+        <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
         <v>88</v>
@@ -8781,9 +8727,9 @@
         <v>9163741069</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
-        <v>39</v>
+    <row r="27" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="38">
+        <v>26</v>
       </c>
       <c r="B27" s="17" t="s">
         <v>89</v>
@@ -8792,9 +8738,9 @@
         <v>3324411691</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
-        <v>40</v>
+    <row r="28" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="38">
+        <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>90</v>
@@ -8803,9 +8749,9 @@
         <v>3324413804</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
-        <v>41</v>
+    <row r="29" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="38">
+        <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>92</v>
@@ -8814,9 +8760,9 @@
         <v>9830688888</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>42</v>
+    <row r="30" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="38">
+        <v>29</v>
       </c>
       <c r="B30" s="17" t="s">
         <v>94</v>
@@ -8825,9 +8771,9 @@
         <v>9073985531</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>43</v>
+    <row r="31" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="38">
+        <v>30</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>96</v>
@@ -8836,9 +8782,9 @@
         <v>3324712220</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
-        <v>44</v>
+    <row r="32" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="38">
+        <v>31</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>97</v>
@@ -8847,9 +8793,9 @@
         <v>3324131158</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
-        <v>45</v>
+    <row r="33" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="38">
+        <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>98</v>
@@ -8858,9 +8804,9 @@
         <v>9836242629</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
-        <v>46</v>
+    <row r="34" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="38">
+        <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>99</v>
@@ -8869,9 +8815,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
-        <v>47</v>
+    <row r="35" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="38">
+        <v>34</v>
       </c>
       <c r="B35" s="17" t="s">
         <v>102</v>
@@ -8880,9 +8826,9 @@
         <v>9051973905</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
-        <v>48</v>
+    <row r="36" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="38">
+        <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>104</v>
@@ -8891,9 +8837,9 @@
         <v>9674850783</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
-        <v>49</v>
+    <row r="37" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="38">
+        <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>106</v>
@@ -8902,9 +8848,9 @@
         <v>9674111783</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
-        <v>50</v>
+    <row r="38" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="38">
+        <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>108</v>
@@ -8913,9 +8859,9 @@
         <v>33218260082</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
-        <v>51</v>
+    <row r="39" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="38">
+        <v>38</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>110</v>
@@ -8924,9 +8870,9 @@
         <v>3322879202</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
-        <v>52</v>
+    <row r="40" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="38">
+        <v>39</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>112</v>
@@ -8935,9 +8881,9 @@
         <v>3322841546</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
-        <v>53</v>
+    <row r="41" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="38">
+        <v>40</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>114</v>
@@ -8946,9 +8892,9 @@
         <v>3322484593</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
-        <v>54</v>
+    <row r="42" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="38">
+        <v>41</v>
       </c>
       <c r="B42" s="17" t="s">
         <v>116</v>
@@ -8957,9 +8903,9 @@
         <v>3322297741</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
-        <v>55</v>
+    <row r="43" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="38">
+        <v>42</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>118</v>
@@ -8968,9 +8914,9 @@
         <v>3324793241</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
-        <v>56</v>
+    <row r="44" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="38">
+        <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>120</v>
@@ -8979,9 +8925,9 @@
         <v>3324344455</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
-        <v>57</v>
+    <row r="45" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="38">
+        <v>44</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>120</v>
@@ -8990,9 +8936,9 @@
         <v>3340083093</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
-        <v>58</v>
+    <row r="46" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="38">
+        <v>45</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>122</v>
@@ -9001,9 +8947,9 @@
         <v>3324618002</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2">
-        <v>59</v>
+    <row r="47" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="38">
+        <v>46</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>124</v>
@@ -9012,9 +8958,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="2">
-        <v>60</v>
+    <row r="48" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="38">
+        <v>47</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>127</v>
@@ -9023,9 +8969,9 @@
         <v>3324569090</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="2">
-        <v>61</v>
+    <row r="49" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="38">
+        <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>129</v>
@@ -9034,9 +8980,9 @@
         <v>3322233062</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="2">
-        <v>62</v>
+    <row r="50" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="38">
+        <v>49</v>
       </c>
       <c r="B50" s="17" t="s">
         <v>131</v>
@@ -9045,9 +8991,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="2">
-        <v>63</v>
+    <row r="51" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="38">
+        <v>50</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>134</v>
@@ -9056,9 +9002,9 @@
         <v>3324793600</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>64</v>
+    <row r="52" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="38">
+        <v>51</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>136</v>
@@ -9067,9 +9013,9 @@
         <v>3324866629</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>65</v>
+    <row r="53" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="38">
+        <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
         <v>138</v>
@@ -9078,9 +9024,9 @@
         <v>3322848038</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>66</v>
+    <row r="54" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="38">
+        <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>140</v>
@@ -9089,9 +9035,9 @@
         <v>905188888</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>67</v>
+    <row r="55" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="38">
+        <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>142</v>
@@ -9100,9 +9046,9 @@
         <v>7596949952</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A56" s="2">
-        <v>68</v>
+    <row r="56" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="38">
+        <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>144</v>
@@ -9111,9 +9057,9 @@
         <v>7478196910</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="2">
-        <v>69</v>
+    <row r="57" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="38">
+        <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>146</v>
@@ -9122,9 +9068,9 @@
         <v>7044447761</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="2">
-        <v>70</v>
+    <row r="58" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="38">
+        <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>148</v>
@@ -9133,9 +9079,9 @@
         <v>7059600647</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="2">
-        <v>71</v>
+    <row r="59" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="38">
+        <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
         <v>150</v>
@@ -9144,9 +9090,9 @@
         <v>3340072444</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>72</v>
+    <row r="60" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="38">
+        <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
         <v>152</v>
@@ -9155,9 +9101,9 @@
         <v>9903102957</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="2">
-        <v>73</v>
+    <row r="61" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="38">
+        <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>154</v>
@@ -9166,9 +9112,9 @@
         <v>7605080650</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A62" s="2">
-        <v>74</v>
+    <row r="62" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="38">
+        <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
         <v>155</v>
@@ -9177,9 +9123,9 @@
         <v>3324752135</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A63" s="2">
-        <v>75</v>
+    <row r="63" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="38">
+        <v>62</v>
       </c>
       <c r="B63" s="17" t="s">
         <v>157</v>
@@ -9188,9 +9134,9 @@
         <v>9674645471</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A64" s="2">
-        <v>76</v>
+    <row r="64" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="38">
+        <v>63</v>
       </c>
       <c r="B64" s="17" t="s">
         <v>158</v>
@@ -9199,9 +9145,9 @@
         <v>9073681886</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="2">
-        <v>77</v>
+    <row r="65" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="38">
+        <v>64</v>
       </c>
       <c r="B65" s="17" t="s">
         <v>159</v>
@@ -9210,9 +9156,9 @@
         <v>3324316997</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="2">
-        <v>78</v>
+    <row r="66" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="38">
+        <v>65</v>
       </c>
       <c r="B66" s="17" t="s">
         <v>161</v>
@@ -9221,9 +9167,9 @@
         <v>3322291779</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="2">
-        <v>79</v>
+    <row r="67" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="38">
+        <v>66</v>
       </c>
       <c r="B67" s="17" t="s">
         <v>163</v>
@@ -9232,9 +9178,9 @@
         <v>3323215151</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="2">
-        <v>80</v>
+    <row r="68" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="38">
+        <v>67</v>
       </c>
       <c r="B68" s="17" t="s">
         <v>165</v>
@@ -9243,9 +9189,9 @@
         <v>3323342404</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="2">
-        <v>81</v>
+    <row r="69" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="38">
+        <v>68</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>167</v>
@@ -9254,9 +9200,9 @@
         <v>168</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="2">
-        <v>82</v>
+    <row r="70" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="38">
+        <v>69</v>
       </c>
       <c r="B70" s="17" t="s">
         <v>169</v>
@@ -9265,9 +9211,9 @@
         <v>170</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A71" s="2">
-        <v>83</v>
+    <row r="71" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="38">
+        <v>70</v>
       </c>
       <c r="B71" s="17" t="s">
         <v>171</v>
@@ -9276,9 +9222,9 @@
         <v>9606279184</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A72" s="2">
-        <v>84</v>
+    <row r="72" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="38">
+        <v>71</v>
       </c>
       <c r="B72" s="17" t="s">
         <v>172</v>
@@ -9287,9 +9233,9 @@
         <v>8777867589</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="2">
-        <v>85</v>
+    <row r="73" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="38">
+        <v>72</v>
       </c>
       <c r="B73" s="17" t="s">
         <v>174</v>
@@ -9298,9 +9244,9 @@
         <v>8017672075</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="2">
-        <v>86</v>
+    <row r="74" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="38">
+        <v>73</v>
       </c>
       <c r="B74" s="17" t="s">
         <v>175</v>
@@ -9309,9 +9255,9 @@
         <v>3324492810</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
-        <v>87</v>
+    <row r="75" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="38">
+        <v>74</v>
       </c>
       <c r="B75" s="17" t="s">
         <v>176</v>
@@ -9320,9 +9266,9 @@
         <v>3324967196</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
-        <v>88</v>
+    <row r="76" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="38">
+        <v>75</v>
       </c>
       <c r="B76" s="17" t="s">
         <v>178</v>
@@ -9331,9 +9277,9 @@
         <v>9830701347</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
-        <v>89</v>
+    <row r="77" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="38">
+        <v>76</v>
       </c>
       <c r="B77" s="17" t="s">
         <v>180</v>
@@ -9342,9 +9288,9 @@
         <v>3324961723</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
-        <v>90</v>
+    <row r="78" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="38">
+        <v>77</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>181</v>
@@ -9353,9 +9299,9 @@
         <v>9007792852</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <v>91</v>
+    <row r="79" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="38">
+        <v>78</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>183</v>
@@ -9364,9 +9310,9 @@
         <v>8902765583</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <v>92</v>
+    <row r="80" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="38">
+        <v>79</v>
       </c>
       <c r="B80" s="17" t="s">
         <v>184</v>
@@ -9375,9 +9321,9 @@
         <v>9331866252</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <v>93</v>
+    <row r="81" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="38">
+        <v>80</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>185</v>
@@ -9386,9 +9332,9 @@
         <v>9903540099</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" s="2">
-        <v>94</v>
+    <row r="82" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="38">
+        <v>81</v>
       </c>
       <c r="B82" s="17" t="s">
         <v>186</v>
@@ -9397,9 +9343,9 @@
         <v>8336998663</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="2">
-        <v>95</v>
+    <row r="83" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="38">
+        <v>82</v>
       </c>
       <c r="B83" s="17" t="s">
         <v>187</v>
@@ -9408,9 +9354,9 @@
         <v>9339527506</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A84" s="2">
-        <v>96</v>
+    <row r="84" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="38">
+        <v>83</v>
       </c>
       <c r="B84" s="17" t="s">
         <v>188</v>
@@ -9419,9 +9365,9 @@
         <v>9903312630</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="2">
-        <v>97</v>
+    <row r="85" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="38">
+        <v>84</v>
       </c>
       <c r="B85" s="17" t="s">
         <v>189</v>
@@ -9430,9 +9376,9 @@
         <v>9836747400</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
-        <v>98</v>
+    <row r="86" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="38">
+        <v>85</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>190</v>
@@ -9441,9 +9387,9 @@
         <v>8100188019</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A87" s="2">
-        <v>99</v>
+    <row r="87" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="38">
+        <v>86</v>
       </c>
       <c r="B87" s="17" t="s">
         <v>191</v>
@@ -9452,9 +9398,9 @@
         <v>196</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A88" s="2">
-        <v>100</v>
+    <row r="88" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="38">
+        <v>87</v>
       </c>
       <c r="B88" s="17" t="s">
         <v>198</v>
@@ -9463,9 +9409,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="2">
-        <v>101</v>
+    <row r="89" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="38">
+        <v>88</v>
       </c>
       <c r="B89" s="17" t="s">
         <v>199</v>
@@ -9474,9 +9420,9 @@
         <v>200</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A90" s="2">
-        <v>102</v>
+    <row r="90" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="38">
+        <v>89</v>
       </c>
       <c r="B90" s="17" t="s">
         <v>23</v>
@@ -9485,9 +9431,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A91" s="2">
-        <v>103</v>
+    <row r="91" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="38">
+        <v>90</v>
       </c>
       <c r="B91" s="17" t="s">
         <v>192</v>
@@ -9496,9 +9442,9 @@
         <v>202</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A92" s="2">
-        <v>104</v>
+    <row r="92" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="38">
+        <v>91</v>
       </c>
       <c r="B92" s="17" t="s">
         <v>193</v>
@@ -9507,9 +9453,9 @@
         <v>203</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A93" s="2">
-        <v>105</v>
+    <row r="93" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="38">
+        <v>92</v>
       </c>
       <c r="B93" s="17" t="s">
         <v>194</v>
@@ -9518,9 +9464,9 @@
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A94" s="2">
-        <v>106</v>
+    <row r="94" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="38">
+        <v>93</v>
       </c>
       <c r="B94" s="17" t="s">
         <v>195</v>
@@ -9529,9 +9475,9 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A95" s="2">
-        <v>107</v>
+    <row r="95" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="38">
+        <v>94</v>
       </c>
       <c r="B95" s="17" t="s">
         <v>206</v>
@@ -9540,9 +9486,9 @@
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A96" s="2">
-        <v>108</v>
+    <row r="96" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="38">
+        <v>95</v>
       </c>
       <c r="B96" s="17" t="s">
         <v>208</v>
@@ -9551,9 +9497,9 @@
         <v>209</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A97" s="2">
-        <v>109</v>
+    <row r="97" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="38">
+        <v>96</v>
       </c>
       <c r="B97" s="17" t="s">
         <v>211</v>
@@ -9562,9 +9508,9 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A98" s="2">
-        <v>110</v>
+    <row r="98" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="38">
+        <v>97</v>
       </c>
       <c r="B98" s="17" t="s">
         <v>213</v>
@@ -9573,9 +9519,9 @@
         <v>214</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A99" s="2">
-        <v>111</v>
+    <row r="99" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="38">
+        <v>98</v>
       </c>
       <c r="B99" s="17" t="s">
         <v>215</v>
@@ -9584,9 +9530,9 @@
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A100" s="2">
-        <v>112</v>
+    <row r="100" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="38">
+        <v>99</v>
       </c>
       <c r="B100" s="17" t="s">
         <v>217</v>
@@ -9595,9 +9541,9 @@
         <v>218</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A101" s="2">
-        <v>113</v>
+    <row r="101" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="38">
+        <v>100</v>
       </c>
       <c r="B101" s="17" t="s">
         <v>219</v>
@@ -9606,9 +9552,9 @@
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A102" s="2">
-        <v>114</v>
+    <row r="102" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="38">
+        <v>101</v>
       </c>
       <c r="B102" s="17" t="s">
         <v>221</v>
@@ -9617,9 +9563,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A103" s="2">
-        <v>115</v>
+    <row r="103" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="38">
+        <v>102</v>
       </c>
       <c r="B103" s="17" t="s">
         <v>223</v>
@@ -9628,9 +9574,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="2">
-        <v>116</v>
+    <row r="104" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="38">
+        <v>103</v>
       </c>
       <c r="B104" s="17" t="s">
         <v>225</v>
@@ -9639,9 +9585,9 @@
         <v>226</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="2">
-        <v>117</v>
+    <row r="105" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="38">
+        <v>104</v>
       </c>
       <c r="B105" s="17" t="s">
         <v>227</v>
@@ -9650,9 +9596,9 @@
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A106" s="2">
-        <v>118</v>
+    <row r="106" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="38">
+        <v>105</v>
       </c>
       <c r="B106" s="17" t="s">
         <v>230</v>
@@ -9661,9 +9607,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="2">
-        <v>119</v>
+    <row r="107" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="38">
+        <v>106</v>
       </c>
       <c r="B107" s="17" t="s">
         <v>231</v>
@@ -9672,9 +9618,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A108" s="2">
-        <v>120</v>
+    <row r="108" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="38">
+        <v>107</v>
       </c>
       <c r="B108" s="17" t="s">
         <v>233</v>
@@ -9683,9 +9629,9 @@
         <v>234</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A109" s="2">
-        <v>121</v>
+    <row r="109" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="38">
+        <v>108</v>
       </c>
       <c r="B109" s="17" t="s">
         <v>235</v>
@@ -9694,9 +9640,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A110" s="2">
-        <v>122</v>
+    <row r="110" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="38">
+        <v>109</v>
       </c>
       <c r="B110" s="17" t="s">
         <v>435</v>
@@ -9705,9 +9651,9 @@
         <v>426</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A111" s="2">
-        <v>123</v>
+    <row r="111" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="38">
+        <v>110</v>
       </c>
       <c r="B111" s="17" t="s">
         <v>436</v>
@@ -9718,15 +9664,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp"/>
-    <hyperlink ref="C6" r:id="rId2" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w"/>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId2" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T179"/>
   <sheetViews>
     <sheetView topLeftCell="D49" workbookViewId="0">
@@ -12952,23 +12898,23 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C36" r:id="rId1"/>
-    <hyperlink ref="C37" r:id="rId2"/>
-    <hyperlink ref="D41" r:id="rId3" display="https://www.google.com/search?sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;tbs=lf:1,lf_ui:2&amp;tbm=lcl&amp;sxsrf=ACQVn0-yjBygfThguW8-plBveMrMzDiPGw:1704870884151&amp;q=engineering+colleges+in+south+calcutta&amp;rflfq=1&amp;num=10&amp;sa=X&amp;ved=2ahUKEwjQ47_7otKDAxUve2wGHY_pCzEQjGp6BAgXEAE&amp;biw=1536&amp;bih=730&amp;dpr=1.25"/>
-    <hyperlink ref="C43" r:id="rId4"/>
-    <hyperlink ref="D47" r:id="rId5" display="https://www.google.com/search?q=engineering+colleges+kolkata&amp;sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;biw=1536&amp;bih=730&amp;tbm=lcl&amp;sxsrf=ACQVn09cs4SfDApVNizAZQHyNbKrHkG1kw%3A1704870889163&amp;ei=6UOeZYunCcqWseMP2bOt0A4&amp;ved=0ahUKEwjLv_H9otKDAxVKS2wGHdlZC-oQ4dUDCAk&amp;uact=5&amp;oq=engineering+colleges+kolkata&amp;gs_lp=Eg1nd3Mtd2l6LWxvY2FsIhxlbmdpbmVlcmluZyBjb2xsZWdlcyBrb2xrYXRhMgUQABiABDIGEAAYFhgeMgYQABgWGB4yCBAAGBYYHhgPMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeSPErUNUEWOgmcAF4AJABAZgBqwGgAb0XqgEEMC4yM7gBA8gBAPgBAcICCxAAGIAEGIoFGIYDwgIEECMYJ8ICCxAAGIAEGIoFGJECwgIKEAAYgAQYFBiHAsICDhAAGIAEGIoFGJECGMkDiAYB&amp;sclient=gws-wiz-local"/>
-    <hyperlink ref="C49" r:id="rId6"/>
+    <hyperlink ref="C36" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C37" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="D41" r:id="rId3" display="https://www.google.com/search?sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;tbs=lf:1,lf_ui:2&amp;tbm=lcl&amp;sxsrf=ACQVn0-yjBygfThguW8-plBveMrMzDiPGw:1704870884151&amp;q=engineering+colleges+in+south+calcutta&amp;rflfq=1&amp;num=10&amp;sa=X&amp;ved=2ahUKEwjQ47_7otKDAxUve2wGHY_pCzEQjGp6BAgXEAE&amp;biw=1536&amp;bih=730&amp;dpr=1.25" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="C43" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="D47" r:id="rId5" display="https://www.google.com/search?q=engineering+colleges+kolkata&amp;sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;biw=1536&amp;bih=730&amp;tbm=lcl&amp;sxsrf=ACQVn09cs4SfDApVNizAZQHyNbKrHkG1kw%3A1704870889163&amp;ei=6UOeZYunCcqWseMP2bOt0A4&amp;ved=0ahUKEwjLv_H9otKDAxVKS2wGHdlZC-oQ4dUDCAk&amp;uact=5&amp;oq=engineering+colleges+kolkata&amp;gs_lp=Eg1nd3Mtd2l6LWxvY2FsIhxlbmdpbmVlcmluZyBjb2xsZWdlcyBrb2xrYXRhMgUQABiABDIGEAAYFhgeMgYQABgWGB4yCBAAGBYYHhgPMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeSPErUNUEWOgmcAF4AJABAZgBqwGgAb0XqgEEMC4yM7gBA8gBAPgBAcICCxAAGIAEGIoFGIYDwgIEECMYJ8ICCxAAGIAEGIoFGJECwgIKEAAYgAQYFBiHAsICDhAAGIAEGIoFGJECGMkDiAYB&amp;sclient=gws-wiz-local" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="C49" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -12977,7 +12923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update schools & college workshop details
Update schools & college workshop details
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC592C92-F0F2-4034-88DE-AFAFD16052A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24940854-468C-40D3-8F3C-4B0B18429C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Rahul-Calls" sheetId="11" r:id="rId3"/>
     <sheet name="College-Details" sheetId="10" r:id="rId4"/>
     <sheet name="Notes" sheetId="9" r:id="rId5"/>
+    <sheet name="Calling-Steps" sheetId="12" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'School-Details'!$A$1:$U$124</definedName>
@@ -124,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="447">
   <si>
     <t>CBSE</t>
   </si>
@@ -1456,6 +1457,27 @@
   </si>
   <si>
     <t>Today's Date</t>
+  </si>
+  <si>
+    <t>Out of 200 schools, list 100 good schools and 100 not so good schools</t>
+  </si>
+  <si>
+    <t>Out of 200 colleges, list 100 technical colleges and 100 non-technical colleges</t>
+  </si>
+  <si>
+    <t>Make a list of atleast 200 schools and 200 colleges</t>
+  </si>
+  <si>
+    <t>Get the school board name,contact person phone no &amp; contact email id</t>
+  </si>
+  <si>
+    <t>Call the contact person for free workshop</t>
+  </si>
+  <si>
+    <t>Shoot the mail to concerned person</t>
+  </si>
+  <si>
+    <t>After 1 week, do follow up for email over phone</t>
   </si>
 </sst>
 </file>
@@ -1835,7 +1857,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1957,6 +1979,15 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1978,14 +2009,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2270,7 +2298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -2295,23 +2323,23 @@
     <row r="2" spans="2:18" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="61" t="s">
         <v>293</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="60"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="63"/>
       <c r="I2" s="29"/>
       <c r="K2" s="27"/>
       <c r="L2" s="28"/>
-      <c r="M2" s="61" t="s">
+      <c r="M2" s="64" t="s">
         <v>374</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="63"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="66"/>
       <c r="R2" s="29"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
@@ -2540,17 +2568,17 @@
         <v>13</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="57" t="s">
+      <c r="G11" s="60" t="s">
         <v>210</v>
       </c>
-      <c r="H11" s="57"/>
+      <c r="H11" s="60"/>
       <c r="I11" s="31"/>
       <c r="K11" s="30"/>
       <c r="O11" s="14"/>
-      <c r="P11" s="57" t="s">
+      <c r="P11" s="60" t="s">
         <v>210</v>
       </c>
-      <c r="Q11" s="57"/>
+      <c r="Q11" s="60"/>
       <c r="R11" s="31"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
@@ -8452,36 +8480,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="65" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="58" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="65" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="58" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38">
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="57" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="65" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="58" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="59" t="s">
         <v>46</v>
       </c>
     </row>
@@ -13042,4 +13070,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F63719A-CCC7-4313-BE81-ADB215E91107}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="68" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>446</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TWO MORE SCHOOL ADDED
TWO MORE SCHOOLS ADDED
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DD5A69-2F4F-47D9-8C2E-CF3DF64FAC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4FCCBF-E9F5-4CCF-BB1D-F19F8E5E9248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="453">
   <si>
     <t>CBSE</t>
   </si>
@@ -1478,6 +1478,24 @@
   </si>
   <si>
     <t>After 1 week, do follow up for email over phone</t>
+  </si>
+  <si>
+    <t>LJD DIAMOND HARBOUR</t>
+  </si>
+  <si>
+    <t>9830028261</t>
+  </si>
+  <si>
+    <t>DIAMOND HARBOUR</t>
+  </si>
+  <si>
+    <t>Oakwood School</t>
+  </si>
+  <si>
+    <t>9330312096</t>
+  </si>
+  <si>
+    <t>KAMALGAZI</t>
   </si>
 </sst>
 </file>
@@ -2355,7 +2373,7 @@
       </c>
       <c r="D4" s="16">
         <f>MAX('School-Details'!A:A)</f>
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>265</v>
@@ -2488,7 +2506,7 @@
       </c>
       <c r="D8" s="54">
         <f ca="1">ROUND(D11/(D7-D6+1),0)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>283</v>
@@ -2565,7 +2583,7 @@
       </c>
       <c r="D11" s="14">
         <f>COUNTIF('School-Details'!U:U,C11)</f>
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="62" t="s">
@@ -2777,7 +2795,7 @@
       </c>
       <c r="D17" s="14">
         <f>COUNTIF('School-Details'!U:U,C17)</f>
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="F17" s="22">
         <v>45413</v>
@@ -2853,7 +2871,7 @@
       </c>
       <c r="D19" s="16">
         <f>SUM(D11:D18)</f>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F19" s="22">
         <v>45474</v>
@@ -2992,7 +3010,7 @@
       </c>
       <c r="D23" s="14">
         <f>COUNTIF('School-Details'!T:T,C23)</f>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F23" s="22">
         <v>45597</v>
@@ -3029,7 +3047,7 @@
       </c>
       <c r="D24" s="14">
         <f>SUM(D22:D23)</f>
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F24" s="22">
         <v>45627</v>
@@ -3199,7 +3217,7 @@
       </c>
       <c r="D30" s="56">
         <f>D24+D26+D29</f>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E30" s="35"/>
       <c r="F30" s="35"/>
@@ -3263,13 +3281,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U124"/>
+  <dimension ref="A1:U126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D123" sqref="D123"/>
+      <selection pane="bottomRight" activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3440,7 +3458,7 @@
         <v>3</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3523,7 +3541,7 @@
         <v>4</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3640,7 +3658,7 @@
         <v>3</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
@@ -3680,7 +3698,7 @@
         <v>4</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -3760,7 +3778,7 @@
         <v>4</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -3840,7 +3858,7 @@
         <v>5</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="72" hidden="1" x14ac:dyDescent="0.3">
@@ -3960,7 +3978,7 @@
         <v>5</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -4117,7 +4135,7 @@
         <v>3</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -4339,7 +4357,7 @@
         <v>4</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -4383,7 +4401,7 @@
         <v>4</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -4427,7 +4445,7 @@
         <v>4</v>
       </c>
       <c r="U27" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -4519,7 +4537,7 @@
         <v>4</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -4563,7 +4581,7 @@
         <v>3</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -4695,7 +4713,7 @@
         <v>3</v>
       </c>
       <c r="U33" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.3">
@@ -4735,7 +4753,7 @@
         <v>4</v>
       </c>
       <c r="U34" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
@@ -4869,7 +4887,7 @@
         <v>4</v>
       </c>
       <c r="U37" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.3">
@@ -4949,7 +4967,7 @@
         <v>4</v>
       </c>
       <c r="U39" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
@@ -5033,7 +5051,7 @@
         <v>4</v>
       </c>
       <c r="U41" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
@@ -6156,7 +6174,7 @@
         <v>4</v>
       </c>
       <c r="S67" s="10">
-        <f t="shared" ref="S67:S124" si="2">SUM(N67:R67)</f>
+        <f t="shared" ref="S67:S125" si="2">SUM(N67:R67)</f>
         <v>22</v>
       </c>
       <c r="T67" s="10">
@@ -6204,7 +6222,7 @@
         <v>20</v>
       </c>
       <c r="T68" s="10">
-        <f t="shared" ref="T68:T124" si="3">ROUND(S68/5,0)</f>
+        <f t="shared" ref="T68:T125" si="3">ROUND(S68/5,0)</f>
         <v>4</v>
       </c>
       <c r="U68" s="10" t="s">
@@ -8508,6 +8526,66 @@
       </c>
       <c r="U124" s="10" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="17" t="s">
+        <v>447</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="G125" s="40" t="s">
+        <v>449</v>
+      </c>
+      <c r="N125" s="1">
+        <v>1</v>
+      </c>
+      <c r="O125" s="1">
+        <v>4</v>
+      </c>
+      <c r="P125" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q125" s="1">
+        <v>4</v>
+      </c>
+      <c r="R125" s="1">
+        <v>4</v>
+      </c>
+      <c r="S125" s="1">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="T125" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U125" s="10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A126" s="2">
+        <v>125</v>
+      </c>
+      <c r="B126" s="17" t="s">
+        <v>450</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="G126" s="40" t="s">
+        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the college details
Updated the college details
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4FCCBF-E9F5-4CCF-BB1D-F19F8E5E9248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9152DADE-15E6-468B-86F6-0E6909B87A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -96,7 +96,7 @@
     <author>del</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="454">
   <si>
     <t>CBSE</t>
   </si>
@@ -1496,6 +1496,9 @@
   </si>
   <si>
     <t>KAMALGAZI</t>
+  </si>
+  <si>
+    <t>Department</t>
   </si>
 </sst>
 </file>
@@ -2316,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2387,8 +2390,8 @@
         <v>366</v>
       </c>
       <c r="M4" s="16">
-        <f>COUNTIF('College-Details'!J:J,L4)</f>
-        <v>0</v>
+        <f>COUNTIF('College-Details'!K:K,L4)</f>
+        <v>53</v>
       </c>
       <c r="O4" s="21" t="s">
         <v>265</v>
@@ -2420,14 +2423,14 @@
         <v>367</v>
       </c>
       <c r="M5" s="16">
-        <f>COUNTIF('College-Details'!J:J,L5)</f>
+        <f>COUNTIF('College-Details'!K:K,L5)</f>
         <v>0</v>
       </c>
       <c r="O5" s="14" t="s">
         <v>210</v>
       </c>
       <c r="P5" s="14">
-        <f>COUNTIF('College-Details'!L:L,O5)</f>
+        <f>COUNTIF('College-Details'!M:M,O5)</f>
         <v>0</v>
       </c>
       <c r="R5" s="31"/>
@@ -2460,7 +2463,7 @@
         <v>267</v>
       </c>
       <c r="P6" s="14">
-        <f>COUNTIF('College-Details'!L:L,O6)</f>
+        <f>COUNTIF('College-Details'!M:M,O6)</f>
         <v>0</v>
       </c>
       <c r="R6" s="31"/>
@@ -2487,14 +2490,14 @@
         <v>369</v>
       </c>
       <c r="M7" s="16">
-        <f>SUM('College-Details'!I:I)/M6</f>
+        <f>SUM('College-Details'!J:J)/M6</f>
         <v>0</v>
       </c>
       <c r="O7" s="14" t="s">
         <v>268</v>
       </c>
       <c r="P7" s="14">
-        <f>COUNTIF('College-Details'!L:L,O7)</f>
+        <f>COUNTIF('College-Details'!M:M,O7)</f>
         <v>0</v>
       </c>
       <c r="R7" s="31"/>
@@ -2506,7 +2509,7 @@
       </c>
       <c r="D8" s="54">
         <f ca="1">ROUND(D11/(D7-D6+1),0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>283</v>
@@ -2525,7 +2528,7 @@
         <v>283</v>
       </c>
       <c r="P8" s="14">
-        <f>COUNTIF('College-Details'!L:L,O8)</f>
+        <f>COUNTIF('College-Details'!M:M,O8)</f>
         <v>0</v>
       </c>
       <c r="R8" s="31"/>
@@ -2583,7 +2586,7 @@
       </c>
       <c r="D11" s="14">
         <f>COUNTIF('School-Details'!U:U,C11)</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="62" t="s">
@@ -2660,7 +2663,7 @@
         <v>251</v>
       </c>
       <c r="M13" s="14">
-        <f>COUNTIF('College-Details'!T:T,L13)</f>
+        <f>COUNTIF('College-Details'!U:U,L13)</f>
         <v>0</v>
       </c>
       <c r="O13" s="22">
@@ -2698,7 +2701,7 @@
         <v>253</v>
       </c>
       <c r="M14" s="14">
-        <f>COUNTIF('College-Details'!T:T,L14)</f>
+        <f>COUNTIF('College-Details'!U:U,L14)</f>
         <v>0</v>
       </c>
       <c r="O14" s="22">
@@ -2736,7 +2739,7 @@
         <v>255</v>
       </c>
       <c r="M15" s="14">
-        <f>COUNTIF('College-Details'!T:T,L15)</f>
+        <f>COUNTIF('College-Details'!U:U,L15)</f>
         <v>0</v>
       </c>
       <c r="O15" s="22">
@@ -2774,7 +2777,7 @@
         <v>257</v>
       </c>
       <c r="M16" s="14">
-        <f>COUNTIF('College-Details'!T:T,L16)</f>
+        <f>COUNTIF('College-Details'!U:U,L16)</f>
         <v>0</v>
       </c>
       <c r="O16" s="22">
@@ -2795,7 +2798,7 @@
       </c>
       <c r="D17" s="14">
         <f>COUNTIF('School-Details'!U:U,C17)</f>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F17" s="22">
         <v>45413</v>
@@ -2812,7 +2815,7 @@
         <v>259</v>
       </c>
       <c r="M17" s="14">
-        <f>COUNTIF('College-Details'!T:T,L17)</f>
+        <f>COUNTIF('College-Details'!U:U,L17)</f>
         <v>0</v>
       </c>
       <c r="O17" s="22">
@@ -2850,7 +2853,7 @@
         <v>261</v>
       </c>
       <c r="M18" s="14">
-        <f>COUNTIF('College-Details'!T:T,L18)</f>
+        <f>COUNTIF('College-Details'!U:U,L18)</f>
         <v>0</v>
       </c>
       <c r="O18" s="22">
@@ -2871,7 +2874,7 @@
       </c>
       <c r="D19" s="16">
         <f>SUM(D11:D18)</f>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F19" s="22">
         <v>45474</v>
@@ -2888,7 +2891,7 @@
         <v>263</v>
       </c>
       <c r="M19" s="14">
-        <f>COUNTIF('College-Details'!T:T,L19)</f>
+        <f>COUNTIF('College-Details'!U:U,L19)</f>
         <v>53</v>
       </c>
       <c r="O19" s="22">
@@ -2919,7 +2922,7 @@
         <v>279</v>
       </c>
       <c r="M20" s="14">
-        <f>COUNTIF('College-Details'!T:T,L20)</f>
+        <f>COUNTIF('College-Details'!U:U,L20)</f>
         <v>0</v>
       </c>
       <c r="O20" s="22">
@@ -3010,7 +3013,7 @@
       </c>
       <c r="D23" s="14">
         <f>COUNTIF('School-Details'!T:T,C23)</f>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F23" s="22">
         <v>45597</v>
@@ -3047,7 +3050,7 @@
       </c>
       <c r="D24" s="14">
         <f>SUM(D22:D23)</f>
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F24" s="22">
         <v>45627</v>
@@ -3066,7 +3069,7 @@
         <v>5</v>
       </c>
       <c r="M24" s="14">
-        <f>COUNTIF('College-Details'!S:S,L24)</f>
+        <f>COUNTIF('College-Details'!T:T,L24)</f>
         <v>0</v>
       </c>
       <c r="O24" s="22">
@@ -3108,7 +3111,7 @@
         <v>4</v>
       </c>
       <c r="M25" s="14">
-        <f>COUNTIF('College-Details'!S:S,L25)</f>
+        <f>COUNTIF('College-Details'!T:T,L25)</f>
         <v>0</v>
       </c>
       <c r="O25" s="16" t="s">
@@ -3163,7 +3166,7 @@
         <v>3</v>
       </c>
       <c r="M27" s="14">
-        <f>COUNTIF('College-Details'!S:S,L27)</f>
+        <f>COUNTIF('College-Details'!T:T,L27)</f>
         <v>0</v>
       </c>
       <c r="R27" s="31"/>
@@ -3205,7 +3208,7 @@
         <v>2</v>
       </c>
       <c r="M29" s="14">
-        <f>COUNTIF('College-Details'!S:S,L29)</f>
+        <f>COUNTIF('College-Details'!T:T,L29)</f>
         <v>0</v>
       </c>
       <c r="R29" s="31"/>
@@ -3217,7 +3220,7 @@
       </c>
       <c r="D30" s="56">
         <f>D24+D26+D29</f>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E30" s="35"/>
       <c r="F30" s="35"/>
@@ -3229,7 +3232,7 @@
         <v>1</v>
       </c>
       <c r="M30" s="14">
-        <f>COUNTIF('College-Details'!S:S,L30)</f>
+        <f>COUNTIF('College-Details'!T:T,L30)</f>
         <v>0</v>
       </c>
       <c r="R30" s="31"/>
@@ -3283,11 +3286,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:U126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="I114" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F127" sqref="F127"/>
+      <selection pane="bottomRight" activeCell="U126" sqref="U126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6174,7 +6177,7 @@
         <v>4</v>
       </c>
       <c r="S67" s="10">
-        <f t="shared" ref="S67:S125" si="2">SUM(N67:R67)</f>
+        <f t="shared" ref="S67:S126" si="2">SUM(N67:R67)</f>
         <v>22</v>
       </c>
       <c r="T67" s="10">
@@ -6222,7 +6225,7 @@
         <v>20</v>
       </c>
       <c r="T68" s="10">
-        <f t="shared" ref="T68:T125" si="3">ROUND(S68/5,0)</f>
+        <f t="shared" ref="T68:T126" si="3">ROUND(S68/5,0)</f>
         <v>4</v>
       </c>
       <c r="U68" s="10" t="s">
@@ -8525,7 +8528,7 @@
         <v>4</v>
       </c>
       <c r="U124" s="10" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="125" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
@@ -8586,6 +8589,32 @@
       </c>
       <c r="G126" s="40" t="s">
         <v>452</v>
+      </c>
+      <c r="N126" s="1">
+        <v>4</v>
+      </c>
+      <c r="O126" s="1">
+        <v>4</v>
+      </c>
+      <c r="P126" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q126" s="1">
+        <v>3</v>
+      </c>
+      <c r="R126" s="1">
+        <v>4</v>
+      </c>
+      <c r="S126" s="1">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="T126" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U126" s="10" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -8666,10 +8695,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:T179"/>
+  <dimension ref="A1:U179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8679,18 +8708,18 @@
     <col min="3" max="3" width="32.5546875" style="40" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" style="39" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16" style="40" customWidth="1"/>
-    <col min="8" max="10" width="11" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.6640625" style="40" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" style="1"/>
-    <col min="15" max="15" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="9.109375" style="1"/>
-    <col min="20" max="20" width="19" style="1" customWidth="1"/>
+    <col min="6" max="8" width="16" style="40" customWidth="1"/>
+    <col min="9" max="11" width="11" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" style="40" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" style="1"/>
+    <col min="16" max="16" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="9.109375" style="1"/>
+    <col min="21" max="21" width="19" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -8707,52 +8736,55 @@
         <v>4</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>282</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="R1" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="U1" s="20" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -8765,13 +8797,12 @@
       <c r="E2" s="40" t="s">
         <v>299</v>
       </c>
-      <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10">
-        <v>0</v>
-      </c>
+      <c r="K2" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="M2" s="10"/>
       <c r="N2" s="10">
         <v>0</v>
       </c>
@@ -8788,14 +8819,17 @@
         <v>0</v>
       </c>
       <c r="S2" s="10">
-        <f>ROUND(R2/5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="10">
+        <f>ROUND(S2/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -8808,8 +8842,8 @@
       <c r="E3" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="M3" s="10">
-        <v>0</v>
+      <c r="K3" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N3" s="10">
         <v>0</v>
@@ -8827,14 +8861,17 @@
         <v>0</v>
       </c>
       <c r="S3" s="10">
-        <f t="shared" ref="S3:S35" si="0">ROUND(R3/5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="10">
+        <f t="shared" ref="T3:T35" si="0">ROUND(S3/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -8847,8 +8884,8 @@
       <c r="E4" s="40" t="s">
         <v>305</v>
       </c>
-      <c r="M4" s="10">
-        <v>0</v>
+      <c r="K4" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N4" s="10">
         <v>0</v>
@@ -8866,14 +8903,17 @@
         <v>0</v>
       </c>
       <c r="S4" s="10">
+        <v>0</v>
+      </c>
+      <c r="T4" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T4" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U4" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -8886,8 +8926,8 @@
       <c r="E5" s="40" t="s">
         <v>302</v>
       </c>
-      <c r="M5" s="10">
-        <v>0</v>
+      <c r="K5" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N5" s="10">
         <v>0</v>
@@ -8905,14 +8945,17 @@
         <v>0</v>
       </c>
       <c r="S5" s="10">
+        <v>0</v>
+      </c>
+      <c r="T5" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T5" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="U5" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -8925,8 +8968,8 @@
       <c r="E6" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="M6" s="10">
-        <v>0</v>
+      <c r="K6" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N6" s="10">
         <v>0</v>
@@ -8944,14 +8987,17 @@
         <v>0</v>
       </c>
       <c r="S6" s="10">
+        <v>0</v>
+      </c>
+      <c r="T6" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T6" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="U6" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -8964,8 +9010,8 @@
       <c r="E7" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="M7" s="10">
-        <v>0</v>
+      <c r="K7" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N7" s="10">
         <v>0</v>
@@ -8983,14 +9029,17 @@
         <v>0</v>
       </c>
       <c r="S7" s="10">
+        <v>0</v>
+      </c>
+      <c r="T7" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T7" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U7" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -9000,12 +9049,12 @@
       <c r="D8" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="K8" s="40" t="s">
+      <c r="K8" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="L8" s="40" t="s">
         <v>316</v>
       </c>
-      <c r="M8" s="10">
-        <v>0</v>
-      </c>
       <c r="N8" s="10">
         <v>0</v>
       </c>
@@ -9022,14 +9071,17 @@
         <v>0</v>
       </c>
       <c r="S8" s="10">
+        <v>0</v>
+      </c>
+      <c r="T8" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T8" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U8" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -9039,8 +9091,8 @@
       <c r="D9" s="39">
         <v>9903250730</v>
       </c>
-      <c r="M9" s="10">
-        <v>0</v>
+      <c r="K9" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N9" s="10">
         <v>0</v>
@@ -9058,14 +9110,17 @@
         <v>0</v>
       </c>
       <c r="S9" s="10">
+        <v>0</v>
+      </c>
+      <c r="T9" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T9" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U9" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -9075,8 +9130,8 @@
       <c r="D10" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="M10" s="10">
-        <v>0</v>
+      <c r="K10" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N10" s="10">
         <v>0</v>
@@ -9094,14 +9149,17 @@
         <v>0</v>
       </c>
       <c r="S10" s="10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T10" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U10" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -9112,8 +9170,8 @@
       <c r="D11" s="39" t="s">
         <v>321</v>
       </c>
-      <c r="M11" s="10">
-        <v>0</v>
+      <c r="K11" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N11" s="10">
         <v>0</v>
@@ -9131,14 +9189,17 @@
         <v>0</v>
       </c>
       <c r="S11" s="10">
+        <v>0</v>
+      </c>
+      <c r="T11" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T11" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U11" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -9148,8 +9209,8 @@
       <c r="D12" s="39">
         <v>9635253261</v>
       </c>
-      <c r="M12" s="10">
-        <v>0</v>
+      <c r="K12" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N12" s="10">
         <v>0</v>
@@ -9167,14 +9228,17 @@
         <v>0</v>
       </c>
       <c r="S12" s="10">
+        <v>0</v>
+      </c>
+      <c r="T12" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T12" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U12" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -9184,8 +9248,8 @@
       <c r="D13" s="39">
         <v>8017700500</v>
       </c>
-      <c r="M13" s="10">
-        <v>0</v>
+      <c r="K13" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N13" s="10">
         <v>0</v>
@@ -9203,14 +9267,17 @@
         <v>0</v>
       </c>
       <c r="S13" s="10">
+        <v>0</v>
+      </c>
+      <c r="T13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T13" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U13" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -9220,8 +9287,8 @@
       <c r="D14" s="39">
         <v>8420123333</v>
       </c>
-      <c r="M14" s="10">
-        <v>0</v>
+      <c r="K14" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N14" s="10">
         <v>0</v>
@@ -9239,14 +9306,17 @@
         <v>0</v>
       </c>
       <c r="S14" s="10">
+        <v>0</v>
+      </c>
+      <c r="T14" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T14" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U14" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -9256,8 +9326,8 @@
       <c r="D15" s="39" t="s">
         <v>326</v>
       </c>
-      <c r="M15" s="10">
-        <v>0</v>
+      <c r="K15" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N15" s="10">
         <v>0</v>
@@ -9275,14 +9345,17 @@
         <v>0</v>
       </c>
       <c r="S15" s="10">
+        <v>0</v>
+      </c>
+      <c r="T15" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T15" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U15" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -9292,8 +9365,8 @@
       <c r="D16" s="39" t="s">
         <v>328</v>
       </c>
-      <c r="M16" s="10">
-        <v>0</v>
+      <c r="K16" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N16" s="10">
         <v>0</v>
@@ -9311,14 +9384,17 @@
         <v>0</v>
       </c>
       <c r="S16" s="10">
+        <v>0</v>
+      </c>
+      <c r="T16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T16" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U16" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -9328,8 +9404,8 @@
       <c r="D17" s="39" t="s">
         <v>330</v>
       </c>
-      <c r="M17" s="10">
-        <v>0</v>
+      <c r="K17" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N17" s="10">
         <v>0</v>
@@ -9347,14 +9423,17 @@
         <v>0</v>
       </c>
       <c r="S17" s="10">
+        <v>0</v>
+      </c>
+      <c r="T17" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T17" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U17" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -9364,8 +9443,8 @@
       <c r="D18" s="39" t="s">
         <v>332</v>
       </c>
-      <c r="M18" s="10">
-        <v>0</v>
+      <c r="K18" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N18" s="10">
         <v>0</v>
@@ -9383,14 +9462,17 @@
         <v>0</v>
       </c>
       <c r="S18" s="10">
+        <v>0</v>
+      </c>
+      <c r="T18" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T18" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U18" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -9400,8 +9482,8 @@
       <c r="D19" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="M19" s="10">
-        <v>0</v>
+      <c r="K19" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N19" s="10">
         <v>0</v>
@@ -9419,14 +9501,17 @@
         <v>0</v>
       </c>
       <c r="S19" s="10">
+        <v>0</v>
+      </c>
+      <c r="T19" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T19" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U19" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -9437,8 +9522,8 @@
       <c r="D20" s="43" t="s">
         <v>336</v>
       </c>
-      <c r="M20" s="10">
-        <v>0</v>
+      <c r="K20" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N20" s="10">
         <v>0</v>
@@ -9456,14 +9541,17 @@
         <v>0</v>
       </c>
       <c r="S20" s="10">
+        <v>0</v>
+      </c>
+      <c r="T20" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T20" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U20" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -9474,8 +9562,8 @@
       <c r="D21" s="39" t="s">
         <v>338</v>
       </c>
-      <c r="M21" s="10">
-        <v>0</v>
+      <c r="K21" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N21" s="10">
         <v>0</v>
@@ -9493,14 +9581,17 @@
         <v>0</v>
       </c>
       <c r="S21" s="10">
+        <v>0</v>
+      </c>
+      <c r="T21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T21" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U21" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -9510,8 +9601,8 @@
       <c r="D22" s="39" t="s">
         <v>340</v>
       </c>
-      <c r="M22" s="10">
-        <v>0</v>
+      <c r="K22" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N22" s="10">
         <v>0</v>
@@ -9529,14 +9620,17 @@
         <v>0</v>
       </c>
       <c r="S22" s="10">
+        <v>0</v>
+      </c>
+      <c r="T22" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T22" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U22" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -9547,8 +9641,8 @@
       <c r="D23" s="39" t="s">
         <v>342</v>
       </c>
-      <c r="M23" s="10">
-        <v>0</v>
+      <c r="K23" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N23" s="10">
         <v>0</v>
@@ -9566,14 +9660,17 @@
         <v>0</v>
       </c>
       <c r="S23" s="10">
+        <v>0</v>
+      </c>
+      <c r="T23" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T23" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U23" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -9584,8 +9681,8 @@
       <c r="D24" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="M24" s="10">
-        <v>0</v>
+      <c r="K24" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N24" s="10">
         <v>0</v>
@@ -9603,14 +9700,17 @@
         <v>0</v>
       </c>
       <c r="S24" s="10">
+        <v>0</v>
+      </c>
+      <c r="T24" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T24" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U24" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -9621,8 +9721,8 @@
       <c r="D25" s="39" t="s">
         <v>346</v>
       </c>
-      <c r="M25" s="10">
-        <v>0</v>
+      <c r="K25" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N25" s="10">
         <v>0</v>
@@ -9640,14 +9740,17 @@
         <v>0</v>
       </c>
       <c r="S25" s="10">
+        <v>0</v>
+      </c>
+      <c r="T25" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T25" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U25" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -9658,8 +9761,8 @@
       <c r="D26" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="M26" s="10">
-        <v>0</v>
+      <c r="K26" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N26" s="10">
         <v>0</v>
@@ -9677,14 +9780,17 @@
         <v>0</v>
       </c>
       <c r="S26" s="10">
+        <v>0</v>
+      </c>
+      <c r="T26" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T26" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U26" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -9694,8 +9800,8 @@
       <c r="D27" s="39" t="s">
         <v>350</v>
       </c>
-      <c r="M27" s="10">
-        <v>0</v>
+      <c r="K27" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N27" s="10">
         <v>0</v>
@@ -9713,14 +9819,17 @@
         <v>0</v>
       </c>
       <c r="S27" s="10">
+        <v>0</v>
+      </c>
+      <c r="T27" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T27" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U27" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -9730,8 +9839,8 @@
       <c r="D28" s="39" t="s">
         <v>352</v>
       </c>
-      <c r="M28" s="10">
-        <v>0</v>
+      <c r="K28" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N28" s="10">
         <v>0</v>
@@ -9749,14 +9858,17 @@
         <v>0</v>
       </c>
       <c r="S28" s="10">
+        <v>0</v>
+      </c>
+      <c r="T28" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T28" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U28" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -9767,8 +9879,8 @@
       <c r="D29" s="39" t="s">
         <v>354</v>
       </c>
-      <c r="M29" s="10">
-        <v>0</v>
+      <c r="K29" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N29" s="10">
         <v>0</v>
@@ -9786,14 +9898,17 @@
         <v>0</v>
       </c>
       <c r="S29" s="10">
+        <v>0</v>
+      </c>
+      <c r="T29" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T29" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U29" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -9804,8 +9919,8 @@
       <c r="D30" s="39" t="s">
         <v>356</v>
       </c>
-      <c r="M30" s="10">
-        <v>0</v>
+      <c r="K30" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N30" s="10">
         <v>0</v>
@@ -9823,14 +9938,17 @@
         <v>0</v>
       </c>
       <c r="S30" s="10">
+        <v>0</v>
+      </c>
+      <c r="T30" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T30" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U30" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -9841,8 +9959,8 @@
       <c r="D31" s="39" t="s">
         <v>358</v>
       </c>
-      <c r="M31" s="10">
-        <v>0</v>
+      <c r="K31" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N31" s="10">
         <v>0</v>
@@ -9860,14 +9978,17 @@
         <v>0</v>
       </c>
       <c r="S31" s="10">
+        <v>0</v>
+      </c>
+      <c r="T31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T31" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U31" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -9877,8 +9998,8 @@
       <c r="D32" s="39" t="s">
         <v>360</v>
       </c>
-      <c r="M32" s="10">
-        <v>0</v>
+      <c r="K32" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N32" s="10">
         <v>0</v>
@@ -9896,14 +10017,17 @@
         <v>0</v>
       </c>
       <c r="S32" s="10">
+        <v>0</v>
+      </c>
+      <c r="T32" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T32" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U32" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -9913,8 +10037,8 @@
       <c r="D33" s="39" t="s">
         <v>362</v>
       </c>
-      <c r="M33" s="10">
-        <v>0</v>
+      <c r="K33" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N33" s="10">
         <v>0</v>
@@ -9932,14 +10056,17 @@
         <v>0</v>
       </c>
       <c r="S33" s="10">
+        <v>0</v>
+      </c>
+      <c r="T33" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T33" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U33" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -9949,8 +10076,8 @@
       <c r="D34" s="39" t="s">
         <v>364</v>
       </c>
-      <c r="M34" s="10">
-        <v>0</v>
+      <c r="K34" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N34" s="10">
         <v>0</v>
@@ -9968,14 +10095,17 @@
         <v>0</v>
       </c>
       <c r="S34" s="10">
+        <v>0</v>
+      </c>
+      <c r="T34" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T34" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U34" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -9985,8 +10115,8 @@
       <c r="D35" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="M35" s="10">
-        <v>0</v>
+      <c r="K35" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N35" s="10">
         <v>0</v>
@@ -10004,14 +10134,17 @@
         <v>0</v>
       </c>
       <c r="S35" s="10">
+        <v>0</v>
+      </c>
+      <c r="T35" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T35" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U35" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -10027,8 +10160,8 @@
       <c r="E36" s="40" t="s">
         <v>379</v>
       </c>
-      <c r="M36" s="10">
-        <v>0</v>
+      <c r="K36" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N36" s="10">
         <v>0</v>
@@ -10046,14 +10179,17 @@
         <v>0</v>
       </c>
       <c r="S36" s="10">
-        <f t="shared" ref="S36:S54" si="1">ROUND(R36/5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="T36" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="T36" s="10">
+        <f t="shared" ref="T36:T54" si="1">ROUND(S36/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U36" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -10069,8 +10205,8 @@
       <c r="E37" s="40" t="s">
         <v>383</v>
       </c>
-      <c r="M37" s="10">
-        <v>0</v>
+      <c r="K37" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N37" s="10">
         <v>0</v>
@@ -10088,14 +10224,17 @@
         <v>0</v>
       </c>
       <c r="S37" s="10">
+        <v>0</v>
+      </c>
+      <c r="T37" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T37" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U37" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -10108,8 +10247,8 @@
       <c r="E38" s="40" t="s">
         <v>387</v>
       </c>
-      <c r="M38" s="10">
-        <v>0</v>
+      <c r="K38" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N38" s="10">
         <v>0</v>
@@ -10127,14 +10266,17 @@
         <v>0</v>
       </c>
       <c r="S38" s="10">
+        <v>0</v>
+      </c>
+      <c r="T38" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T38" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U38" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -10147,8 +10289,8 @@
       <c r="E39" s="40" t="s">
         <v>389</v>
       </c>
-      <c r="M39" s="10">
-        <v>0</v>
+      <c r="K39" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N39" s="10">
         <v>0</v>
@@ -10166,14 +10308,17 @@
         <v>0</v>
       </c>
       <c r="S39" s="10">
+        <v>0</v>
+      </c>
+      <c r="T39" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T39" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="U39" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -10186,8 +10331,8 @@
       <c r="E40" s="40" t="s">
         <v>391</v>
       </c>
-      <c r="M40" s="10">
-        <v>0</v>
+      <c r="K40" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N40" s="10">
         <v>0</v>
@@ -10205,14 +10350,17 @@
         <v>0</v>
       </c>
       <c r="S40" s="10">
+        <v>0</v>
+      </c>
+      <c r="T40" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T40" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U40" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -10225,8 +10373,8 @@
       <c r="E41" s="40" t="s">
         <v>395</v>
       </c>
-      <c r="M41" s="10">
-        <v>0</v>
+      <c r="K41" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N41" s="10">
         <v>0</v>
@@ -10244,14 +10392,17 @@
         <v>0</v>
       </c>
       <c r="S41" s="10">
+        <v>0</v>
+      </c>
+      <c r="T41" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T41" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U41" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -10264,8 +10415,8 @@
       <c r="E42" s="40" t="s">
         <v>398</v>
       </c>
-      <c r="M42" s="10">
-        <v>0</v>
+      <c r="K42" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N42" s="10">
         <v>0</v>
@@ -10283,14 +10434,17 @@
         <v>0</v>
       </c>
       <c r="S42" s="10">
+        <v>0</v>
+      </c>
+      <c r="T42" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T42" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="U42" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -10306,8 +10460,8 @@
       <c r="E43" s="40" t="s">
         <v>402</v>
       </c>
-      <c r="M43" s="10">
-        <v>0</v>
+      <c r="K43" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N43" s="10">
         <v>0</v>
@@ -10325,14 +10479,17 @@
         <v>0</v>
       </c>
       <c r="S43" s="10">
+        <v>0</v>
+      </c>
+      <c r="T43" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T43" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U43" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -10345,8 +10502,8 @@
       <c r="E44" s="40" t="s">
         <v>405</v>
       </c>
-      <c r="M44" s="10">
-        <v>0</v>
+      <c r="K44" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N44" s="10">
         <v>0</v>
@@ -10364,14 +10521,17 @@
         <v>0</v>
       </c>
       <c r="S44" s="10">
+        <v>0</v>
+      </c>
+      <c r="T44" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T44" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U44" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -10384,8 +10544,8 @@
       <c r="E45" s="40" t="s">
         <v>407</v>
       </c>
-      <c r="M45" s="10">
-        <v>0</v>
+      <c r="K45" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N45" s="10">
         <v>0</v>
@@ -10403,14 +10563,17 @@
         <v>0</v>
       </c>
       <c r="S45" s="10">
+        <v>0</v>
+      </c>
+      <c r="T45" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T45" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U45" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -10423,8 +10586,8 @@
       <c r="E46" s="40" t="s">
         <v>411</v>
       </c>
-      <c r="M46" s="10">
-        <v>0</v>
+      <c r="K46" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N46" s="10">
         <v>0</v>
@@ -10442,14 +10605,17 @@
         <v>0</v>
       </c>
       <c r="S46" s="10">
+        <v>0</v>
+      </c>
+      <c r="T46" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T46" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="U46" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -10462,8 +10628,8 @@
       <c r="E47" s="40" t="s">
         <v>414</v>
       </c>
-      <c r="M47" s="10">
-        <v>0</v>
+      <c r="K47" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N47" s="10">
         <v>0</v>
@@ -10481,14 +10647,17 @@
         <v>0</v>
       </c>
       <c r="S47" s="10">
+        <v>0</v>
+      </c>
+      <c r="T47" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T47" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U47" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -10501,8 +10670,8 @@
       <c r="E48" s="40" t="s">
         <v>407</v>
       </c>
-      <c r="M48" s="10">
-        <v>0</v>
+      <c r="K48" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N48" s="10">
         <v>0</v>
@@ -10520,14 +10689,17 @@
         <v>0</v>
       </c>
       <c r="S48" s="10">
+        <v>0</v>
+      </c>
+      <c r="T48" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T48" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="U48" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -10543,8 +10715,8 @@
       <c r="E49" s="40" t="s">
         <v>422</v>
       </c>
-      <c r="M49" s="10">
-        <v>0</v>
+      <c r="K49" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N49" s="10">
         <v>0</v>
@@ -10562,14 +10734,17 @@
         <v>0</v>
       </c>
       <c r="S49" s="10">
+        <v>0</v>
+      </c>
+      <c r="T49" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T49" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U49" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -10582,8 +10757,8 @@
       <c r="E50" s="40" t="s">
         <v>407</v>
       </c>
-      <c r="M50" s="10">
-        <v>0</v>
+      <c r="K50" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N50" s="10">
         <v>0</v>
@@ -10601,14 +10776,17 @@
         <v>0</v>
       </c>
       <c r="S50" s="10">
+        <v>0</v>
+      </c>
+      <c r="T50" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T50" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="U50" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -10621,8 +10799,8 @@
       <c r="E51" s="40" t="s">
         <v>424</v>
       </c>
-      <c r="M51" s="10">
-        <v>0</v>
+      <c r="K51" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N51" s="10">
         <v>0</v>
@@ -10640,14 +10818,17 @@
         <v>0</v>
       </c>
       <c r="S51" s="10">
+        <v>0</v>
+      </c>
+      <c r="T51" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T51" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="U51" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -10660,8 +10841,8 @@
       <c r="E52" s="40" t="s">
         <v>430</v>
       </c>
-      <c r="M52" s="10">
-        <v>0</v>
+      <c r="K52" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N52" s="10">
         <v>0</v>
@@ -10679,14 +10860,17 @@
         <v>0</v>
       </c>
       <c r="S52" s="10">
+        <v>0</v>
+      </c>
+      <c r="T52" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T52" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U52" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -10699,8 +10883,8 @@
       <c r="E53" s="40" t="s">
         <v>424</v>
       </c>
-      <c r="M53" s="10">
-        <v>0</v>
+      <c r="K53" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N53" s="10">
         <v>0</v>
@@ -10718,14 +10902,17 @@
         <v>0</v>
       </c>
       <c r="S53" s="10">
+        <v>0</v>
+      </c>
+      <c r="T53" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T53" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="U53" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -10738,8 +10925,8 @@
       <c r="E54" s="40" t="s">
         <v>414</v>
       </c>
-      <c r="M54" s="10">
-        <v>0</v>
+      <c r="K54" s="10" t="s">
+        <v>366</v>
       </c>
       <c r="N54" s="10">
         <v>0</v>
@@ -10757,1147 +10944,1150 @@
         <v>0</v>
       </c>
       <c r="S54" s="10">
+        <v>0</v>
+      </c>
+      <c r="T54" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T54" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M55" s="10"/>
+      <c r="U54" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N55" s="10"/>
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
       <c r="Q55" s="10"/>
       <c r="R55" s="10"/>
       <c r="S55" s="10"/>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M56" s="10"/>
+      <c r="T55" s="10"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N56" s="10"/>
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
       <c r="Q56" s="10"/>
       <c r="R56" s="10"/>
       <c r="S56" s="10"/>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M57" s="10"/>
+      <c r="T56" s="10"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N57" s="10"/>
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
       <c r="Q57" s="10"/>
       <c r="R57" s="10"/>
       <c r="S57" s="10"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M58" s="10"/>
+      <c r="T57" s="10"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N58" s="10"/>
       <c r="O58" s="10"/>
       <c r="P58" s="10"/>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M59" s="10"/>
+      <c r="T58" s="10"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N59" s="10"/>
       <c r="O59" s="10"/>
       <c r="P59" s="10"/>
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
       <c r="S59" s="10"/>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M60" s="10"/>
+      <c r="T59" s="10"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N60" s="10"/>
       <c r="O60" s="10"/>
       <c r="P60" s="10"/>
       <c r="Q60" s="10"/>
       <c r="R60" s="10"/>
       <c r="S60" s="10"/>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M61" s="10"/>
+      <c r="T60" s="10"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N61" s="10"/>
       <c r="O61" s="10"/>
       <c r="P61" s="10"/>
       <c r="Q61" s="10"/>
       <c r="R61" s="10"/>
       <c r="S61" s="10"/>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M62" s="10"/>
+      <c r="T61" s="10"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N62" s="10"/>
       <c r="O62" s="10"/>
       <c r="P62" s="10"/>
       <c r="Q62" s="10"/>
       <c r="R62" s="10"/>
       <c r="S62" s="10"/>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M63" s="10"/>
+      <c r="T62" s="10"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N63" s="10"/>
       <c r="O63" s="10"/>
       <c r="P63" s="10"/>
       <c r="Q63" s="10"/>
       <c r="R63" s="10"/>
       <c r="S63" s="10"/>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="M64" s="10"/>
+      <c r="T63" s="10"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="N64" s="10"/>
       <c r="O64" s="10"/>
       <c r="P64" s="10"/>
       <c r="Q64" s="10"/>
       <c r="R64" s="10"/>
       <c r="S64" s="10"/>
-    </row>
-    <row r="65" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M65" s="10"/>
+      <c r="T64" s="10"/>
+    </row>
+    <row r="65" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N65" s="10"/>
       <c r="O65" s="10"/>
       <c r="P65" s="10"/>
       <c r="Q65" s="10"/>
       <c r="R65" s="10"/>
       <c r="S65" s="10"/>
-    </row>
-    <row r="66" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M66" s="10"/>
+      <c r="T65" s="10"/>
+    </row>
+    <row r="66" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N66" s="10"/>
       <c r="O66" s="10"/>
       <c r="P66" s="10"/>
       <c r="Q66" s="10"/>
       <c r="R66" s="10"/>
       <c r="S66" s="10"/>
-    </row>
-    <row r="67" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M67" s="10"/>
+      <c r="T66" s="10"/>
+    </row>
+    <row r="67" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N67" s="10"/>
       <c r="O67" s="10"/>
       <c r="P67" s="10"/>
       <c r="Q67" s="10"/>
       <c r="R67" s="10"/>
       <c r="S67" s="10"/>
-    </row>
-    <row r="68" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M68" s="10"/>
+      <c r="T67" s="10"/>
+    </row>
+    <row r="68" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N68" s="10"/>
       <c r="O68" s="10"/>
       <c r="P68" s="10"/>
       <c r="Q68" s="10"/>
       <c r="R68" s="10"/>
       <c r="S68" s="10"/>
-    </row>
-    <row r="69" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M69" s="10"/>
+      <c r="T68" s="10"/>
+    </row>
+    <row r="69" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N69" s="10"/>
       <c r="O69" s="10"/>
       <c r="P69" s="10"/>
       <c r="Q69" s="10"/>
       <c r="R69" s="10"/>
       <c r="S69" s="10"/>
-    </row>
-    <row r="70" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M70" s="10"/>
+      <c r="T69" s="10"/>
+    </row>
+    <row r="70" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N70" s="10"/>
       <c r="O70" s="10"/>
       <c r="P70" s="10"/>
       <c r="Q70" s="10"/>
       <c r="R70" s="10"/>
       <c r="S70" s="10"/>
-    </row>
-    <row r="71" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M71" s="10"/>
+      <c r="T70" s="10"/>
+    </row>
+    <row r="71" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N71" s="10"/>
       <c r="O71" s="10"/>
       <c r="P71" s="10"/>
       <c r="Q71" s="10"/>
       <c r="R71" s="10"/>
       <c r="S71" s="10"/>
-    </row>
-    <row r="72" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M72" s="10"/>
+      <c r="T71" s="10"/>
+    </row>
+    <row r="72" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N72" s="10"/>
       <c r="O72" s="10"/>
       <c r="P72" s="10"/>
       <c r="Q72" s="10"/>
       <c r="R72" s="10"/>
       <c r="S72" s="10"/>
-    </row>
-    <row r="73" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M73" s="10"/>
+      <c r="T72" s="10"/>
+    </row>
+    <row r="73" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N73" s="10"/>
       <c r="O73" s="10"/>
       <c r="P73" s="10"/>
       <c r="Q73" s="10"/>
       <c r="R73" s="10"/>
       <c r="S73" s="10"/>
-    </row>
-    <row r="74" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M74" s="10"/>
+      <c r="T73" s="10"/>
+    </row>
+    <row r="74" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N74" s="10"/>
       <c r="O74" s="10"/>
       <c r="P74" s="10"/>
       <c r="Q74" s="10"/>
       <c r="R74" s="10"/>
       <c r="S74" s="10"/>
-    </row>
-    <row r="75" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M75" s="10"/>
+      <c r="T74" s="10"/>
+    </row>
+    <row r="75" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N75" s="10"/>
       <c r="O75" s="10"/>
       <c r="P75" s="10"/>
       <c r="Q75" s="10"/>
       <c r="R75" s="10"/>
       <c r="S75" s="10"/>
-    </row>
-    <row r="76" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M76" s="10"/>
+      <c r="T75" s="10"/>
+    </row>
+    <row r="76" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N76" s="10"/>
       <c r="O76" s="10"/>
       <c r="P76" s="10"/>
       <c r="Q76" s="10"/>
       <c r="R76" s="10"/>
       <c r="S76" s="10"/>
-    </row>
-    <row r="77" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M77" s="10"/>
+      <c r="T76" s="10"/>
+    </row>
+    <row r="77" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N77" s="10"/>
       <c r="O77" s="10"/>
       <c r="P77" s="10"/>
       <c r="Q77" s="10"/>
       <c r="R77" s="10"/>
       <c r="S77" s="10"/>
-    </row>
-    <row r="78" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M78" s="10"/>
+      <c r="T77" s="10"/>
+    </row>
+    <row r="78" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N78" s="10"/>
       <c r="O78" s="10"/>
       <c r="P78" s="10"/>
       <c r="Q78" s="10"/>
       <c r="R78" s="10"/>
       <c r="S78" s="10"/>
-    </row>
-    <row r="79" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M79" s="10"/>
+      <c r="T78" s="10"/>
+    </row>
+    <row r="79" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N79" s="10"/>
       <c r="O79" s="10"/>
       <c r="P79" s="10"/>
       <c r="Q79" s="10"/>
       <c r="R79" s="10"/>
       <c r="S79" s="10"/>
-    </row>
-    <row r="80" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M80" s="10"/>
+      <c r="T79" s="10"/>
+    </row>
+    <row r="80" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N80" s="10"/>
       <c r="O80" s="10"/>
       <c r="P80" s="10"/>
       <c r="Q80" s="10"/>
       <c r="R80" s="10"/>
       <c r="S80" s="10"/>
-    </row>
-    <row r="81" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M81" s="10"/>
+      <c r="T80" s="10"/>
+    </row>
+    <row r="81" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N81" s="10"/>
       <c r="O81" s="10"/>
       <c r="P81" s="10"/>
       <c r="Q81" s="10"/>
       <c r="R81" s="10"/>
       <c r="S81" s="10"/>
-    </row>
-    <row r="82" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M82" s="10"/>
+      <c r="T81" s="10"/>
+    </row>
+    <row r="82" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N82" s="10"/>
       <c r="O82" s="10"/>
       <c r="P82" s="10"/>
       <c r="Q82" s="10"/>
       <c r="R82" s="10"/>
       <c r="S82" s="10"/>
-    </row>
-    <row r="83" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M83" s="10"/>
+      <c r="T82" s="10"/>
+    </row>
+    <row r="83" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N83" s="10"/>
       <c r="O83" s="10"/>
       <c r="P83" s="10"/>
       <c r="Q83" s="10"/>
       <c r="R83" s="10"/>
       <c r="S83" s="10"/>
-    </row>
-    <row r="84" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M84" s="10"/>
+      <c r="T83" s="10"/>
+    </row>
+    <row r="84" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N84" s="10"/>
       <c r="O84" s="10"/>
       <c r="P84" s="10"/>
       <c r="Q84" s="10"/>
       <c r="R84" s="10"/>
       <c r="S84" s="10"/>
-    </row>
-    <row r="85" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M85" s="10"/>
+      <c r="T84" s="10"/>
+    </row>
+    <row r="85" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N85" s="10"/>
       <c r="O85" s="10"/>
       <c r="P85" s="10"/>
       <c r="Q85" s="10"/>
       <c r="R85" s="10"/>
       <c r="S85" s="10"/>
-    </row>
-    <row r="86" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M86" s="10"/>
+      <c r="T85" s="10"/>
+    </row>
+    <row r="86" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N86" s="10"/>
       <c r="O86" s="10"/>
       <c r="P86" s="10"/>
       <c r="Q86" s="10"/>
       <c r="R86" s="10"/>
       <c r="S86" s="10"/>
-    </row>
-    <row r="87" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M87" s="10"/>
+      <c r="T86" s="10"/>
+    </row>
+    <row r="87" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N87" s="10"/>
       <c r="O87" s="10"/>
       <c r="P87" s="10"/>
       <c r="Q87" s="10"/>
       <c r="R87" s="10"/>
       <c r="S87" s="10"/>
-    </row>
-    <row r="88" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M88" s="10"/>
+      <c r="T87" s="10"/>
+    </row>
+    <row r="88" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N88" s="10"/>
       <c r="O88" s="10"/>
       <c r="P88" s="10"/>
       <c r="Q88" s="10"/>
       <c r="R88" s="10"/>
       <c r="S88" s="10"/>
-    </row>
-    <row r="89" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M89" s="10"/>
+      <c r="T88" s="10"/>
+    </row>
+    <row r="89" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N89" s="10"/>
       <c r="O89" s="10"/>
       <c r="P89" s="10"/>
       <c r="Q89" s="10"/>
       <c r="R89" s="10"/>
       <c r="S89" s="10"/>
-    </row>
-    <row r="90" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M90" s="10"/>
+      <c r="T89" s="10"/>
+    </row>
+    <row r="90" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N90" s="10"/>
       <c r="O90" s="10"/>
       <c r="P90" s="10"/>
       <c r="Q90" s="10"/>
       <c r="R90" s="10"/>
       <c r="S90" s="10"/>
-    </row>
-    <row r="91" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M91" s="10"/>
+      <c r="T90" s="10"/>
+    </row>
+    <row r="91" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N91" s="10"/>
       <c r="O91" s="10"/>
       <c r="P91" s="10"/>
       <c r="Q91" s="10"/>
       <c r="R91" s="10"/>
       <c r="S91" s="10"/>
-    </row>
-    <row r="92" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M92" s="10"/>
+      <c r="T91" s="10"/>
+    </row>
+    <row r="92" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N92" s="10"/>
       <c r="O92" s="10"/>
       <c r="P92" s="10"/>
       <c r="Q92" s="10"/>
       <c r="R92" s="10"/>
       <c r="S92" s="10"/>
-    </row>
-    <row r="93" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M93" s="10"/>
+      <c r="T92" s="10"/>
+    </row>
+    <row r="93" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N93" s="10"/>
       <c r="O93" s="10"/>
       <c r="P93" s="10"/>
       <c r="Q93" s="10"/>
       <c r="R93" s="10"/>
       <c r="S93" s="10"/>
-    </row>
-    <row r="94" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M94" s="10"/>
+      <c r="T93" s="10"/>
+    </row>
+    <row r="94" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N94" s="10"/>
       <c r="O94" s="10"/>
       <c r="P94" s="10"/>
       <c r="Q94" s="10"/>
       <c r="R94" s="10"/>
       <c r="S94" s="10"/>
-    </row>
-    <row r="95" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M95" s="10"/>
+      <c r="T94" s="10"/>
+    </row>
+    <row r="95" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N95" s="10"/>
       <c r="O95" s="10"/>
       <c r="P95" s="10"/>
       <c r="Q95" s="10"/>
       <c r="R95" s="10"/>
       <c r="S95" s="10"/>
-    </row>
-    <row r="96" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M96" s="10"/>
+      <c r="T95" s="10"/>
+    </row>
+    <row r="96" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N96" s="10"/>
       <c r="O96" s="10"/>
       <c r="P96" s="10"/>
       <c r="Q96" s="10"/>
       <c r="R96" s="10"/>
       <c r="S96" s="10"/>
-    </row>
-    <row r="97" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M97" s="10"/>
+      <c r="T96" s="10"/>
+    </row>
+    <row r="97" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N97" s="10"/>
       <c r="O97" s="10"/>
       <c r="P97" s="10"/>
       <c r="Q97" s="10"/>
       <c r="R97" s="10"/>
       <c r="S97" s="10"/>
-    </row>
-    <row r="98" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M98" s="10"/>
+      <c r="T97" s="10"/>
+    </row>
+    <row r="98" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N98" s="10"/>
       <c r="O98" s="10"/>
       <c r="P98" s="10"/>
       <c r="Q98" s="10"/>
       <c r="R98" s="10"/>
       <c r="S98" s="10"/>
-    </row>
-    <row r="99" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M99" s="10"/>
+      <c r="T98" s="10"/>
+    </row>
+    <row r="99" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N99" s="10"/>
       <c r="O99" s="10"/>
       <c r="P99" s="10"/>
       <c r="Q99" s="10"/>
       <c r="R99" s="10"/>
       <c r="S99" s="10"/>
-    </row>
-    <row r="100" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M100" s="10"/>
+      <c r="T99" s="10"/>
+    </row>
+    <row r="100" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N100" s="10"/>
       <c r="O100" s="10"/>
       <c r="P100" s="10"/>
       <c r="Q100" s="10"/>
       <c r="R100" s="10"/>
       <c r="S100" s="10"/>
-    </row>
-    <row r="101" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M101" s="10"/>
+      <c r="T100" s="10"/>
+    </row>
+    <row r="101" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N101" s="10"/>
       <c r="O101" s="10"/>
       <c r="P101" s="10"/>
       <c r="Q101" s="10"/>
       <c r="R101" s="10"/>
       <c r="S101" s="10"/>
-    </row>
-    <row r="102" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M102" s="10"/>
+      <c r="T101" s="10"/>
+    </row>
+    <row r="102" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N102" s="10"/>
       <c r="O102" s="10"/>
       <c r="P102" s="10"/>
       <c r="Q102" s="10"/>
       <c r="R102" s="10"/>
       <c r="S102" s="10"/>
-    </row>
-    <row r="103" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M103" s="10"/>
+      <c r="T102" s="10"/>
+    </row>
+    <row r="103" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N103" s="10"/>
       <c r="O103" s="10"/>
       <c r="P103" s="10"/>
       <c r="Q103" s="10"/>
       <c r="R103" s="10"/>
       <c r="S103" s="10"/>
-    </row>
-    <row r="104" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M104" s="10"/>
+      <c r="T103" s="10"/>
+    </row>
+    <row r="104" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N104" s="10"/>
       <c r="O104" s="10"/>
       <c r="P104" s="10"/>
       <c r="Q104" s="10"/>
       <c r="R104" s="10"/>
       <c r="S104" s="10"/>
-    </row>
-    <row r="105" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M105" s="10"/>
+      <c r="T104" s="10"/>
+    </row>
+    <row r="105" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N105" s="10"/>
       <c r="O105" s="10"/>
       <c r="P105" s="10"/>
       <c r="Q105" s="10"/>
       <c r="R105" s="10"/>
       <c r="S105" s="10"/>
-    </row>
-    <row r="106" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M106" s="10"/>
+      <c r="T105" s="10"/>
+    </row>
+    <row r="106" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N106" s="10"/>
       <c r="O106" s="10"/>
       <c r="P106" s="10"/>
       <c r="Q106" s="10"/>
       <c r="R106" s="10"/>
       <c r="S106" s="10"/>
-    </row>
-    <row r="107" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M107" s="10"/>
+      <c r="T106" s="10"/>
+    </row>
+    <row r="107" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N107" s="10"/>
       <c r="O107" s="10"/>
       <c r="P107" s="10"/>
       <c r="Q107" s="10"/>
       <c r="R107" s="10"/>
       <c r="S107" s="10"/>
-    </row>
-    <row r="108" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M108" s="10"/>
+      <c r="T107" s="10"/>
+    </row>
+    <row r="108" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N108" s="10"/>
       <c r="O108" s="10"/>
       <c r="P108" s="10"/>
       <c r="Q108" s="10"/>
       <c r="R108" s="10"/>
       <c r="S108" s="10"/>
-    </row>
-    <row r="109" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M109" s="10"/>
+      <c r="T108" s="10"/>
+    </row>
+    <row r="109" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N109" s="10"/>
       <c r="O109" s="10"/>
       <c r="P109" s="10"/>
       <c r="Q109" s="10"/>
       <c r="R109" s="10"/>
       <c r="S109" s="10"/>
-    </row>
-    <row r="110" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M110" s="10"/>
+      <c r="T109" s="10"/>
+    </row>
+    <row r="110" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N110" s="10"/>
       <c r="O110" s="10"/>
       <c r="P110" s="10"/>
       <c r="Q110" s="10"/>
       <c r="R110" s="10"/>
       <c r="S110" s="10"/>
-    </row>
-    <row r="111" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M111" s="10"/>
+      <c r="T110" s="10"/>
+    </row>
+    <row r="111" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N111" s="10"/>
       <c r="O111" s="10"/>
       <c r="P111" s="10"/>
       <c r="Q111" s="10"/>
       <c r="R111" s="10"/>
       <c r="S111" s="10"/>
-    </row>
-    <row r="112" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M112" s="10"/>
+      <c r="T111" s="10"/>
+    </row>
+    <row r="112" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N112" s="10"/>
       <c r="O112" s="10"/>
       <c r="P112" s="10"/>
       <c r="Q112" s="10"/>
       <c r="R112" s="10"/>
       <c r="S112" s="10"/>
-    </row>
-    <row r="113" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M113" s="10"/>
+      <c r="T112" s="10"/>
+    </row>
+    <row r="113" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N113" s="10"/>
       <c r="O113" s="10"/>
       <c r="P113" s="10"/>
       <c r="Q113" s="10"/>
       <c r="R113" s="10"/>
       <c r="S113" s="10"/>
-    </row>
-    <row r="114" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M114" s="10"/>
+      <c r="T113" s="10"/>
+    </row>
+    <row r="114" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N114" s="10"/>
       <c r="O114" s="10"/>
       <c r="P114" s="10"/>
       <c r="Q114" s="10"/>
       <c r="R114" s="10"/>
       <c r="S114" s="10"/>
-    </row>
-    <row r="115" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M115" s="10"/>
+      <c r="T114" s="10"/>
+    </row>
+    <row r="115" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N115" s="10"/>
       <c r="O115" s="10"/>
       <c r="P115" s="10"/>
       <c r="Q115" s="10"/>
       <c r="R115" s="10"/>
       <c r="S115" s="10"/>
-    </row>
-    <row r="116" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M116" s="10"/>
+      <c r="T115" s="10"/>
+    </row>
+    <row r="116" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N116" s="10"/>
       <c r="O116" s="10"/>
       <c r="P116" s="10"/>
       <c r="Q116" s="10"/>
       <c r="R116" s="10"/>
       <c r="S116" s="10"/>
-    </row>
-    <row r="117" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M117" s="10"/>
+      <c r="T116" s="10"/>
+    </row>
+    <row r="117" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
       <c r="P117" s="10"/>
       <c r="Q117" s="10"/>
       <c r="R117" s="10"/>
       <c r="S117" s="10"/>
-    </row>
-    <row r="118" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M118" s="10"/>
+      <c r="T117" s="10"/>
+    </row>
+    <row r="118" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N118" s="10"/>
       <c r="O118" s="10"/>
       <c r="P118" s="10"/>
       <c r="Q118" s="10"/>
       <c r="R118" s="10"/>
       <c r="S118" s="10"/>
-    </row>
-    <row r="119" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M119" s="10"/>
+      <c r="T118" s="10"/>
+    </row>
+    <row r="119" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N119" s="10"/>
       <c r="O119" s="10"/>
       <c r="P119" s="10"/>
       <c r="Q119" s="10"/>
       <c r="R119" s="10"/>
       <c r="S119" s="10"/>
-    </row>
-    <row r="120" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M120" s="10"/>
+      <c r="T119" s="10"/>
+    </row>
+    <row r="120" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N120" s="10"/>
       <c r="O120" s="10"/>
       <c r="P120" s="10"/>
       <c r="Q120" s="10"/>
       <c r="R120" s="10"/>
       <c r="S120" s="10"/>
-    </row>
-    <row r="121" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M121" s="10"/>
+      <c r="T120" s="10"/>
+    </row>
+    <row r="121" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N121" s="10"/>
       <c r="O121" s="10"/>
       <c r="P121" s="10"/>
       <c r="Q121" s="10"/>
       <c r="R121" s="10"/>
       <c r="S121" s="10"/>
-    </row>
-    <row r="122" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M122" s="10"/>
+      <c r="T121" s="10"/>
+    </row>
+    <row r="122" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N122" s="10"/>
       <c r="O122" s="10"/>
       <c r="P122" s="10"/>
       <c r="Q122" s="10"/>
       <c r="R122" s="10"/>
       <c r="S122" s="10"/>
-    </row>
-    <row r="123" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M123" s="10"/>
+      <c r="T122" s="10"/>
+    </row>
+    <row r="123" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N123" s="10"/>
       <c r="O123" s="10"/>
       <c r="P123" s="10"/>
       <c r="Q123" s="10"/>
       <c r="R123" s="10"/>
       <c r="S123" s="10"/>
-    </row>
-    <row r="124" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M124" s="10"/>
+      <c r="T123" s="10"/>
+    </row>
+    <row r="124" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N124" s="10"/>
       <c r="O124" s="10"/>
       <c r="P124" s="10"/>
       <c r="Q124" s="10"/>
       <c r="R124" s="10"/>
       <c r="S124" s="10"/>
-    </row>
-    <row r="125" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M125" s="10"/>
+      <c r="T124" s="10"/>
+    </row>
+    <row r="125" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N125" s="10"/>
       <c r="O125" s="10"/>
       <c r="P125" s="10"/>
       <c r="Q125" s="10"/>
       <c r="R125" s="10"/>
       <c r="S125" s="10"/>
-    </row>
-    <row r="126" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M126" s="10"/>
+      <c r="T125" s="10"/>
+    </row>
+    <row r="126" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N126" s="10"/>
       <c r="O126" s="10"/>
       <c r="P126" s="10"/>
       <c r="Q126" s="10"/>
       <c r="R126" s="10"/>
       <c r="S126" s="10"/>
-    </row>
-    <row r="127" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M127" s="10"/>
+      <c r="T126" s="10"/>
+    </row>
+    <row r="127" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N127" s="10"/>
       <c r="O127" s="10"/>
       <c r="P127" s="10"/>
       <c r="Q127" s="10"/>
       <c r="R127" s="10"/>
       <c r="S127" s="10"/>
-    </row>
-    <row r="128" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M128" s="10"/>
+      <c r="T127" s="10"/>
+    </row>
+    <row r="128" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N128" s="10"/>
       <c r="O128" s="10"/>
       <c r="P128" s="10"/>
       <c r="Q128" s="10"/>
       <c r="R128" s="10"/>
       <c r="S128" s="10"/>
-    </row>
-    <row r="129" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M129" s="10"/>
+      <c r="T128" s="10"/>
+    </row>
+    <row r="129" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N129" s="10"/>
       <c r="O129" s="10"/>
       <c r="P129" s="10"/>
       <c r="Q129" s="10"/>
       <c r="R129" s="10"/>
       <c r="S129" s="10"/>
-    </row>
-    <row r="130" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M130" s="10"/>
+      <c r="T129" s="10"/>
+    </row>
+    <row r="130" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N130" s="10"/>
       <c r="O130" s="10"/>
       <c r="P130" s="10"/>
       <c r="Q130" s="10"/>
       <c r="R130" s="10"/>
       <c r="S130" s="10"/>
-    </row>
-    <row r="131" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M131" s="10"/>
+      <c r="T130" s="10"/>
+    </row>
+    <row r="131" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N131" s="10"/>
       <c r="O131" s="10"/>
       <c r="P131" s="10"/>
       <c r="Q131" s="10"/>
       <c r="R131" s="10"/>
       <c r="S131" s="10"/>
-    </row>
-    <row r="132" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M132" s="10"/>
+      <c r="T131" s="10"/>
+    </row>
+    <row r="132" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N132" s="10"/>
       <c r="O132" s="10"/>
       <c r="P132" s="10"/>
       <c r="Q132" s="10"/>
       <c r="R132" s="10"/>
       <c r="S132" s="10"/>
-    </row>
-    <row r="133" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M133" s="10"/>
+      <c r="T132" s="10"/>
+    </row>
+    <row r="133" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N133" s="10"/>
       <c r="O133" s="10"/>
       <c r="P133" s="10"/>
       <c r="Q133" s="10"/>
       <c r="R133" s="10"/>
       <c r="S133" s="10"/>
-    </row>
-    <row r="134" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M134" s="10"/>
+      <c r="T133" s="10"/>
+    </row>
+    <row r="134" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N134" s="10"/>
       <c r="O134" s="10"/>
       <c r="P134" s="10"/>
       <c r="Q134" s="10"/>
       <c r="R134" s="10"/>
       <c r="S134" s="10"/>
-    </row>
-    <row r="135" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M135" s="10"/>
+      <c r="T134" s="10"/>
+    </row>
+    <row r="135" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N135" s="10"/>
       <c r="O135" s="10"/>
       <c r="P135" s="10"/>
       <c r="Q135" s="10"/>
       <c r="R135" s="10"/>
       <c r="S135" s="10"/>
-    </row>
-    <row r="136" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M136" s="10"/>
+      <c r="T135" s="10"/>
+    </row>
+    <row r="136" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N136" s="10"/>
       <c r="O136" s="10"/>
       <c r="P136" s="10"/>
       <c r="Q136" s="10"/>
       <c r="R136" s="10"/>
       <c r="S136" s="10"/>
-    </row>
-    <row r="137" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M137" s="10"/>
+      <c r="T136" s="10"/>
+    </row>
+    <row r="137" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N137" s="10"/>
       <c r="O137" s="10"/>
       <c r="P137" s="10"/>
       <c r="Q137" s="10"/>
       <c r="R137" s="10"/>
       <c r="S137" s="10"/>
-    </row>
-    <row r="138" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M138" s="10"/>
+      <c r="T137" s="10"/>
+    </row>
+    <row r="138" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N138" s="10"/>
       <c r="O138" s="10"/>
       <c r="P138" s="10"/>
       <c r="Q138" s="10"/>
       <c r="R138" s="10"/>
       <c r="S138" s="10"/>
-    </row>
-    <row r="139" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M139" s="10"/>
+      <c r="T138" s="10"/>
+    </row>
+    <row r="139" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N139" s="10"/>
       <c r="O139" s="10"/>
       <c r="P139" s="10"/>
       <c r="Q139" s="10"/>
       <c r="R139" s="10"/>
       <c r="S139" s="10"/>
-    </row>
-    <row r="140" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M140" s="10"/>
+      <c r="T139" s="10"/>
+    </row>
+    <row r="140" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N140" s="10"/>
       <c r="O140" s="10"/>
       <c r="P140" s="10"/>
       <c r="Q140" s="10"/>
       <c r="R140" s="10"/>
       <c r="S140" s="10"/>
-    </row>
-    <row r="141" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M141" s="10"/>
+      <c r="T140" s="10"/>
+    </row>
+    <row r="141" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N141" s="10"/>
       <c r="O141" s="10"/>
       <c r="P141" s="10"/>
       <c r="Q141" s="10"/>
       <c r="R141" s="10"/>
       <c r="S141" s="10"/>
-    </row>
-    <row r="142" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M142" s="10"/>
+      <c r="T141" s="10"/>
+    </row>
+    <row r="142" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N142" s="10"/>
       <c r="O142" s="10"/>
       <c r="P142" s="10"/>
       <c r="Q142" s="10"/>
       <c r="R142" s="10"/>
       <c r="S142" s="10"/>
-    </row>
-    <row r="143" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M143" s="10"/>
+      <c r="T142" s="10"/>
+    </row>
+    <row r="143" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N143" s="10"/>
       <c r="O143" s="10"/>
       <c r="P143" s="10"/>
       <c r="Q143" s="10"/>
       <c r="R143" s="10"/>
       <c r="S143" s="10"/>
-    </row>
-    <row r="144" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M144" s="10"/>
+      <c r="T143" s="10"/>
+    </row>
+    <row r="144" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N144" s="10"/>
       <c r="O144" s="10"/>
       <c r="P144" s="10"/>
       <c r="Q144" s="10"/>
       <c r="R144" s="10"/>
       <c r="S144" s="10"/>
-    </row>
-    <row r="145" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M145" s="10"/>
+      <c r="T144" s="10"/>
+    </row>
+    <row r="145" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N145" s="10"/>
       <c r="O145" s="10"/>
       <c r="P145" s="10"/>
       <c r="Q145" s="10"/>
       <c r="R145" s="10"/>
       <c r="S145" s="10"/>
-    </row>
-    <row r="146" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M146" s="10"/>
+      <c r="T145" s="10"/>
+    </row>
+    <row r="146" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N146" s="10"/>
       <c r="O146" s="10"/>
       <c r="P146" s="10"/>
       <c r="Q146" s="10"/>
       <c r="R146" s="10"/>
       <c r="S146" s="10"/>
-    </row>
-    <row r="147" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M147" s="10"/>
+      <c r="T146" s="10"/>
+    </row>
+    <row r="147" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N147" s="10"/>
       <c r="O147" s="10"/>
       <c r="P147" s="10"/>
       <c r="Q147" s="10"/>
       <c r="R147" s="10"/>
       <c r="S147" s="10"/>
-    </row>
-    <row r="148" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M148" s="10"/>
+      <c r="T147" s="10"/>
+    </row>
+    <row r="148" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N148" s="10"/>
       <c r="O148" s="10"/>
       <c r="P148" s="10"/>
       <c r="Q148" s="10"/>
       <c r="R148" s="10"/>
       <c r="S148" s="10"/>
-    </row>
-    <row r="149" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M149" s="10"/>
+      <c r="T148" s="10"/>
+    </row>
+    <row r="149" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N149" s="10"/>
       <c r="O149" s="10"/>
       <c r="P149" s="10"/>
       <c r="Q149" s="10"/>
       <c r="R149" s="10"/>
       <c r="S149" s="10"/>
-    </row>
-    <row r="150" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M150" s="10"/>
+      <c r="T149" s="10"/>
+    </row>
+    <row r="150" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N150" s="10"/>
       <c r="O150" s="10"/>
       <c r="P150" s="10"/>
       <c r="Q150" s="10"/>
       <c r="R150" s="10"/>
       <c r="S150" s="10"/>
-    </row>
-    <row r="151" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M151" s="10"/>
+      <c r="T150" s="10"/>
+    </row>
+    <row r="151" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N151" s="10"/>
       <c r="O151" s="10"/>
       <c r="P151" s="10"/>
       <c r="Q151" s="10"/>
       <c r="R151" s="10"/>
       <c r="S151" s="10"/>
-    </row>
-    <row r="152" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M152" s="10"/>
+      <c r="T151" s="10"/>
+    </row>
+    <row r="152" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N152" s="10"/>
       <c r="O152" s="10"/>
       <c r="P152" s="10"/>
       <c r="Q152" s="10"/>
       <c r="R152" s="10"/>
       <c r="S152" s="10"/>
-    </row>
-    <row r="153" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M153" s="10"/>
+      <c r="T152" s="10"/>
+    </row>
+    <row r="153" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N153" s="10"/>
       <c r="O153" s="10"/>
       <c r="P153" s="10"/>
       <c r="Q153" s="10"/>
       <c r="R153" s="10"/>
       <c r="S153" s="10"/>
-    </row>
-    <row r="154" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M154" s="10"/>
+      <c r="T153" s="10"/>
+    </row>
+    <row r="154" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N154" s="10"/>
       <c r="O154" s="10"/>
       <c r="P154" s="10"/>
       <c r="Q154" s="10"/>
       <c r="R154" s="10"/>
       <c r="S154" s="10"/>
-    </row>
-    <row r="155" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M155" s="10"/>
+      <c r="T154" s="10"/>
+    </row>
+    <row r="155" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N155" s="10"/>
       <c r="O155" s="10"/>
       <c r="P155" s="10"/>
       <c r="Q155" s="10"/>
       <c r="R155" s="10"/>
       <c r="S155" s="10"/>
-    </row>
-    <row r="156" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M156" s="10"/>
+      <c r="T155" s="10"/>
+    </row>
+    <row r="156" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N156" s="10"/>
       <c r="O156" s="10"/>
       <c r="P156" s="10"/>
       <c r="Q156" s="10"/>
       <c r="R156" s="10"/>
       <c r="S156" s="10"/>
-    </row>
-    <row r="157" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M157" s="10"/>
+      <c r="T156" s="10"/>
+    </row>
+    <row r="157" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N157" s="10"/>
       <c r="O157" s="10"/>
       <c r="P157" s="10"/>
       <c r="Q157" s="10"/>
       <c r="R157" s="10"/>
       <c r="S157" s="10"/>
-    </row>
-    <row r="158" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M158" s="10"/>
+      <c r="T157" s="10"/>
+    </row>
+    <row r="158" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N158" s="10"/>
       <c r="O158" s="10"/>
       <c r="P158" s="10"/>
       <c r="Q158" s="10"/>
       <c r="R158" s="10"/>
       <c r="S158" s="10"/>
-    </row>
-    <row r="159" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M159" s="10"/>
+      <c r="T158" s="10"/>
+    </row>
+    <row r="159" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N159" s="10"/>
       <c r="O159" s="10"/>
       <c r="P159" s="10"/>
       <c r="Q159" s="10"/>
       <c r="R159" s="10"/>
       <c r="S159" s="10"/>
-    </row>
-    <row r="160" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M160" s="10"/>
+      <c r="T159" s="10"/>
+    </row>
+    <row r="160" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N160" s="10"/>
       <c r="O160" s="10"/>
       <c r="P160" s="10"/>
       <c r="Q160" s="10"/>
       <c r="R160" s="10"/>
       <c r="S160" s="10"/>
-    </row>
-    <row r="161" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M161" s="10"/>
+      <c r="T160" s="10"/>
+    </row>
+    <row r="161" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N161" s="10"/>
       <c r="O161" s="10"/>
       <c r="P161" s="10"/>
       <c r="Q161" s="10"/>
       <c r="R161" s="10"/>
       <c r="S161" s="10"/>
-    </row>
-    <row r="162" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M162" s="10"/>
+      <c r="T161" s="10"/>
+    </row>
+    <row r="162" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N162" s="10"/>
       <c r="O162" s="10"/>
       <c r="P162" s="10"/>
       <c r="Q162" s="10"/>
       <c r="R162" s="10"/>
       <c r="S162" s="10"/>
-    </row>
-    <row r="163" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M163" s="10"/>
+      <c r="T162" s="10"/>
+    </row>
+    <row r="163" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N163" s="10"/>
       <c r="O163" s="10"/>
       <c r="P163" s="10"/>
       <c r="Q163" s="10"/>
       <c r="R163" s="10"/>
       <c r="S163" s="10"/>
-    </row>
-    <row r="164" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M164" s="10"/>
+      <c r="T163" s="10"/>
+    </row>
+    <row r="164" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N164" s="10"/>
       <c r="O164" s="10"/>
       <c r="P164" s="10"/>
       <c r="Q164" s="10"/>
       <c r="R164" s="10"/>
       <c r="S164" s="10"/>
-    </row>
-    <row r="165" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M165" s="10"/>
+      <c r="T164" s="10"/>
+    </row>
+    <row r="165" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N165" s="10"/>
       <c r="O165" s="10"/>
       <c r="P165" s="10"/>
       <c r="Q165" s="10"/>
       <c r="R165" s="10"/>
       <c r="S165" s="10"/>
-    </row>
-    <row r="166" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M166" s="10"/>
+      <c r="T165" s="10"/>
+    </row>
+    <row r="166" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N166" s="10"/>
       <c r="O166" s="10"/>
       <c r="P166" s="10"/>
       <c r="Q166" s="10"/>
       <c r="R166" s="10"/>
       <c r="S166" s="10"/>
-    </row>
-    <row r="167" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M167" s="10"/>
+      <c r="T166" s="10"/>
+    </row>
+    <row r="167" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N167" s="10"/>
       <c r="O167" s="10"/>
       <c r="P167" s="10"/>
       <c r="Q167" s="10"/>
       <c r="R167" s="10"/>
       <c r="S167" s="10"/>
-    </row>
-    <row r="168" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M168" s="10"/>
+      <c r="T167" s="10"/>
+    </row>
+    <row r="168" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N168" s="10"/>
       <c r="O168" s="10"/>
       <c r="P168" s="10"/>
       <c r="Q168" s="10"/>
       <c r="R168" s="10"/>
       <c r="S168" s="10"/>
-    </row>
-    <row r="169" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M169" s="10"/>
+      <c r="T168" s="10"/>
+    </row>
+    <row r="169" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N169" s="10"/>
       <c r="O169" s="10"/>
       <c r="P169" s="10"/>
       <c r="Q169" s="10"/>
       <c r="R169" s="10"/>
       <c r="S169" s="10"/>
-    </row>
-    <row r="170" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M170" s="10"/>
+      <c r="T169" s="10"/>
+    </row>
+    <row r="170" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N170" s="10"/>
       <c r="O170" s="10"/>
       <c r="P170" s="10"/>
       <c r="Q170" s="10"/>
       <c r="R170" s="10"/>
       <c r="S170" s="10"/>
-    </row>
-    <row r="171" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M171" s="10"/>
+      <c r="T170" s="10"/>
+    </row>
+    <row r="171" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N171" s="10"/>
       <c r="O171" s="10"/>
       <c r="P171" s="10"/>
       <c r="Q171" s="10"/>
       <c r="R171" s="10"/>
       <c r="S171" s="10"/>
-    </row>
-    <row r="172" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M172" s="10"/>
+      <c r="T171" s="10"/>
+    </row>
+    <row r="172" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N172" s="10"/>
       <c r="O172" s="10"/>
       <c r="P172" s="10"/>
       <c r="Q172" s="10"/>
       <c r="R172" s="10"/>
       <c r="S172" s="10"/>
-    </row>
-    <row r="173" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M173" s="10"/>
+      <c r="T172" s="10"/>
+    </row>
+    <row r="173" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N173" s="10"/>
       <c r="O173" s="10"/>
       <c r="P173" s="10"/>
       <c r="Q173" s="10"/>
       <c r="R173" s="10"/>
       <c r="S173" s="10"/>
-    </row>
-    <row r="174" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M174" s="10"/>
+      <c r="T173" s="10"/>
+    </row>
+    <row r="174" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N174" s="10"/>
       <c r="O174" s="10"/>
       <c r="P174" s="10"/>
       <c r="Q174" s="10"/>
       <c r="R174" s="10"/>
       <c r="S174" s="10"/>
-    </row>
-    <row r="175" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M175" s="10"/>
+      <c r="T174" s="10"/>
+    </row>
+    <row r="175" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N175" s="10"/>
       <c r="O175" s="10"/>
       <c r="P175" s="10"/>
       <c r="Q175" s="10"/>
       <c r="R175" s="10"/>
       <c r="S175" s="10"/>
-    </row>
-    <row r="176" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M176" s="10"/>
+      <c r="T175" s="10"/>
+    </row>
+    <row r="176" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N176" s="10"/>
       <c r="O176" s="10"/>
       <c r="P176" s="10"/>
       <c r="Q176" s="10"/>
       <c r="R176" s="10"/>
       <c r="S176" s="10"/>
-    </row>
-    <row r="177" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M177" s="10"/>
+      <c r="T176" s="10"/>
+    </row>
+    <row r="177" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N177" s="10"/>
       <c r="O177" s="10"/>
       <c r="P177" s="10"/>
       <c r="Q177" s="10"/>
       <c r="R177" s="10"/>
       <c r="S177" s="10"/>
-    </row>
-    <row r="178" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M178" s="10"/>
+      <c r="T177" s="10"/>
+    </row>
+    <row r="178" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N178" s="10"/>
       <c r="O178" s="10"/>
       <c r="P178" s="10"/>
       <c r="Q178" s="10"/>
       <c r="R178" s="10"/>
       <c r="S178" s="10"/>
-    </row>
-    <row r="179" spans="13:19" x14ac:dyDescent="0.3">
-      <c r="M179" s="10"/>
+      <c r="T178" s="10"/>
+    </row>
+    <row r="179" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N179" s="10"/>
       <c r="O179" s="10"/>
       <c r="P179" s="10"/>
       <c r="Q179" s="10"/>
       <c r="R179" s="10"/>
       <c r="S179" s="10"/>
+      <c r="T179" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L1:L1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated AI School & College
Updated AI School & College
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C3D120-9BD7-471E-97C9-E0A1732F57EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F47CDD-DE6C-444A-A24A-8BAABF6F1B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="507">
   <si>
     <t>CBSE</t>
   </si>
@@ -1604,13 +1604,67 @@
   </si>
   <si>
     <t>https://sriaurobindoschools.org/tffs/</t>
+  </si>
+  <si>
+    <t>nivaananda@yahoo.com</t>
+  </si>
+  <si>
+    <t>depaulschooljayanpur@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.silverpointschool.org/#</t>
+  </si>
+  <si>
+    <t>info@npskolkata.com</t>
+  </si>
+  <si>
+    <t>mhmscal@gmail.com</t>
+  </si>
+  <si>
+    <t>hlpsbhs@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@gardenhighschool.org </t>
+  </si>
+  <si>
+    <t>admission@sishowrah.com</t>
+  </si>
+  <si>
+    <t>nalanda_vidyapith@rediffmail.com</t>
+  </si>
+  <si>
+    <t>ssmacademy.org@gmail.com</t>
+  </si>
+  <si>
+    <t>akshar1998@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enquiries@theoxfordacademy.org </t>
+  </si>
+  <si>
+    <t>ariff.mohsin64@gmail.com</t>
+  </si>
+  <si>
+    <t>http://www.alpsconvert.in</t>
+  </si>
+  <si>
+    <t>http://www.shreebharati.com/033%2024913227%20(head%20mistress)</t>
+  </si>
+  <si>
+    <t>http://srichaitanyatechnoschooln.in/#</t>
+  </si>
+  <si>
+    <t>Sri Chaitanyo Techno New Town</t>
+  </si>
+  <si>
+    <t>033-25535566</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1736,6 +1790,18 @@
     <font>
       <sz val="10"/>
       <color rgb="FF422E59"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF575757"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF404040"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2001,7 +2067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2141,6 +2207,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2470,23 +2539,23 @@
     <row r="2" spans="2:18" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="69" t="s">
         <v>293</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
       <c r="I2" s="29"/>
       <c r="K2" s="27"/>
       <c r="L2" s="28"/>
-      <c r="M2" s="69" t="s">
+      <c r="M2" s="72" t="s">
         <v>374</v>
       </c>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="71"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="74"/>
       <c r="R2" s="29"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
@@ -2556,7 +2625,7 @@
         <v>210</v>
       </c>
       <c r="P5" s="14">
-        <f>COUNTIF('College-Details'!M:M,O5)</f>
+        <f>COUNTIF('College-Details'!N:N,O5)</f>
         <v>0</v>
       </c>
       <c r="R5" s="31"/>
@@ -2589,7 +2658,7 @@
         <v>267</v>
       </c>
       <c r="P6" s="14">
-        <f>COUNTIF('College-Details'!M:M,O6)</f>
+        <f>COUNTIF('College-Details'!N:N,O6)</f>
         <v>0</v>
       </c>
       <c r="R6" s="31"/>
@@ -2623,7 +2692,7 @@
         <v>268</v>
       </c>
       <c r="P7" s="14">
-        <f>COUNTIF('College-Details'!M:M,O7)</f>
+        <f>COUNTIF('College-Details'!N:N,O7)</f>
         <v>0</v>
       </c>
       <c r="R7" s="31"/>
@@ -2654,7 +2723,7 @@
         <v>283</v>
       </c>
       <c r="P8" s="14">
-        <f>COUNTIF('College-Details'!M:M,O8)</f>
+        <f>COUNTIF('College-Details'!N:N,O8)</f>
         <v>0</v>
       </c>
       <c r="R8" s="31"/>
@@ -2715,17 +2784,17 @@
         <v>34</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="65" t="s">
+      <c r="G11" s="68" t="s">
         <v>210</v>
       </c>
-      <c r="H11" s="65"/>
+      <c r="H11" s="68"/>
       <c r="I11" s="31"/>
       <c r="K11" s="30"/>
       <c r="O11" s="14"/>
-      <c r="P11" s="65" t="s">
+      <c r="P11" s="68" t="s">
         <v>210</v>
       </c>
-      <c r="Q11" s="65"/>
+      <c r="Q11" s="68"/>
       <c r="R11" s="31"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
@@ -2789,7 +2858,7 @@
         <v>251</v>
       </c>
       <c r="M13" s="14">
-        <f>COUNTIF('College-Details'!U:U,L13)</f>
+        <f>COUNTIF('College-Details'!V:V,L13)</f>
         <v>0</v>
       </c>
       <c r="O13" s="22">
@@ -2827,7 +2896,7 @@
         <v>253</v>
       </c>
       <c r="M14" s="14">
-        <f>COUNTIF('College-Details'!U:U,L14)</f>
+        <f>COUNTIF('College-Details'!V:V,L14)</f>
         <v>0</v>
       </c>
       <c r="O14" s="22">
@@ -2865,7 +2934,7 @@
         <v>255</v>
       </c>
       <c r="M15" s="14">
-        <f>COUNTIF('College-Details'!U:U,L15)</f>
+        <f>COUNTIF('College-Details'!V:V,L15)</f>
         <v>0</v>
       </c>
       <c r="O15" s="22">
@@ -2903,7 +2972,7 @@
         <v>257</v>
       </c>
       <c r="M16" s="14">
-        <f>COUNTIF('College-Details'!U:U,L16)</f>
+        <f>COUNTIF('College-Details'!V:V,L16)</f>
         <v>0</v>
       </c>
       <c r="O16" s="22">
@@ -2941,7 +3010,7 @@
         <v>259</v>
       </c>
       <c r="M17" s="14">
-        <f>COUNTIF('College-Details'!U:U,L17)</f>
+        <f>COUNTIF('College-Details'!V:V,L17)</f>
         <v>0</v>
       </c>
       <c r="O17" s="22">
@@ -2979,7 +3048,7 @@
         <v>261</v>
       </c>
       <c r="M18" s="14">
-        <f>COUNTIF('College-Details'!U:U,L18)</f>
+        <f>COUNTIF('College-Details'!V:V,L18)</f>
         <v>0</v>
       </c>
       <c r="O18" s="22">
@@ -3017,7 +3086,7 @@
         <v>263</v>
       </c>
       <c r="M19" s="14">
-        <f>COUNTIF('College-Details'!U:U,L19)</f>
+        <f>COUNTIF('College-Details'!V:V,L19)</f>
         <v>53</v>
       </c>
       <c r="O19" s="22">
@@ -3048,7 +3117,7 @@
         <v>279</v>
       </c>
       <c r="M20" s="14">
-        <f>COUNTIF('College-Details'!U:U,L20)</f>
+        <f>COUNTIF('College-Details'!V:V,L20)</f>
         <v>0</v>
       </c>
       <c r="O20" s="22">
@@ -3195,7 +3264,7 @@
         <v>5</v>
       </c>
       <c r="M24" s="14">
-        <f>COUNTIF('College-Details'!T:T,L24)</f>
+        <f>COUNTIF('College-Details'!U:U,L24)</f>
         <v>0</v>
       </c>
       <c r="O24" s="22">
@@ -3237,7 +3306,7 @@
         <v>4</v>
       </c>
       <c r="M25" s="14">
-        <f>COUNTIF('College-Details'!T:T,L25)</f>
+        <f>COUNTIF('College-Details'!U:U,L25)</f>
         <v>0</v>
       </c>
       <c r="O25" s="16" t="s">
@@ -3292,7 +3361,7 @@
         <v>3</v>
       </c>
       <c r="M27" s="14">
-        <f>COUNTIF('College-Details'!T:T,L27)</f>
+        <f>COUNTIF('College-Details'!U:U,L27)</f>
         <v>0</v>
       </c>
       <c r="R27" s="31"/>
@@ -3334,7 +3403,7 @@
         <v>2</v>
       </c>
       <c r="M29" s="14">
-        <f>COUNTIF('College-Details'!T:T,L29)</f>
+        <f>COUNTIF('College-Details'!U:U,L29)</f>
         <v>0</v>
       </c>
       <c r="R29" s="31"/>
@@ -3358,7 +3427,7 @@
         <v>1</v>
       </c>
       <c r="M30" s="14">
-        <f>COUNTIF('College-Details'!T:T,L30)</f>
+        <f>COUNTIF('College-Details'!U:U,L30)</f>
         <v>0</v>
       </c>
       <c r="R30" s="31"/>
@@ -3411,11 +3480,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="K8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4291,12 +4360,15 @@
         <v>251</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>23</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>489</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>60</v>
@@ -4338,6 +4410,7 @@
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D20" s="3"/>
       <c r="F20" s="7" t="s">
         <v>61</v>
       </c>
@@ -5120,7 +5193,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -5129,6 +5202,9 @@
       </c>
       <c r="C38" s="1" t="s">
         <v>77</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>490</v>
       </c>
       <c r="F38" s="8">
         <v>8902488077</v>
@@ -5170,6 +5246,9 @@
       <c r="C39" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D39" s="65" t="s">
+        <v>492</v>
+      </c>
       <c r="F39" s="9">
         <v>9163741069</v>
       </c>
@@ -5200,7 +5279,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -5209,6 +5288,9 @@
       </c>
       <c r="C40" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>491</v>
       </c>
       <c r="F40" s="9">
         <v>3324411691</v>
@@ -5382,6 +5464,9 @@
       <c r="C44" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="D44" s="66" t="s">
+        <v>493</v>
+      </c>
       <c r="F44" s="7">
         <v>3324712220</v>
       </c>
@@ -5422,6 +5507,9 @@
       <c r="C45" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="D45" s="3" t="s">
+        <v>494</v>
+      </c>
       <c r="F45" s="7">
         <v>3324131158</v>
       </c>
@@ -7026,6 +7114,9 @@
       <c r="C82" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="D82" s="3" t="s">
+        <v>495</v>
+      </c>
       <c r="F82" s="7" t="s">
         <v>168</v>
       </c>
@@ -7066,6 +7157,9 @@
       <c r="C83" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D83" s="3" t="s">
+        <v>496</v>
+      </c>
       <c r="F83" s="7" t="s">
         <v>170</v>
       </c>
@@ -7106,6 +7200,9 @@
       <c r="C84" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="D84" s="3" t="s">
+        <v>497</v>
+      </c>
       <c r="F84" s="7">
         <v>9606279184</v>
       </c>
@@ -7180,7 +7277,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -7189,6 +7286,9 @@
       </c>
       <c r="C86" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>498</v>
       </c>
       <c r="F86" s="7">
         <v>8017672075</v>
@@ -7230,6 +7330,9 @@
       <c r="C87" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D87" s="3" t="s">
+        <v>499</v>
+      </c>
       <c r="F87" s="7">
         <v>3324492810</v>
       </c>
@@ -7348,7 +7451,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -7357,6 +7460,9 @@
       </c>
       <c r="C90" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>500</v>
       </c>
       <c r="F90" s="7">
         <v>3324961723</v>
@@ -7442,6 +7548,12 @@
       <c r="C92" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="D92" s="67" t="s">
+        <v>501</v>
+      </c>
+      <c r="E92" s="67" t="s">
+        <v>502</v>
+      </c>
       <c r="F92" s="7">
         <v>8902765583</v>
       </c>
@@ -7472,7 +7584,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -7481,6 +7593,9 @@
       </c>
       <c r="C93" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>503</v>
       </c>
       <c r="F93" s="7">
         <v>9331866252</v>
@@ -7512,18 +7627,21 @@
         <v>263</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>185</v>
+        <v>505</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F94" s="7">
-        <v>9903540099</v>
+      <c r="D94" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>506</v>
       </c>
       <c r="O94" s="10">
         <v>1</v>
@@ -8928,19 +9046,30 @@
     <hyperlink ref="D17" r:id="rId71" xr:uid="{4B58FE9C-FCB3-4E9C-864B-84CFD88CF409}"/>
     <hyperlink ref="D18" r:id="rId72" xr:uid="{8D0F79EA-9E76-42A8-B6DE-38DCF086D2BD}"/>
     <hyperlink ref="E18" r:id="rId73" xr:uid="{294A50A6-666F-49B6-B8C5-CC133E5CC526}"/>
+    <hyperlink ref="D19" r:id="rId74" xr:uid="{3411E3DE-249B-43C6-861A-C24AA2D10629}"/>
+    <hyperlink ref="D38" r:id="rId75" xr:uid="{51D43514-0760-4B71-B43C-B4E18F6C03BD}"/>
+    <hyperlink ref="D40" r:id="rId76" xr:uid="{C53F92AF-72F3-42FA-96A3-44E82E52EE23}"/>
+    <hyperlink ref="D44" r:id="rId77" xr:uid="{D96EB2AF-EDA4-447F-85B9-36AE533C9CAB}"/>
+    <hyperlink ref="D45" r:id="rId78" xr:uid="{63E956BC-EB66-4FDE-BA79-2F74BB9DCB55}"/>
+    <hyperlink ref="D82" r:id="rId79" xr:uid="{5F4352DE-F44C-4573-AB0F-C62280AED2C7}"/>
+    <hyperlink ref="D83" r:id="rId80" xr:uid="{C2649A64-240A-4675-8D35-CA592B0D7D2F}"/>
+    <hyperlink ref="D84" r:id="rId81" xr:uid="{7346E54C-CDF3-486C-B28D-387D21A1BCBE}"/>
+    <hyperlink ref="D86" r:id="rId82" xr:uid="{B4F97ACF-EA33-47B5-90D6-7BC872FE370E}"/>
+    <hyperlink ref="D87" r:id="rId83" xr:uid="{86E652CD-E20A-4FFB-AE0F-8142DCB6C066}"/>
+    <hyperlink ref="D90" r:id="rId84" xr:uid="{A0ED5720-7123-4A54-A72C-0783F12FFE50}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId74"/>
-  <legacyDrawing r:id="rId75"/>
+  <pageSetup orientation="portrait" r:id="rId85"/>
+  <legacyDrawing r:id="rId86"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:U179"/>
+  <dimension ref="A1:V179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8953,16 +9082,17 @@
     <col min="6" max="8" width="16" style="40" customWidth="1"/>
     <col min="9" max="10" width="11" style="1" customWidth="1"/>
     <col min="11" max="11" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" style="40" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="1"/>
-    <col min="16" max="16" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="9.109375" style="1"/>
-    <col min="21" max="21" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" style="40" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="1"/>
+    <col min="17" max="17" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="9.109375" style="1"/>
+    <col min="22" max="22" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>1</v>
       </c>
@@ -8997,37 +9127,40 @@
         <v>296</v>
       </c>
       <c r="L1" s="18" t="s">
+        <v>454</v>
+      </c>
+      <c r="M1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="V1" s="20" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>1</v>
       </c>
@@ -9045,10 +9178,8 @@
       <c r="K2" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10">
-        <v>0</v>
-      </c>
+      <c r="L2" s="10"/>
+      <c r="N2" s="10"/>
       <c r="O2" s="10">
         <v>0</v>
       </c>
@@ -9065,14 +9196,17 @@
         <v>0</v>
       </c>
       <c r="T2" s="10">
-        <f>ROUND(S2/5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="U2" s="10">
+        <f>ROUND(T2/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -9088,9 +9222,7 @@
       <c r="K3" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N3" s="10">
-        <v>0</v>
-      </c>
+      <c r="L3" s="10"/>
       <c r="O3" s="10">
         <v>0</v>
       </c>
@@ -9107,14 +9239,17 @@
         <v>0</v>
       </c>
       <c r="T3" s="10">
-        <f t="shared" ref="T3:T35" si="0">ROUND(S3/5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="10">
+        <f t="shared" ref="U3:U35" si="0">ROUND(T3/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -9130,9 +9265,7 @@
       <c r="K4" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N4" s="10">
-        <v>0</v>
-      </c>
+      <c r="L4" s="10"/>
       <c r="O4" s="10">
         <v>0</v>
       </c>
@@ -9149,14 +9282,17 @@
         <v>0</v>
       </c>
       <c r="T4" s="10">
+        <v>0</v>
+      </c>
+      <c r="U4" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U4" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V4" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -9172,9 +9308,7 @@
       <c r="K5" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N5" s="10">
-        <v>0</v>
-      </c>
+      <c r="L5" s="10"/>
       <c r="O5" s="10">
         <v>0</v>
       </c>
@@ -9191,14 +9325,17 @@
         <v>0</v>
       </c>
       <c r="T5" s="10">
+        <v>0</v>
+      </c>
+      <c r="U5" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U5" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="V5" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -9214,9 +9351,7 @@
       <c r="K6" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N6" s="10">
-        <v>0</v>
-      </c>
+      <c r="L6" s="10"/>
       <c r="O6" s="10">
         <v>0</v>
       </c>
@@ -9233,14 +9368,17 @@
         <v>0</v>
       </c>
       <c r="T6" s="10">
+        <v>0</v>
+      </c>
+      <c r="U6" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U6" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="V6" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -9256,9 +9394,7 @@
       <c r="K7" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N7" s="10">
-        <v>0</v>
-      </c>
+      <c r="L7" s="10"/>
       <c r="O7" s="10">
         <v>0</v>
       </c>
@@ -9275,14 +9411,17 @@
         <v>0</v>
       </c>
       <c r="T7" s="10">
+        <v>0</v>
+      </c>
+      <c r="U7" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U7" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V7" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -9295,12 +9434,10 @@
       <c r="K8" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="L8" s="40" t="s">
+      <c r="L8" s="10"/>
+      <c r="M8" s="40" t="s">
         <v>316</v>
       </c>
-      <c r="N8" s="10">
-        <v>0</v>
-      </c>
       <c r="O8" s="10">
         <v>0</v>
       </c>
@@ -9317,14 +9454,17 @@
         <v>0</v>
       </c>
       <c r="T8" s="10">
+        <v>0</v>
+      </c>
+      <c r="U8" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U8" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V8" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -9337,9 +9477,7 @@
       <c r="K9" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N9" s="10">
-        <v>0</v>
-      </c>
+      <c r="L9" s="10"/>
       <c r="O9" s="10">
         <v>0</v>
       </c>
@@ -9356,14 +9494,17 @@
         <v>0</v>
       </c>
       <c r="T9" s="10">
+        <v>0</v>
+      </c>
+      <c r="U9" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U9" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V9" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -9376,9 +9517,7 @@
       <c r="K10" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N10" s="10">
-        <v>0</v>
-      </c>
+      <c r="L10" s="10"/>
       <c r="O10" s="10">
         <v>0</v>
       </c>
@@ -9395,14 +9534,17 @@
         <v>0</v>
       </c>
       <c r="T10" s="10">
+        <v>0</v>
+      </c>
+      <c r="U10" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U10" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V10" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -9416,9 +9558,7 @@
       <c r="K11" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N11" s="10">
-        <v>0</v>
-      </c>
+      <c r="L11" s="10"/>
       <c r="O11" s="10">
         <v>0</v>
       </c>
@@ -9435,14 +9575,17 @@
         <v>0</v>
       </c>
       <c r="T11" s="10">
+        <v>0</v>
+      </c>
+      <c r="U11" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U11" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V11" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -9455,9 +9598,7 @@
       <c r="K12" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N12" s="10">
-        <v>0</v>
-      </c>
+      <c r="L12" s="10"/>
       <c r="O12" s="10">
         <v>0</v>
       </c>
@@ -9474,14 +9615,17 @@
         <v>0</v>
       </c>
       <c r="T12" s="10">
+        <v>0</v>
+      </c>
+      <c r="U12" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U12" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V12" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -9494,9 +9638,7 @@
       <c r="K13" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N13" s="10">
-        <v>0</v>
-      </c>
+      <c r="L13" s="10"/>
       <c r="O13" s="10">
         <v>0</v>
       </c>
@@ -9513,14 +9655,17 @@
         <v>0</v>
       </c>
       <c r="T13" s="10">
+        <v>0</v>
+      </c>
+      <c r="U13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U13" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V13" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -9533,9 +9678,7 @@
       <c r="K14" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N14" s="10">
-        <v>0</v>
-      </c>
+      <c r="L14" s="10"/>
       <c r="O14" s="10">
         <v>0</v>
       </c>
@@ -9552,14 +9695,17 @@
         <v>0</v>
       </c>
       <c r="T14" s="10">
+        <v>0</v>
+      </c>
+      <c r="U14" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U14" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V14" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -9572,9 +9718,7 @@
       <c r="K15" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N15" s="10">
-        <v>0</v>
-      </c>
+      <c r="L15" s="10"/>
       <c r="O15" s="10">
         <v>0</v>
       </c>
@@ -9591,14 +9735,17 @@
         <v>0</v>
       </c>
       <c r="T15" s="10">
+        <v>0</v>
+      </c>
+      <c r="U15" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U15" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V15" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -9611,9 +9758,7 @@
       <c r="K16" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N16" s="10">
-        <v>0</v>
-      </c>
+      <c r="L16" s="10"/>
       <c r="O16" s="10">
         <v>0</v>
       </c>
@@ -9630,14 +9775,17 @@
         <v>0</v>
       </c>
       <c r="T16" s="10">
+        <v>0</v>
+      </c>
+      <c r="U16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U16" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V16" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -9650,9 +9798,7 @@
       <c r="K17" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N17" s="10">
-        <v>0</v>
-      </c>
+      <c r="L17" s="10"/>
       <c r="O17" s="10">
         <v>0</v>
       </c>
@@ -9669,14 +9815,17 @@
         <v>0</v>
       </c>
       <c r="T17" s="10">
+        <v>0</v>
+      </c>
+      <c r="U17" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U17" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V17" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -9689,9 +9838,7 @@
       <c r="K18" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N18" s="10">
-        <v>0</v>
-      </c>
+      <c r="L18" s="10"/>
       <c r="O18" s="10">
         <v>0</v>
       </c>
@@ -9708,14 +9855,17 @@
         <v>0</v>
       </c>
       <c r="T18" s="10">
+        <v>0</v>
+      </c>
+      <c r="U18" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U18" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V18" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -9728,9 +9878,7 @@
       <c r="K19" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N19" s="10">
-        <v>0</v>
-      </c>
+      <c r="L19" s="10"/>
       <c r="O19" s="10">
         <v>0</v>
       </c>
@@ -9747,14 +9895,17 @@
         <v>0</v>
       </c>
       <c r="T19" s="10">
+        <v>0</v>
+      </c>
+      <c r="U19" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U19" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V19" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -9768,9 +9919,7 @@
       <c r="K20" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N20" s="10">
-        <v>0</v>
-      </c>
+      <c r="L20" s="10"/>
       <c r="O20" s="10">
         <v>0</v>
       </c>
@@ -9787,14 +9936,17 @@
         <v>0</v>
       </c>
       <c r="T20" s="10">
+        <v>0</v>
+      </c>
+      <c r="U20" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U20" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V20" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -9808,9 +9960,7 @@
       <c r="K21" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N21" s="10">
-        <v>0</v>
-      </c>
+      <c r="L21" s="10"/>
       <c r="O21" s="10">
         <v>0</v>
       </c>
@@ -9827,14 +9977,17 @@
         <v>0</v>
       </c>
       <c r="T21" s="10">
+        <v>0</v>
+      </c>
+      <c r="U21" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U21" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V21" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -9847,9 +10000,7 @@
       <c r="K22" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N22" s="10">
-        <v>0</v>
-      </c>
+      <c r="L22" s="10"/>
       <c r="O22" s="10">
         <v>0</v>
       </c>
@@ -9866,14 +10017,17 @@
         <v>0</v>
       </c>
       <c r="T22" s="10">
+        <v>0</v>
+      </c>
+      <c r="U22" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U22" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V22" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -9887,9 +10041,7 @@
       <c r="K23" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N23" s="10">
-        <v>0</v>
-      </c>
+      <c r="L23" s="10"/>
       <c r="O23" s="10">
         <v>0</v>
       </c>
@@ -9906,14 +10058,17 @@
         <v>0</v>
       </c>
       <c r="T23" s="10">
+        <v>0</v>
+      </c>
+      <c r="U23" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U23" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V23" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -9927,9 +10082,7 @@
       <c r="K24" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N24" s="10">
-        <v>0</v>
-      </c>
+      <c r="L24" s="10"/>
       <c r="O24" s="10">
         <v>0</v>
       </c>
@@ -9946,14 +10099,17 @@
         <v>0</v>
       </c>
       <c r="T24" s="10">
+        <v>0</v>
+      </c>
+      <c r="U24" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U24" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V24" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -9967,9 +10123,7 @@
       <c r="K25" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N25" s="10">
-        <v>0</v>
-      </c>
+      <c r="L25" s="10"/>
       <c r="O25" s="10">
         <v>0</v>
       </c>
@@ -9986,14 +10140,17 @@
         <v>0</v>
       </c>
       <c r="T25" s="10">
+        <v>0</v>
+      </c>
+      <c r="U25" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U25" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V25" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -10007,9 +10164,7 @@
       <c r="K26" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N26" s="10">
-        <v>0</v>
-      </c>
+      <c r="L26" s="10"/>
       <c r="O26" s="10">
         <v>0</v>
       </c>
@@ -10026,14 +10181,17 @@
         <v>0</v>
       </c>
       <c r="T26" s="10">
+        <v>0</v>
+      </c>
+      <c r="U26" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U26" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V26" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -10046,9 +10204,7 @@
       <c r="K27" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N27" s="10">
-        <v>0</v>
-      </c>
+      <c r="L27" s="10"/>
       <c r="O27" s="10">
         <v>0</v>
       </c>
@@ -10065,14 +10221,17 @@
         <v>0</v>
       </c>
       <c r="T27" s="10">
+        <v>0</v>
+      </c>
+      <c r="U27" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U27" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V27" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -10085,9 +10244,7 @@
       <c r="K28" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N28" s="10">
-        <v>0</v>
-      </c>
+      <c r="L28" s="10"/>
       <c r="O28" s="10">
         <v>0</v>
       </c>
@@ -10104,14 +10261,17 @@
         <v>0</v>
       </c>
       <c r="T28" s="10">
+        <v>0</v>
+      </c>
+      <c r="U28" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U28" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V28" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -10125,9 +10285,7 @@
       <c r="K29" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N29" s="10">
-        <v>0</v>
-      </c>
+      <c r="L29" s="10"/>
       <c r="O29" s="10">
         <v>0</v>
       </c>
@@ -10144,14 +10302,17 @@
         <v>0</v>
       </c>
       <c r="T29" s="10">
+        <v>0</v>
+      </c>
+      <c r="U29" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U29" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V29" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -10165,9 +10326,7 @@
       <c r="K30" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N30" s="10">
-        <v>0</v>
-      </c>
+      <c r="L30" s="10"/>
       <c r="O30" s="10">
         <v>0</v>
       </c>
@@ -10184,14 +10343,17 @@
         <v>0</v>
       </c>
       <c r="T30" s="10">
+        <v>0</v>
+      </c>
+      <c r="U30" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U30" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V30" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -10205,9 +10367,7 @@
       <c r="K31" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N31" s="10">
-        <v>0</v>
-      </c>
+      <c r="L31" s="10"/>
       <c r="O31" s="10">
         <v>0</v>
       </c>
@@ -10224,14 +10384,17 @@
         <v>0</v>
       </c>
       <c r="T31" s="10">
+        <v>0</v>
+      </c>
+      <c r="U31" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U31" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V31" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -10244,9 +10407,7 @@
       <c r="K32" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N32" s="10">
-        <v>0</v>
-      </c>
+      <c r="L32" s="10"/>
       <c r="O32" s="10">
         <v>0</v>
       </c>
@@ -10263,14 +10424,17 @@
         <v>0</v>
       </c>
       <c r="T32" s="10">
+        <v>0</v>
+      </c>
+      <c r="U32" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U32" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V32" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -10283,9 +10447,7 @@
       <c r="K33" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N33" s="10">
-        <v>0</v>
-      </c>
+      <c r="L33" s="10"/>
       <c r="O33" s="10">
         <v>0</v>
       </c>
@@ -10302,14 +10464,17 @@
         <v>0</v>
       </c>
       <c r="T33" s="10">
+        <v>0</v>
+      </c>
+      <c r="U33" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U33" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V33" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -10322,9 +10487,7 @@
       <c r="K34" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N34" s="10">
-        <v>0</v>
-      </c>
+      <c r="L34" s="10"/>
       <c r="O34" s="10">
         <v>0</v>
       </c>
@@ -10341,14 +10504,17 @@
         <v>0</v>
       </c>
       <c r="T34" s="10">
+        <v>0</v>
+      </c>
+      <c r="U34" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U34" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V34" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -10361,9 +10527,7 @@
       <c r="K35" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N35" s="10">
-        <v>0</v>
-      </c>
+      <c r="L35" s="10"/>
       <c r="O35" s="10">
         <v>0</v>
       </c>
@@ -10380,14 +10544,17 @@
         <v>0</v>
       </c>
       <c r="T35" s="10">
+        <v>0</v>
+      </c>
+      <c r="U35" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U35" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V35" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -10406,9 +10573,7 @@
       <c r="K36" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N36" s="10">
-        <v>0</v>
-      </c>
+      <c r="L36" s="10"/>
       <c r="O36" s="10">
         <v>0</v>
       </c>
@@ -10425,14 +10590,17 @@
         <v>0</v>
       </c>
       <c r="T36" s="10">
-        <f t="shared" ref="T36:T54" si="1">ROUND(S36/5,0)</f>
-        <v>0</v>
-      </c>
-      <c r="U36" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="U36" s="10">
+        <f t="shared" ref="U36:U54" si="1">ROUND(T36/5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V36" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -10451,9 +10619,7 @@
       <c r="K37" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N37" s="10">
-        <v>0</v>
-      </c>
+      <c r="L37" s="10"/>
       <c r="O37" s="10">
         <v>0</v>
       </c>
@@ -10470,14 +10636,17 @@
         <v>0</v>
       </c>
       <c r="T37" s="10">
+        <v>0</v>
+      </c>
+      <c r="U37" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U37" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V37" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -10493,9 +10662,7 @@
       <c r="K38" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N38" s="10">
-        <v>0</v>
-      </c>
+      <c r="L38" s="10"/>
       <c r="O38" s="10">
         <v>0</v>
       </c>
@@ -10512,14 +10679,17 @@
         <v>0</v>
       </c>
       <c r="T38" s="10">
+        <v>0</v>
+      </c>
+      <c r="U38" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U38" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V38" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -10535,9 +10705,7 @@
       <c r="K39" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N39" s="10">
-        <v>0</v>
-      </c>
+      <c r="L39" s="10"/>
       <c r="O39" s="10">
         <v>0</v>
       </c>
@@ -10554,14 +10722,17 @@
         <v>0</v>
       </c>
       <c r="T39" s="10">
+        <v>0</v>
+      </c>
+      <c r="U39" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U39" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V39" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -10577,9 +10748,7 @@
       <c r="K40" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N40" s="10">
-        <v>0</v>
-      </c>
+      <c r="L40" s="10"/>
       <c r="O40" s="10">
         <v>0</v>
       </c>
@@ -10596,14 +10765,17 @@
         <v>0</v>
       </c>
       <c r="T40" s="10">
+        <v>0</v>
+      </c>
+      <c r="U40" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U40" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V40" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -10619,9 +10791,7 @@
       <c r="K41" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N41" s="10">
-        <v>0</v>
-      </c>
+      <c r="L41" s="10"/>
       <c r="O41" s="10">
         <v>0</v>
       </c>
@@ -10638,14 +10808,17 @@
         <v>0</v>
       </c>
       <c r="T41" s="10">
+        <v>0</v>
+      </c>
+      <c r="U41" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U41" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V41" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -10661,9 +10834,7 @@
       <c r="K42" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N42" s="10">
-        <v>0</v>
-      </c>
+      <c r="L42" s="10"/>
       <c r="O42" s="10">
         <v>0</v>
       </c>
@@ -10680,14 +10851,17 @@
         <v>0</v>
       </c>
       <c r="T42" s="10">
+        <v>0</v>
+      </c>
+      <c r="U42" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U42" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="V42" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -10706,9 +10880,7 @@
       <c r="K43" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N43" s="10">
-        <v>0</v>
-      </c>
+      <c r="L43" s="10"/>
       <c r="O43" s="10">
         <v>0</v>
       </c>
@@ -10725,14 +10897,17 @@
         <v>0</v>
       </c>
       <c r="T43" s="10">
+        <v>0</v>
+      </c>
+      <c r="U43" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U43" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V43" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -10748,9 +10923,7 @@
       <c r="K44" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N44" s="10">
-        <v>0</v>
-      </c>
+      <c r="L44" s="10"/>
       <c r="O44" s="10">
         <v>0</v>
       </c>
@@ -10767,14 +10940,17 @@
         <v>0</v>
       </c>
       <c r="T44" s="10">
+        <v>0</v>
+      </c>
+      <c r="U44" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U44" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V44" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -10790,9 +10966,7 @@
       <c r="K45" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N45" s="10">
-        <v>0</v>
-      </c>
+      <c r="L45" s="10"/>
       <c r="O45" s="10">
         <v>0</v>
       </c>
@@ -10809,14 +10983,17 @@
         <v>0</v>
       </c>
       <c r="T45" s="10">
+        <v>0</v>
+      </c>
+      <c r="U45" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U45" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V45" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -10832,9 +11009,7 @@
       <c r="K46" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N46" s="10">
-        <v>0</v>
-      </c>
+      <c r="L46" s="10"/>
       <c r="O46" s="10">
         <v>0</v>
       </c>
@@ -10851,14 +11026,17 @@
         <v>0</v>
       </c>
       <c r="T46" s="10">
+        <v>0</v>
+      </c>
+      <c r="U46" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U46" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="V46" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -10874,9 +11052,7 @@
       <c r="K47" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N47" s="10">
-        <v>0</v>
-      </c>
+      <c r="L47" s="10"/>
       <c r="O47" s="10">
         <v>0</v>
       </c>
@@ -10893,14 +11069,17 @@
         <v>0</v>
       </c>
       <c r="T47" s="10">
+        <v>0</v>
+      </c>
+      <c r="U47" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U47" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V47" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -10916,9 +11095,7 @@
       <c r="K48" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N48" s="10">
-        <v>0</v>
-      </c>
+      <c r="L48" s="10"/>
       <c r="O48" s="10">
         <v>0</v>
       </c>
@@ -10935,14 +11112,17 @@
         <v>0</v>
       </c>
       <c r="T48" s="10">
+        <v>0</v>
+      </c>
+      <c r="U48" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U48" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="V48" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -10961,9 +11141,7 @@
       <c r="K49" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N49" s="10">
-        <v>0</v>
-      </c>
+      <c r="L49" s="10"/>
       <c r="O49" s="10">
         <v>0</v>
       </c>
@@ -10980,14 +11158,17 @@
         <v>0</v>
       </c>
       <c r="T49" s="10">
+        <v>0</v>
+      </c>
+      <c r="U49" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U49" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V49" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -11003,9 +11184,7 @@
       <c r="K50" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N50" s="10">
-        <v>0</v>
-      </c>
+      <c r="L50" s="10"/>
       <c r="O50" s="10">
         <v>0</v>
       </c>
@@ -11022,14 +11201,17 @@
         <v>0</v>
       </c>
       <c r="T50" s="10">
+        <v>0</v>
+      </c>
+      <c r="U50" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U50" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="V50" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -11045,9 +11227,7 @@
       <c r="K51" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N51" s="10">
-        <v>0</v>
-      </c>
+      <c r="L51" s="10"/>
       <c r="O51" s="10">
         <v>0</v>
       </c>
@@ -11064,14 +11244,17 @@
         <v>0</v>
       </c>
       <c r="T51" s="10">
+        <v>0</v>
+      </c>
+      <c r="U51" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U51" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V51" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -11087,9 +11270,7 @@
       <c r="K52" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N52" s="10">
-        <v>0</v>
-      </c>
+      <c r="L52" s="10"/>
       <c r="O52" s="10">
         <v>0</v>
       </c>
@@ -11106,14 +11287,17 @@
         <v>0</v>
       </c>
       <c r="T52" s="10">
+        <v>0</v>
+      </c>
+      <c r="U52" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U52" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="V52" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -11129,9 +11313,7 @@
       <c r="K53" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N53" s="10">
-        <v>0</v>
-      </c>
+      <c r="L53" s="10"/>
       <c r="O53" s="10">
         <v>0</v>
       </c>
@@ -11148,14 +11330,17 @@
         <v>0</v>
       </c>
       <c r="T53" s="10">
+        <v>0</v>
+      </c>
+      <c r="U53" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U53" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V53" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -11171,9 +11356,7 @@
       <c r="K54" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="N54" s="10">
-        <v>0</v>
-      </c>
+      <c r="L54" s="10"/>
       <c r="O54" s="10">
         <v>0</v>
       </c>
@@ -11190,1144 +11373,1147 @@
         <v>0</v>
       </c>
       <c r="T54" s="10">
+        <v>0</v>
+      </c>
+      <c r="U54" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U54" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N55" s="10"/>
+      <c r="V54" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
       <c r="Q55" s="10"/>
       <c r="R55" s="10"/>
       <c r="S55" s="10"/>
       <c r="T55" s="10"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N56" s="10"/>
+      <c r="U55" s="10"/>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
       <c r="Q56" s="10"/>
       <c r="R56" s="10"/>
       <c r="S56" s="10"/>
       <c r="T56" s="10"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N57" s="10"/>
+      <c r="U56" s="10"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
       <c r="Q57" s="10"/>
       <c r="R57" s="10"/>
       <c r="S57" s="10"/>
       <c r="T57" s="10"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N58" s="10"/>
+      <c r="U57" s="10"/>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O58" s="10"/>
       <c r="P58" s="10"/>
       <c r="Q58" s="10"/>
       <c r="R58" s="10"/>
       <c r="S58" s="10"/>
       <c r="T58" s="10"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N59" s="10"/>
+      <c r="U58" s="10"/>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O59" s="10"/>
       <c r="P59" s="10"/>
       <c r="Q59" s="10"/>
       <c r="R59" s="10"/>
       <c r="S59" s="10"/>
       <c r="T59" s="10"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N60" s="10"/>
+      <c r="U59" s="10"/>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O60" s="10"/>
       <c r="P60" s="10"/>
       <c r="Q60" s="10"/>
       <c r="R60" s="10"/>
       <c r="S60" s="10"/>
       <c r="T60" s="10"/>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N61" s="10"/>
+      <c r="U60" s="10"/>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O61" s="10"/>
       <c r="P61" s="10"/>
       <c r="Q61" s="10"/>
       <c r="R61" s="10"/>
       <c r="S61" s="10"/>
       <c r="T61" s="10"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N62" s="10"/>
+      <c r="U61" s="10"/>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O62" s="10"/>
       <c r="P62" s="10"/>
       <c r="Q62" s="10"/>
       <c r="R62" s="10"/>
       <c r="S62" s="10"/>
       <c r="T62" s="10"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N63" s="10"/>
+      <c r="U62" s="10"/>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O63" s="10"/>
       <c r="P63" s="10"/>
       <c r="Q63" s="10"/>
       <c r="R63" s="10"/>
       <c r="S63" s="10"/>
       <c r="T63" s="10"/>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="N64" s="10"/>
+      <c r="U63" s="10"/>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="O64" s="10"/>
       <c r="P64" s="10"/>
       <c r="Q64" s="10"/>
       <c r="R64" s="10"/>
       <c r="S64" s="10"/>
       <c r="T64" s="10"/>
-    </row>
-    <row r="65" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N65" s="10"/>
+      <c r="U64" s="10"/>
+    </row>
+    <row r="65" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O65" s="10"/>
       <c r="P65" s="10"/>
       <c r="Q65" s="10"/>
       <c r="R65" s="10"/>
       <c r="S65" s="10"/>
       <c r="T65" s="10"/>
-    </row>
-    <row r="66" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N66" s="10"/>
+      <c r="U65" s="10"/>
+    </row>
+    <row r="66" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O66" s="10"/>
       <c r="P66" s="10"/>
       <c r="Q66" s="10"/>
       <c r="R66" s="10"/>
       <c r="S66" s="10"/>
       <c r="T66" s="10"/>
-    </row>
-    <row r="67" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N67" s="10"/>
+      <c r="U66" s="10"/>
+    </row>
+    <row r="67" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O67" s="10"/>
       <c r="P67" s="10"/>
       <c r="Q67" s="10"/>
       <c r="R67" s="10"/>
       <c r="S67" s="10"/>
       <c r="T67" s="10"/>
-    </row>
-    <row r="68" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N68" s="10"/>
+      <c r="U67" s="10"/>
+    </row>
+    <row r="68" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O68" s="10"/>
       <c r="P68" s="10"/>
       <c r="Q68" s="10"/>
       <c r="R68" s="10"/>
       <c r="S68" s="10"/>
       <c r="T68" s="10"/>
-    </row>
-    <row r="69" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N69" s="10"/>
+      <c r="U68" s="10"/>
+    </row>
+    <row r="69" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O69" s="10"/>
       <c r="P69" s="10"/>
       <c r="Q69" s="10"/>
       <c r="R69" s="10"/>
       <c r="S69" s="10"/>
       <c r="T69" s="10"/>
-    </row>
-    <row r="70" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N70" s="10"/>
+      <c r="U69" s="10"/>
+    </row>
+    <row r="70" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O70" s="10"/>
       <c r="P70" s="10"/>
       <c r="Q70" s="10"/>
       <c r="R70" s="10"/>
       <c r="S70" s="10"/>
       <c r="T70" s="10"/>
-    </row>
-    <row r="71" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N71" s="10"/>
+      <c r="U70" s="10"/>
+    </row>
+    <row r="71" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O71" s="10"/>
       <c r="P71" s="10"/>
       <c r="Q71" s="10"/>
       <c r="R71" s="10"/>
       <c r="S71" s="10"/>
       <c r="T71" s="10"/>
-    </row>
-    <row r="72" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N72" s="10"/>
+      <c r="U71" s="10"/>
+    </row>
+    <row r="72" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O72" s="10"/>
       <c r="P72" s="10"/>
       <c r="Q72" s="10"/>
       <c r="R72" s="10"/>
       <c r="S72" s="10"/>
       <c r="T72" s="10"/>
-    </row>
-    <row r="73" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N73" s="10"/>
+      <c r="U72" s="10"/>
+    </row>
+    <row r="73" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O73" s="10"/>
       <c r="P73" s="10"/>
       <c r="Q73" s="10"/>
       <c r="R73" s="10"/>
       <c r="S73" s="10"/>
       <c r="T73" s="10"/>
-    </row>
-    <row r="74" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N74" s="10"/>
+      <c r="U73" s="10"/>
+    </row>
+    <row r="74" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O74" s="10"/>
       <c r="P74" s="10"/>
       <c r="Q74" s="10"/>
       <c r="R74" s="10"/>
       <c r="S74" s="10"/>
       <c r="T74" s="10"/>
-    </row>
-    <row r="75" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N75" s="10"/>
+      <c r="U74" s="10"/>
+    </row>
+    <row r="75" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O75" s="10"/>
       <c r="P75" s="10"/>
       <c r="Q75" s="10"/>
       <c r="R75" s="10"/>
       <c r="S75" s="10"/>
       <c r="T75" s="10"/>
-    </row>
-    <row r="76" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N76" s="10"/>
+      <c r="U75" s="10"/>
+    </row>
+    <row r="76" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O76" s="10"/>
       <c r="P76" s="10"/>
       <c r="Q76" s="10"/>
       <c r="R76" s="10"/>
       <c r="S76" s="10"/>
       <c r="T76" s="10"/>
-    </row>
-    <row r="77" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N77" s="10"/>
+      <c r="U76" s="10"/>
+    </row>
+    <row r="77" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O77" s="10"/>
       <c r="P77" s="10"/>
       <c r="Q77" s="10"/>
       <c r="R77" s="10"/>
       <c r="S77" s="10"/>
       <c r="T77" s="10"/>
-    </row>
-    <row r="78" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N78" s="10"/>
+      <c r="U77" s="10"/>
+    </row>
+    <row r="78" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O78" s="10"/>
       <c r="P78" s="10"/>
       <c r="Q78" s="10"/>
       <c r="R78" s="10"/>
       <c r="S78" s="10"/>
       <c r="T78" s="10"/>
-    </row>
-    <row r="79" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N79" s="10"/>
+      <c r="U78" s="10"/>
+    </row>
+    <row r="79" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O79" s="10"/>
       <c r="P79" s="10"/>
       <c r="Q79" s="10"/>
       <c r="R79" s="10"/>
       <c r="S79" s="10"/>
       <c r="T79" s="10"/>
-    </row>
-    <row r="80" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N80" s="10"/>
+      <c r="U79" s="10"/>
+    </row>
+    <row r="80" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O80" s="10"/>
       <c r="P80" s="10"/>
       <c r="Q80" s="10"/>
       <c r="R80" s="10"/>
       <c r="S80" s="10"/>
       <c r="T80" s="10"/>
-    </row>
-    <row r="81" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N81" s="10"/>
+      <c r="U80" s="10"/>
+    </row>
+    <row r="81" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O81" s="10"/>
       <c r="P81" s="10"/>
       <c r="Q81" s="10"/>
       <c r="R81" s="10"/>
       <c r="S81" s="10"/>
       <c r="T81" s="10"/>
-    </row>
-    <row r="82" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N82" s="10"/>
+      <c r="U81" s="10"/>
+    </row>
+    <row r="82" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O82" s="10"/>
       <c r="P82" s="10"/>
       <c r="Q82" s="10"/>
       <c r="R82" s="10"/>
       <c r="S82" s="10"/>
       <c r="T82" s="10"/>
-    </row>
-    <row r="83" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N83" s="10"/>
+      <c r="U82" s="10"/>
+    </row>
+    <row r="83" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O83" s="10"/>
       <c r="P83" s="10"/>
       <c r="Q83" s="10"/>
       <c r="R83" s="10"/>
       <c r="S83" s="10"/>
       <c r="T83" s="10"/>
-    </row>
-    <row r="84" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N84" s="10"/>
+      <c r="U83" s="10"/>
+    </row>
+    <row r="84" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O84" s="10"/>
       <c r="P84" s="10"/>
       <c r="Q84" s="10"/>
       <c r="R84" s="10"/>
       <c r="S84" s="10"/>
       <c r="T84" s="10"/>
-    </row>
-    <row r="85" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N85" s="10"/>
+      <c r="U84" s="10"/>
+    </row>
+    <row r="85" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O85" s="10"/>
       <c r="P85" s="10"/>
       <c r="Q85" s="10"/>
       <c r="R85" s="10"/>
       <c r="S85" s="10"/>
       <c r="T85" s="10"/>
-    </row>
-    <row r="86" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N86" s="10"/>
+      <c r="U85" s="10"/>
+    </row>
+    <row r="86" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O86" s="10"/>
       <c r="P86" s="10"/>
       <c r="Q86" s="10"/>
       <c r="R86" s="10"/>
       <c r="S86" s="10"/>
       <c r="T86" s="10"/>
-    </row>
-    <row r="87" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N87" s="10"/>
+      <c r="U86" s="10"/>
+    </row>
+    <row r="87" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O87" s="10"/>
       <c r="P87" s="10"/>
       <c r="Q87" s="10"/>
       <c r="R87" s="10"/>
       <c r="S87" s="10"/>
       <c r="T87" s="10"/>
-    </row>
-    <row r="88" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N88" s="10"/>
+      <c r="U87" s="10"/>
+    </row>
+    <row r="88" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O88" s="10"/>
       <c r="P88" s="10"/>
       <c r="Q88" s="10"/>
       <c r="R88" s="10"/>
       <c r="S88" s="10"/>
       <c r="T88" s="10"/>
-    </row>
-    <row r="89" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N89" s="10"/>
+      <c r="U88" s="10"/>
+    </row>
+    <row r="89" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O89" s="10"/>
       <c r="P89" s="10"/>
       <c r="Q89" s="10"/>
       <c r="R89" s="10"/>
       <c r="S89" s="10"/>
       <c r="T89" s="10"/>
-    </row>
-    <row r="90" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N90" s="10"/>
+      <c r="U89" s="10"/>
+    </row>
+    <row r="90" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O90" s="10"/>
       <c r="P90" s="10"/>
       <c r="Q90" s="10"/>
       <c r="R90" s="10"/>
       <c r="S90" s="10"/>
       <c r="T90" s="10"/>
-    </row>
-    <row r="91" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N91" s="10"/>
+      <c r="U90" s="10"/>
+    </row>
+    <row r="91" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O91" s="10"/>
       <c r="P91" s="10"/>
       <c r="Q91" s="10"/>
       <c r="R91" s="10"/>
       <c r="S91" s="10"/>
       <c r="T91" s="10"/>
-    </row>
-    <row r="92" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N92" s="10"/>
+      <c r="U91" s="10"/>
+    </row>
+    <row r="92" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O92" s="10"/>
       <c r="P92" s="10"/>
       <c r="Q92" s="10"/>
       <c r="R92" s="10"/>
       <c r="S92" s="10"/>
       <c r="T92" s="10"/>
-    </row>
-    <row r="93" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N93" s="10"/>
+      <c r="U92" s="10"/>
+    </row>
+    <row r="93" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O93" s="10"/>
       <c r="P93" s="10"/>
       <c r="Q93" s="10"/>
       <c r="R93" s="10"/>
       <c r="S93" s="10"/>
       <c r="T93" s="10"/>
-    </row>
-    <row r="94" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N94" s="10"/>
+      <c r="U93" s="10"/>
+    </row>
+    <row r="94" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O94" s="10"/>
       <c r="P94" s="10"/>
       <c r="Q94" s="10"/>
       <c r="R94" s="10"/>
       <c r="S94" s="10"/>
       <c r="T94" s="10"/>
-    </row>
-    <row r="95" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N95" s="10"/>
+      <c r="U94" s="10"/>
+    </row>
+    <row r="95" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O95" s="10"/>
       <c r="P95" s="10"/>
       <c r="Q95" s="10"/>
       <c r="R95" s="10"/>
       <c r="S95" s="10"/>
       <c r="T95" s="10"/>
-    </row>
-    <row r="96" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N96" s="10"/>
+      <c r="U95" s="10"/>
+    </row>
+    <row r="96" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O96" s="10"/>
       <c r="P96" s="10"/>
       <c r="Q96" s="10"/>
       <c r="R96" s="10"/>
       <c r="S96" s="10"/>
       <c r="T96" s="10"/>
-    </row>
-    <row r="97" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N97" s="10"/>
+      <c r="U96" s="10"/>
+    </row>
+    <row r="97" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O97" s="10"/>
       <c r="P97" s="10"/>
       <c r="Q97" s="10"/>
       <c r="R97" s="10"/>
       <c r="S97" s="10"/>
       <c r="T97" s="10"/>
-    </row>
-    <row r="98" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N98" s="10"/>
+      <c r="U97" s="10"/>
+    </row>
+    <row r="98" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O98" s="10"/>
       <c r="P98" s="10"/>
       <c r="Q98" s="10"/>
       <c r="R98" s="10"/>
       <c r="S98" s="10"/>
       <c r="T98" s="10"/>
-    </row>
-    <row r="99" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N99" s="10"/>
+      <c r="U98" s="10"/>
+    </row>
+    <row r="99" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O99" s="10"/>
       <c r="P99" s="10"/>
       <c r="Q99" s="10"/>
       <c r="R99" s="10"/>
       <c r="S99" s="10"/>
       <c r="T99" s="10"/>
-    </row>
-    <row r="100" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N100" s="10"/>
+      <c r="U99" s="10"/>
+    </row>
+    <row r="100" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O100" s="10"/>
       <c r="P100" s="10"/>
       <c r="Q100" s="10"/>
       <c r="R100" s="10"/>
       <c r="S100" s="10"/>
       <c r="T100" s="10"/>
-    </row>
-    <row r="101" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N101" s="10"/>
+      <c r="U100" s="10"/>
+    </row>
+    <row r="101" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O101" s="10"/>
       <c r="P101" s="10"/>
       <c r="Q101" s="10"/>
       <c r="R101" s="10"/>
       <c r="S101" s="10"/>
       <c r="T101" s="10"/>
-    </row>
-    <row r="102" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N102" s="10"/>
+      <c r="U101" s="10"/>
+    </row>
+    <row r="102" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O102" s="10"/>
       <c r="P102" s="10"/>
       <c r="Q102" s="10"/>
       <c r="R102" s="10"/>
       <c r="S102" s="10"/>
       <c r="T102" s="10"/>
-    </row>
-    <row r="103" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N103" s="10"/>
+      <c r="U102" s="10"/>
+    </row>
+    <row r="103" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O103" s="10"/>
       <c r="P103" s="10"/>
       <c r="Q103" s="10"/>
       <c r="R103" s="10"/>
       <c r="S103" s="10"/>
       <c r="T103" s="10"/>
-    </row>
-    <row r="104" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N104" s="10"/>
+      <c r="U103" s="10"/>
+    </row>
+    <row r="104" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O104" s="10"/>
       <c r="P104" s="10"/>
       <c r="Q104" s="10"/>
       <c r="R104" s="10"/>
       <c r="S104" s="10"/>
       <c r="T104" s="10"/>
-    </row>
-    <row r="105" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N105" s="10"/>
+      <c r="U104" s="10"/>
+    </row>
+    <row r="105" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O105" s="10"/>
       <c r="P105" s="10"/>
       <c r="Q105" s="10"/>
       <c r="R105" s="10"/>
       <c r="S105" s="10"/>
       <c r="T105" s="10"/>
-    </row>
-    <row r="106" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N106" s="10"/>
+      <c r="U105" s="10"/>
+    </row>
+    <row r="106" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O106" s="10"/>
       <c r="P106" s="10"/>
       <c r="Q106" s="10"/>
       <c r="R106" s="10"/>
       <c r="S106" s="10"/>
       <c r="T106" s="10"/>
-    </row>
-    <row r="107" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N107" s="10"/>
+      <c r="U106" s="10"/>
+    </row>
+    <row r="107" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O107" s="10"/>
       <c r="P107" s="10"/>
       <c r="Q107" s="10"/>
       <c r="R107" s="10"/>
       <c r="S107" s="10"/>
       <c r="T107" s="10"/>
-    </row>
-    <row r="108" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N108" s="10"/>
+      <c r="U107" s="10"/>
+    </row>
+    <row r="108" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O108" s="10"/>
       <c r="P108" s="10"/>
       <c r="Q108" s="10"/>
       <c r="R108" s="10"/>
       <c r="S108" s="10"/>
       <c r="T108" s="10"/>
-    </row>
-    <row r="109" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N109" s="10"/>
+      <c r="U108" s="10"/>
+    </row>
+    <row r="109" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O109" s="10"/>
       <c r="P109" s="10"/>
       <c r="Q109" s="10"/>
       <c r="R109" s="10"/>
       <c r="S109" s="10"/>
       <c r="T109" s="10"/>
-    </row>
-    <row r="110" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N110" s="10"/>
+      <c r="U109" s="10"/>
+    </row>
+    <row r="110" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O110" s="10"/>
       <c r="P110" s="10"/>
       <c r="Q110" s="10"/>
       <c r="R110" s="10"/>
       <c r="S110" s="10"/>
       <c r="T110" s="10"/>
-    </row>
-    <row r="111" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N111" s="10"/>
+      <c r="U110" s="10"/>
+    </row>
+    <row r="111" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O111" s="10"/>
       <c r="P111" s="10"/>
       <c r="Q111" s="10"/>
       <c r="R111" s="10"/>
       <c r="S111" s="10"/>
       <c r="T111" s="10"/>
-    </row>
-    <row r="112" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N112" s="10"/>
+      <c r="U111" s="10"/>
+    </row>
+    <row r="112" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O112" s="10"/>
       <c r="P112" s="10"/>
       <c r="Q112" s="10"/>
       <c r="R112" s="10"/>
       <c r="S112" s="10"/>
       <c r="T112" s="10"/>
-    </row>
-    <row r="113" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N113" s="10"/>
+      <c r="U112" s="10"/>
+    </row>
+    <row r="113" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O113" s="10"/>
       <c r="P113" s="10"/>
       <c r="Q113" s="10"/>
       <c r="R113" s="10"/>
       <c r="S113" s="10"/>
       <c r="T113" s="10"/>
-    </row>
-    <row r="114" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N114" s="10"/>
+      <c r="U113" s="10"/>
+    </row>
+    <row r="114" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O114" s="10"/>
       <c r="P114" s="10"/>
       <c r="Q114" s="10"/>
       <c r="R114" s="10"/>
       <c r="S114" s="10"/>
       <c r="T114" s="10"/>
-    </row>
-    <row r="115" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N115" s="10"/>
+      <c r="U114" s="10"/>
+    </row>
+    <row r="115" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O115" s="10"/>
       <c r="P115" s="10"/>
       <c r="Q115" s="10"/>
       <c r="R115" s="10"/>
       <c r="S115" s="10"/>
       <c r="T115" s="10"/>
-    </row>
-    <row r="116" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N116" s="10"/>
+      <c r="U115" s="10"/>
+    </row>
+    <row r="116" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O116" s="10"/>
       <c r="P116" s="10"/>
       <c r="Q116" s="10"/>
       <c r="R116" s="10"/>
       <c r="S116" s="10"/>
       <c r="T116" s="10"/>
-    </row>
-    <row r="117" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N117" s="10"/>
+      <c r="U116" s="10"/>
+    </row>
+    <row r="117" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O117" s="10"/>
       <c r="P117" s="10"/>
       <c r="Q117" s="10"/>
       <c r="R117" s="10"/>
       <c r="S117" s="10"/>
       <c r="T117" s="10"/>
-    </row>
-    <row r="118" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N118" s="10"/>
+      <c r="U117" s="10"/>
+    </row>
+    <row r="118" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O118" s="10"/>
       <c r="P118" s="10"/>
       <c r="Q118" s="10"/>
       <c r="R118" s="10"/>
       <c r="S118" s="10"/>
       <c r="T118" s="10"/>
-    </row>
-    <row r="119" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N119" s="10"/>
+      <c r="U118" s="10"/>
+    </row>
+    <row r="119" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O119" s="10"/>
       <c r="P119" s="10"/>
       <c r="Q119" s="10"/>
       <c r="R119" s="10"/>
       <c r="S119" s="10"/>
       <c r="T119" s="10"/>
-    </row>
-    <row r="120" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N120" s="10"/>
+      <c r="U119" s="10"/>
+    </row>
+    <row r="120" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O120" s="10"/>
       <c r="P120" s="10"/>
       <c r="Q120" s="10"/>
       <c r="R120" s="10"/>
       <c r="S120" s="10"/>
       <c r="T120" s="10"/>
-    </row>
-    <row r="121" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N121" s="10"/>
+      <c r="U120" s="10"/>
+    </row>
+    <row r="121" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O121" s="10"/>
       <c r="P121" s="10"/>
       <c r="Q121" s="10"/>
       <c r="R121" s="10"/>
       <c r="S121" s="10"/>
       <c r="T121" s="10"/>
-    </row>
-    <row r="122" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N122" s="10"/>
+      <c r="U121" s="10"/>
+    </row>
+    <row r="122" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O122" s="10"/>
       <c r="P122" s="10"/>
       <c r="Q122" s="10"/>
       <c r="R122" s="10"/>
       <c r="S122" s="10"/>
       <c r="T122" s="10"/>
-    </row>
-    <row r="123" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N123" s="10"/>
+      <c r="U122" s="10"/>
+    </row>
+    <row r="123" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O123" s="10"/>
       <c r="P123" s="10"/>
       <c r="Q123" s="10"/>
       <c r="R123" s="10"/>
       <c r="S123" s="10"/>
       <c r="T123" s="10"/>
-    </row>
-    <row r="124" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N124" s="10"/>
+      <c r="U123" s="10"/>
+    </row>
+    <row r="124" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O124" s="10"/>
       <c r="P124" s="10"/>
       <c r="Q124" s="10"/>
       <c r="R124" s="10"/>
       <c r="S124" s="10"/>
       <c r="T124" s="10"/>
-    </row>
-    <row r="125" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N125" s="10"/>
+      <c r="U124" s="10"/>
+    </row>
+    <row r="125" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O125" s="10"/>
       <c r="P125" s="10"/>
       <c r="Q125" s="10"/>
       <c r="R125" s="10"/>
       <c r="S125" s="10"/>
       <c r="T125" s="10"/>
-    </row>
-    <row r="126" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N126" s="10"/>
+      <c r="U125" s="10"/>
+    </row>
+    <row r="126" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O126" s="10"/>
       <c r="P126" s="10"/>
       <c r="Q126" s="10"/>
       <c r="R126" s="10"/>
       <c r="S126" s="10"/>
       <c r="T126" s="10"/>
-    </row>
-    <row r="127" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N127" s="10"/>
+      <c r="U126" s="10"/>
+    </row>
+    <row r="127" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O127" s="10"/>
       <c r="P127" s="10"/>
       <c r="Q127" s="10"/>
       <c r="R127" s="10"/>
       <c r="S127" s="10"/>
       <c r="T127" s="10"/>
-    </row>
-    <row r="128" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N128" s="10"/>
+      <c r="U127" s="10"/>
+    </row>
+    <row r="128" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O128" s="10"/>
       <c r="P128" s="10"/>
       <c r="Q128" s="10"/>
       <c r="R128" s="10"/>
       <c r="S128" s="10"/>
       <c r="T128" s="10"/>
-    </row>
-    <row r="129" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N129" s="10"/>
+      <c r="U128" s="10"/>
+    </row>
+    <row r="129" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O129" s="10"/>
       <c r="P129" s="10"/>
       <c r="Q129" s="10"/>
       <c r="R129" s="10"/>
       <c r="S129" s="10"/>
       <c r="T129" s="10"/>
-    </row>
-    <row r="130" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N130" s="10"/>
+      <c r="U129" s="10"/>
+    </row>
+    <row r="130" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O130" s="10"/>
       <c r="P130" s="10"/>
       <c r="Q130" s="10"/>
       <c r="R130" s="10"/>
       <c r="S130" s="10"/>
       <c r="T130" s="10"/>
-    </row>
-    <row r="131" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N131" s="10"/>
+      <c r="U130" s="10"/>
+    </row>
+    <row r="131" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O131" s="10"/>
       <c r="P131" s="10"/>
       <c r="Q131" s="10"/>
       <c r="R131" s="10"/>
       <c r="S131" s="10"/>
       <c r="T131" s="10"/>
-    </row>
-    <row r="132" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N132" s="10"/>
+      <c r="U131" s="10"/>
+    </row>
+    <row r="132" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O132" s="10"/>
       <c r="P132" s="10"/>
       <c r="Q132" s="10"/>
       <c r="R132" s="10"/>
       <c r="S132" s="10"/>
       <c r="T132" s="10"/>
-    </row>
-    <row r="133" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N133" s="10"/>
+      <c r="U132" s="10"/>
+    </row>
+    <row r="133" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O133" s="10"/>
       <c r="P133" s="10"/>
       <c r="Q133" s="10"/>
       <c r="R133" s="10"/>
       <c r="S133" s="10"/>
       <c r="T133" s="10"/>
-    </row>
-    <row r="134" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N134" s="10"/>
+      <c r="U133" s="10"/>
+    </row>
+    <row r="134" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O134" s="10"/>
       <c r="P134" s="10"/>
       <c r="Q134" s="10"/>
       <c r="R134" s="10"/>
       <c r="S134" s="10"/>
       <c r="T134" s="10"/>
-    </row>
-    <row r="135" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N135" s="10"/>
+      <c r="U134" s="10"/>
+    </row>
+    <row r="135" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O135" s="10"/>
       <c r="P135" s="10"/>
       <c r="Q135" s="10"/>
       <c r="R135" s="10"/>
       <c r="S135" s="10"/>
       <c r="T135" s="10"/>
-    </row>
-    <row r="136" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N136" s="10"/>
+      <c r="U135" s="10"/>
+    </row>
+    <row r="136" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O136" s="10"/>
       <c r="P136" s="10"/>
       <c r="Q136" s="10"/>
       <c r="R136" s="10"/>
       <c r="S136" s="10"/>
       <c r="T136" s="10"/>
-    </row>
-    <row r="137" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N137" s="10"/>
+      <c r="U136" s="10"/>
+    </row>
+    <row r="137" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O137" s="10"/>
       <c r="P137" s="10"/>
       <c r="Q137" s="10"/>
       <c r="R137" s="10"/>
       <c r="S137" s="10"/>
       <c r="T137" s="10"/>
-    </row>
-    <row r="138" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N138" s="10"/>
+      <c r="U137" s="10"/>
+    </row>
+    <row r="138" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O138" s="10"/>
       <c r="P138" s="10"/>
       <c r="Q138" s="10"/>
       <c r="R138" s="10"/>
       <c r="S138" s="10"/>
       <c r="T138" s="10"/>
-    </row>
-    <row r="139" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N139" s="10"/>
+      <c r="U138" s="10"/>
+    </row>
+    <row r="139" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O139" s="10"/>
       <c r="P139" s="10"/>
       <c r="Q139" s="10"/>
       <c r="R139" s="10"/>
       <c r="S139" s="10"/>
       <c r="T139" s="10"/>
-    </row>
-    <row r="140" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N140" s="10"/>
+      <c r="U139" s="10"/>
+    </row>
+    <row r="140" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O140" s="10"/>
       <c r="P140" s="10"/>
       <c r="Q140" s="10"/>
       <c r="R140" s="10"/>
       <c r="S140" s="10"/>
       <c r="T140" s="10"/>
-    </row>
-    <row r="141" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N141" s="10"/>
+      <c r="U140" s="10"/>
+    </row>
+    <row r="141" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O141" s="10"/>
       <c r="P141" s="10"/>
       <c r="Q141" s="10"/>
       <c r="R141" s="10"/>
       <c r="S141" s="10"/>
       <c r="T141" s="10"/>
-    </row>
-    <row r="142" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N142" s="10"/>
+      <c r="U141" s="10"/>
+    </row>
+    <row r="142" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O142" s="10"/>
       <c r="P142" s="10"/>
       <c r="Q142" s="10"/>
       <c r="R142" s="10"/>
       <c r="S142" s="10"/>
       <c r="T142" s="10"/>
-    </row>
-    <row r="143" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N143" s="10"/>
+      <c r="U142" s="10"/>
+    </row>
+    <row r="143" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O143" s="10"/>
       <c r="P143" s="10"/>
       <c r="Q143" s="10"/>
       <c r="R143" s="10"/>
       <c r="S143" s="10"/>
       <c r="T143" s="10"/>
-    </row>
-    <row r="144" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N144" s="10"/>
+      <c r="U143" s="10"/>
+    </row>
+    <row r="144" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O144" s="10"/>
       <c r="P144" s="10"/>
       <c r="Q144" s="10"/>
       <c r="R144" s="10"/>
       <c r="S144" s="10"/>
       <c r="T144" s="10"/>
-    </row>
-    <row r="145" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N145" s="10"/>
+      <c r="U144" s="10"/>
+    </row>
+    <row r="145" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O145" s="10"/>
       <c r="P145" s="10"/>
       <c r="Q145" s="10"/>
       <c r="R145" s="10"/>
       <c r="S145" s="10"/>
       <c r="T145" s="10"/>
-    </row>
-    <row r="146" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N146" s="10"/>
+      <c r="U145" s="10"/>
+    </row>
+    <row r="146" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O146" s="10"/>
       <c r="P146" s="10"/>
       <c r="Q146" s="10"/>
       <c r="R146" s="10"/>
       <c r="S146" s="10"/>
       <c r="T146" s="10"/>
-    </row>
-    <row r="147" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N147" s="10"/>
+      <c r="U146" s="10"/>
+    </row>
+    <row r="147" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O147" s="10"/>
       <c r="P147" s="10"/>
       <c r="Q147" s="10"/>
       <c r="R147" s="10"/>
       <c r="S147" s="10"/>
       <c r="T147" s="10"/>
-    </row>
-    <row r="148" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N148" s="10"/>
+      <c r="U147" s="10"/>
+    </row>
+    <row r="148" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O148" s="10"/>
       <c r="P148" s="10"/>
       <c r="Q148" s="10"/>
       <c r="R148" s="10"/>
       <c r="S148" s="10"/>
       <c r="T148" s="10"/>
-    </row>
-    <row r="149" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N149" s="10"/>
+      <c r="U148" s="10"/>
+    </row>
+    <row r="149" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O149" s="10"/>
       <c r="P149" s="10"/>
       <c r="Q149" s="10"/>
       <c r="R149" s="10"/>
       <c r="S149" s="10"/>
       <c r="T149" s="10"/>
-    </row>
-    <row r="150" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N150" s="10"/>
+      <c r="U149" s="10"/>
+    </row>
+    <row r="150" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O150" s="10"/>
       <c r="P150" s="10"/>
       <c r="Q150" s="10"/>
       <c r="R150" s="10"/>
       <c r="S150" s="10"/>
       <c r="T150" s="10"/>
-    </row>
-    <row r="151" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N151" s="10"/>
+      <c r="U150" s="10"/>
+    </row>
+    <row r="151" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O151" s="10"/>
       <c r="P151" s="10"/>
       <c r="Q151" s="10"/>
       <c r="R151" s="10"/>
       <c r="S151" s="10"/>
       <c r="T151" s="10"/>
-    </row>
-    <row r="152" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N152" s="10"/>
+      <c r="U151" s="10"/>
+    </row>
+    <row r="152" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O152" s="10"/>
       <c r="P152" s="10"/>
       <c r="Q152" s="10"/>
       <c r="R152" s="10"/>
       <c r="S152" s="10"/>
       <c r="T152" s="10"/>
-    </row>
-    <row r="153" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N153" s="10"/>
+      <c r="U152" s="10"/>
+    </row>
+    <row r="153" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O153" s="10"/>
       <c r="P153" s="10"/>
       <c r="Q153" s="10"/>
       <c r="R153" s="10"/>
       <c r="S153" s="10"/>
       <c r="T153" s="10"/>
-    </row>
-    <row r="154" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N154" s="10"/>
+      <c r="U153" s="10"/>
+    </row>
+    <row r="154" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O154" s="10"/>
       <c r="P154" s="10"/>
       <c r="Q154" s="10"/>
       <c r="R154" s="10"/>
       <c r="S154" s="10"/>
       <c r="T154" s="10"/>
-    </row>
-    <row r="155" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N155" s="10"/>
+      <c r="U154" s="10"/>
+    </row>
+    <row r="155" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O155" s="10"/>
       <c r="P155" s="10"/>
       <c r="Q155" s="10"/>
       <c r="R155" s="10"/>
       <c r="S155" s="10"/>
       <c r="T155" s="10"/>
-    </row>
-    <row r="156" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N156" s="10"/>
+      <c r="U155" s="10"/>
+    </row>
+    <row r="156" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O156" s="10"/>
       <c r="P156" s="10"/>
       <c r="Q156" s="10"/>
       <c r="R156" s="10"/>
       <c r="S156" s="10"/>
       <c r="T156" s="10"/>
-    </row>
-    <row r="157" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N157" s="10"/>
+      <c r="U156" s="10"/>
+    </row>
+    <row r="157" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O157" s="10"/>
       <c r="P157" s="10"/>
       <c r="Q157" s="10"/>
       <c r="R157" s="10"/>
       <c r="S157" s="10"/>
       <c r="T157" s="10"/>
-    </row>
-    <row r="158" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N158" s="10"/>
+      <c r="U157" s="10"/>
+    </row>
+    <row r="158" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O158" s="10"/>
       <c r="P158" s="10"/>
       <c r="Q158" s="10"/>
       <c r="R158" s="10"/>
       <c r="S158" s="10"/>
       <c r="T158" s="10"/>
-    </row>
-    <row r="159" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N159" s="10"/>
+      <c r="U158" s="10"/>
+    </row>
+    <row r="159" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O159" s="10"/>
       <c r="P159" s="10"/>
       <c r="Q159" s="10"/>
       <c r="R159" s="10"/>
       <c r="S159" s="10"/>
       <c r="T159" s="10"/>
-    </row>
-    <row r="160" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N160" s="10"/>
+      <c r="U159" s="10"/>
+    </row>
+    <row r="160" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O160" s="10"/>
       <c r="P160" s="10"/>
       <c r="Q160" s="10"/>
       <c r="R160" s="10"/>
       <c r="S160" s="10"/>
       <c r="T160" s="10"/>
-    </row>
-    <row r="161" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N161" s="10"/>
+      <c r="U160" s="10"/>
+    </row>
+    <row r="161" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O161" s="10"/>
       <c r="P161" s="10"/>
       <c r="Q161" s="10"/>
       <c r="R161" s="10"/>
       <c r="S161" s="10"/>
       <c r="T161" s="10"/>
-    </row>
-    <row r="162" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N162" s="10"/>
+      <c r="U161" s="10"/>
+    </row>
+    <row r="162" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O162" s="10"/>
       <c r="P162" s="10"/>
       <c r="Q162" s="10"/>
       <c r="R162" s="10"/>
       <c r="S162" s="10"/>
       <c r="T162" s="10"/>
-    </row>
-    <row r="163" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N163" s="10"/>
+      <c r="U162" s="10"/>
+    </row>
+    <row r="163" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O163" s="10"/>
       <c r="P163" s="10"/>
       <c r="Q163" s="10"/>
       <c r="R163" s="10"/>
       <c r="S163" s="10"/>
       <c r="T163" s="10"/>
-    </row>
-    <row r="164" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N164" s="10"/>
+      <c r="U163" s="10"/>
+    </row>
+    <row r="164" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O164" s="10"/>
       <c r="P164" s="10"/>
       <c r="Q164" s="10"/>
       <c r="R164" s="10"/>
       <c r="S164" s="10"/>
       <c r="T164" s="10"/>
-    </row>
-    <row r="165" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N165" s="10"/>
+      <c r="U164" s="10"/>
+    </row>
+    <row r="165" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O165" s="10"/>
       <c r="P165" s="10"/>
       <c r="Q165" s="10"/>
       <c r="R165" s="10"/>
       <c r="S165" s="10"/>
       <c r="T165" s="10"/>
-    </row>
-    <row r="166" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N166" s="10"/>
+      <c r="U165" s="10"/>
+    </row>
+    <row r="166" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O166" s="10"/>
       <c r="P166" s="10"/>
       <c r="Q166" s="10"/>
       <c r="R166" s="10"/>
       <c r="S166" s="10"/>
       <c r="T166" s="10"/>
-    </row>
-    <row r="167" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N167" s="10"/>
+      <c r="U166" s="10"/>
+    </row>
+    <row r="167" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O167" s="10"/>
       <c r="P167" s="10"/>
       <c r="Q167" s="10"/>
       <c r="R167" s="10"/>
       <c r="S167" s="10"/>
       <c r="T167" s="10"/>
-    </row>
-    <row r="168" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N168" s="10"/>
+      <c r="U167" s="10"/>
+    </row>
+    <row r="168" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O168" s="10"/>
       <c r="P168" s="10"/>
       <c r="Q168" s="10"/>
       <c r="R168" s="10"/>
       <c r="S168" s="10"/>
       <c r="T168" s="10"/>
-    </row>
-    <row r="169" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N169" s="10"/>
+      <c r="U168" s="10"/>
+    </row>
+    <row r="169" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O169" s="10"/>
       <c r="P169" s="10"/>
       <c r="Q169" s="10"/>
       <c r="R169" s="10"/>
       <c r="S169" s="10"/>
       <c r="T169" s="10"/>
-    </row>
-    <row r="170" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N170" s="10"/>
+      <c r="U169" s="10"/>
+    </row>
+    <row r="170" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O170" s="10"/>
       <c r="P170" s="10"/>
       <c r="Q170" s="10"/>
       <c r="R170" s="10"/>
       <c r="S170" s="10"/>
       <c r="T170" s="10"/>
-    </row>
-    <row r="171" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N171" s="10"/>
+      <c r="U170" s="10"/>
+    </row>
+    <row r="171" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O171" s="10"/>
       <c r="P171" s="10"/>
       <c r="Q171" s="10"/>
       <c r="R171" s="10"/>
       <c r="S171" s="10"/>
       <c r="T171" s="10"/>
-    </row>
-    <row r="172" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N172" s="10"/>
+      <c r="U171" s="10"/>
+    </row>
+    <row r="172" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O172" s="10"/>
       <c r="P172" s="10"/>
       <c r="Q172" s="10"/>
       <c r="R172" s="10"/>
       <c r="S172" s="10"/>
       <c r="T172" s="10"/>
-    </row>
-    <row r="173" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N173" s="10"/>
+      <c r="U172" s="10"/>
+    </row>
+    <row r="173" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O173" s="10"/>
       <c r="P173" s="10"/>
       <c r="Q173" s="10"/>
       <c r="R173" s="10"/>
       <c r="S173" s="10"/>
       <c r="T173" s="10"/>
-    </row>
-    <row r="174" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N174" s="10"/>
+      <c r="U173" s="10"/>
+    </row>
+    <row r="174" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O174" s="10"/>
       <c r="P174" s="10"/>
       <c r="Q174" s="10"/>
       <c r="R174" s="10"/>
       <c r="S174" s="10"/>
       <c r="T174" s="10"/>
-    </row>
-    <row r="175" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N175" s="10"/>
+      <c r="U174" s="10"/>
+    </row>
+    <row r="175" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O175" s="10"/>
       <c r="P175" s="10"/>
       <c r="Q175" s="10"/>
       <c r="R175" s="10"/>
       <c r="S175" s="10"/>
       <c r="T175" s="10"/>
-    </row>
-    <row r="176" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N176" s="10"/>
+      <c r="U175" s="10"/>
+    </row>
+    <row r="176" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O176" s="10"/>
       <c r="P176" s="10"/>
       <c r="Q176" s="10"/>
       <c r="R176" s="10"/>
       <c r="S176" s="10"/>
       <c r="T176" s="10"/>
-    </row>
-    <row r="177" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N177" s="10"/>
+      <c r="U176" s="10"/>
+    </row>
+    <row r="177" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O177" s="10"/>
       <c r="P177" s="10"/>
       <c r="Q177" s="10"/>
       <c r="R177" s="10"/>
       <c r="S177" s="10"/>
       <c r="T177" s="10"/>
-    </row>
-    <row r="178" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N178" s="10"/>
+      <c r="U177" s="10"/>
+    </row>
+    <row r="178" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O178" s="10"/>
       <c r="P178" s="10"/>
       <c r="Q178" s="10"/>
       <c r="R178" s="10"/>
       <c r="S178" s="10"/>
       <c r="T178" s="10"/>
-    </row>
-    <row r="179" spans="14:20" x14ac:dyDescent="0.3">
-      <c r="N179" s="10"/>
+      <c r="U178" s="10"/>
+    </row>
+    <row r="179" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O179" s="10"/>
       <c r="P179" s="10"/>
       <c r="Q179" s="10"/>
       <c r="R179" s="10"/>
       <c r="S179" s="10"/>
       <c r="T179" s="10"/>
+      <c r="U179" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
-      <formula1>"Initial,Potential,Customer,Support,Upsells,Reject,Not-Contacted,Ex-Customer"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
+      <formula1>"Initial,Potential,Customer,Workshop Fixed,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0300-000002000000}">

</xml_diff>

<commit_message>
Updated AI Workshop & Schools
Updated AI Workshop & Schools
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FDC802-9D60-4F54-AB36-F9E0B7913E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDD071A-49FF-49FC-80E8-7C515B386D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="573">
   <si>
     <t>CBSE</t>
   </si>
@@ -1864,6 +1864,9 @@
   </si>
   <si>
     <t>wbasansol.etechno@narayanagroup.com</t>
+  </si>
+  <si>
+    <t>Workshop Fixed</t>
   </si>
 </sst>
 </file>
@@ -2050,7 +2053,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -2163,36 +2166,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -2405,8 +2378,6 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2428,7 +2399,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2443,13 +2421,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2733,8 +2706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:Q2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,27 +2731,33 @@
     <row r="2" spans="2:18" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="68" t="s">
         <v>293</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="29"/>
       <c r="K2" s="27"/>
       <c r="L2" s="28"/>
-      <c r="M2" s="72" t="s">
+      <c r="M2" s="71" t="s">
         <v>374</v>
       </c>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="74"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="73"/>
       <c r="R2" s="29"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="30"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
       <c r="I3" s="31"/>
       <c r="K3" s="30"/>
       <c r="R3" s="31"/>
@@ -2792,12 +2771,14 @@
         <f>MAX('School-Details'!A:A)</f>
         <v>143</v>
       </c>
+      <c r="E4" s="74"/>
       <c r="F4" s="21" t="s">
         <v>265</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>266</v>
       </c>
+      <c r="H4" s="74"/>
       <c r="I4" s="31"/>
       <c r="K4" s="30"/>
       <c r="L4" s="16" t="s">
@@ -2824,6 +2805,7 @@
         <f>ROUND(SUM('School-Details'!K:K)/D4,2)</f>
         <v>0.01</v>
       </c>
+      <c r="E5" s="74"/>
       <c r="F5" s="14" t="s">
         <v>210</v>
       </c>
@@ -2831,6 +2813,7 @@
         <f>COUNTIF('School-Details'!N:N,F5)</f>
         <v>0</v>
       </c>
+      <c r="H5" s="74"/>
       <c r="I5" s="31"/>
       <c r="K5" s="30"/>
       <c r="L5" s="16" t="s">
@@ -2857,6 +2840,7 @@
       <c r="D6" s="53">
         <v>45299</v>
       </c>
+      <c r="E6" s="74"/>
       <c r="F6" s="14" t="s">
         <v>267</v>
       </c>
@@ -2864,6 +2848,7 @@
         <f>COUNTIF('School-Details'!N:N,F6)</f>
         <v>1</v>
       </c>
+      <c r="H6" s="74"/>
       <c r="I6" s="31"/>
       <c r="K6" s="30"/>
       <c r="L6" s="16" t="s">
@@ -2891,6 +2876,7 @@
         <f ca="1">TODAY()</f>
         <v>45307</v>
       </c>
+      <c r="E7" s="74"/>
       <c r="F7" s="14" t="s">
         <v>268</v>
       </c>
@@ -2898,6 +2884,7 @@
         <f>COUNTIF('School-Details'!N:N,F7)</f>
         <v>0</v>
       </c>
+      <c r="H7" s="74"/>
       <c r="I7" s="31"/>
       <c r="K7" s="30"/>
       <c r="L7" s="16" t="s">
@@ -2925,6 +2912,7 @@
         <f ca="1">ROUND(D11/(D7-D6+1),0)</f>
         <v>4</v>
       </c>
+      <c r="E8" s="74"/>
       <c r="F8" s="14" t="s">
         <v>283</v>
       </c>
@@ -2932,6 +2920,7 @@
         <f>COUNTIF('School-Details'!N:N,F8)</f>
         <v>0</v>
       </c>
+      <c r="H8" s="74"/>
       <c r="I8" s="31"/>
       <c r="K8" s="30"/>
       <c r="L8" s="16" t="s">
@@ -2949,6 +2938,9 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="30"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
       <c r="F9" s="16" t="s">
         <v>244</v>
       </c>
@@ -2956,6 +2948,7 @@
         <f>SUM(G5:G8)</f>
         <v>1</v>
       </c>
+      <c r="H9" s="74"/>
       <c r="I9" s="31"/>
       <c r="K9" s="30"/>
       <c r="L9" s="16" t="s">
@@ -2982,6 +2975,10 @@
       <c r="D10" s="21" t="s">
         <v>264</v>
       </c>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
       <c r="I10" s="31"/>
       <c r="K10" s="30"/>
       <c r="L10" s="16" t="s">
@@ -3002,18 +2999,19 @@
         <f>COUNTIF('School-Details'!V:V,C11)</f>
         <v>34</v>
       </c>
+      <c r="E11" s="74"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="68" t="s">
+      <c r="G11" s="67" t="s">
         <v>210</v>
       </c>
-      <c r="H11" s="68"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="31"/>
       <c r="K11" s="30"/>
       <c r="O11" s="14"/>
-      <c r="P11" s="68" t="s">
+      <c r="P11" s="67" t="s">
         <v>210</v>
       </c>
-      <c r="Q11" s="68"/>
+      <c r="Q11" s="67"/>
       <c r="R11" s="31"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
@@ -3025,6 +3023,7 @@
         <f>COUNTIF('School-Details'!V:V,C12)</f>
         <v>0</v>
       </c>
+      <c r="E12" s="74"/>
       <c r="F12" s="21" t="s">
         <v>269</v>
       </c>
@@ -3062,6 +3061,7 @@
         <f>COUNTIF('School-Details'!V:V,C13)</f>
         <v>0</v>
       </c>
+      <c r="E13" s="74"/>
       <c r="F13" s="22">
         <v>45292</v>
       </c>
@@ -3094,12 +3094,13 @@
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="30"/>
       <c r="C14" s="14" t="s">
-        <v>257</v>
+        <v>572</v>
       </c>
       <c r="D14" s="14">
         <f>COUNTIF('School-Details'!V:V,C14)</f>
         <v>0</v>
       </c>
+      <c r="E14" s="74"/>
       <c r="F14" s="22">
         <v>45323</v>
       </c>
@@ -3132,12 +3133,13 @@
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="30"/>
       <c r="C15" s="14" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D15" s="14">
         <f>COUNTIF('School-Details'!V:V,C15)</f>
         <v>0</v>
       </c>
+      <c r="E15" s="74"/>
       <c r="F15" s="22">
         <v>45352</v>
       </c>
@@ -3170,12 +3172,13 @@
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="30"/>
       <c r="C16" s="14" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D16" s="14">
         <f>COUNTIF('School-Details'!V:V,C16)</f>
-        <v>0</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E16" s="74"/>
       <c r="F16" s="22">
         <v>45383</v>
       </c>
@@ -3188,7 +3191,7 @@
       <c r="I16" s="31"/>
       <c r="K16" s="30"/>
       <c r="L16" s="14" t="s">
-        <v>257</v>
+        <v>572</v>
       </c>
       <c r="M16" s="14">
         <f>COUNTIF('College-Details'!V:V,L16)</f>
@@ -3208,12 +3211,13 @@
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="30"/>
       <c r="C17" s="14" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="D17" s="14">
         <f>COUNTIF('School-Details'!V:V,C17)</f>
-        <v>91</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E17" s="74"/>
       <c r="F17" s="22">
         <v>45413</v>
       </c>
@@ -3226,7 +3230,7 @@
       <c r="I17" s="31"/>
       <c r="K17" s="30"/>
       <c r="L17" s="14" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="M17" s="14">
         <f>COUNTIF('College-Details'!V:V,L17)</f>
@@ -3245,13 +3249,14 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B18" s="30"/>
-      <c r="C18" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="D18" s="14">
-        <f>COUNTIF('School-Details'!V:V,C18)</f>
-        <v>0</v>
-      </c>
+      <c r="C18" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D18" s="16">
+        <f>SUM(D11:D17)</f>
+        <v>125</v>
+      </c>
+      <c r="E18" s="74"/>
       <c r="F18" s="22">
         <v>45444</v>
       </c>
@@ -3264,11 +3269,11 @@
       <c r="I18" s="31"/>
       <c r="K18" s="30"/>
       <c r="L18" s="14" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M18" s="14">
         <f>COUNTIF('College-Details'!V:V,L18)</f>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="O18" s="22">
         <v>45444</v>
@@ -3283,13 +3288,9 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="30"/>
-      <c r="C19" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="D19" s="16">
-        <f>SUM(D11:D18)</f>
-        <v>125</v>
-      </c>
+      <c r="C19" s="74"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
       <c r="F19" s="22">
         <v>45474</v>
       </c>
@@ -3302,11 +3303,11 @@
       <c r="I19" s="31"/>
       <c r="K19" s="30"/>
       <c r="L19" s="14" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="M19" s="14">
         <f>COUNTIF('College-Details'!V:V,L19)</f>
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="O19" s="22">
         <v>45474</v>
@@ -3320,7 +3321,14 @@
       <c r="R19" s="31"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="30"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="21" t="s">
+        <v>274</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="E20" s="74"/>
       <c r="F20" s="22">
         <v>45505</v>
       </c>
@@ -3332,12 +3340,12 @@
       </c>
       <c r="I20" s="31"/>
       <c r="K20" s="30"/>
-      <c r="L20" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="M20" s="14">
-        <f>COUNTIF('College-Details'!V:V,L20)</f>
-        <v>0</v>
+      <c r="L20" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="M20" s="16">
+        <f>SUM(M13:M19)</f>
+        <v>53</v>
       </c>
       <c r="O20" s="22">
         <v>45505</v>
@@ -3351,13 +3359,17 @@
       <c r="R20" s="31"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="32"/>
-      <c r="C21" s="21" t="s">
-        <v>274</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>264</v>
-      </c>
+      <c r="B21" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="14">
+        <v>5</v>
+      </c>
+      <c r="D21" s="14">
+        <f>COUNTIF('School-Details'!U:U,C21)</f>
+        <v>10</v>
+      </c>
+      <c r="E21" s="74"/>
       <c r="F21" s="22">
         <v>45536</v>
       </c>
@@ -3369,13 +3381,6 @@
       </c>
       <c r="I21" s="31"/>
       <c r="K21" s="30"/>
-      <c r="L21" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="M21" s="16">
-        <f>SUM(M13:M20)</f>
-        <v>53</v>
-      </c>
       <c r="O21" s="22">
         <v>45536</v>
       </c>
@@ -3388,16 +3393,15 @@
       <c r="R21" s="31"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="33" t="s">
-        <v>272</v>
-      </c>
+      <c r="B22" s="14"/>
       <c r="C22" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="14">
         <f>COUNTIF('School-Details'!U:U,C22)</f>
-        <v>10</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E22" s="74"/>
       <c r="F22" s="22">
         <v>45566</v>
       </c>
@@ -3421,14 +3425,15 @@
       <c r="R22" s="31"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B23" s="33"/>
-      <c r="C23" s="14">
-        <v>4</v>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14" t="s">
+        <v>275</v>
       </c>
       <c r="D23" s="14">
-        <f>COUNTIF('School-Details'!U:U,C23)</f>
-        <v>55</v>
-      </c>
+        <f>SUM(D21:D22)</f>
+        <v>65</v>
+      </c>
+      <c r="E23" s="74"/>
       <c r="F23" s="22">
         <v>45597</v>
       </c>
@@ -3458,14 +3463,17 @@
       <c r="R23" s="31"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B24" s="33"/>
-      <c r="C24" s="14" t="s">
-        <v>275</v>
+      <c r="B24" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C24" s="14">
+        <v>3</v>
       </c>
       <c r="D24" s="14">
-        <f>SUM(D22:D23)</f>
-        <v>65</v>
-      </c>
+        <f>COUNTIF('School-Details'!U:U,C24)</f>
+        <v>50</v>
+      </c>
+      <c r="E24" s="74"/>
       <c r="F24" s="22">
         <v>45627</v>
       </c>
@@ -3498,16 +3506,15 @@
       <c r="R24" s="31"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B25" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="C25" s="14">
-        <v>3</v>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14" t="s">
+        <v>277</v>
       </c>
       <c r="D25" s="14">
-        <f>COUNTIF('School-Details'!U:U,C25)</f>
+        <f>SUM(D24)</f>
         <v>50</v>
       </c>
+      <c r="E25" s="74"/>
       <c r="F25" s="16" t="s">
         <v>244</v>
       </c>
@@ -3542,14 +3549,20 @@
       <c r="R25" s="31"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B26" s="33"/>
-      <c r="C26" s="14" t="s">
-        <v>277</v>
+      <c r="B26" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="C26" s="14">
+        <v>2</v>
       </c>
       <c r="D26" s="14">
-        <f>SUM(D25)</f>
-        <v>50</v>
-      </c>
+        <f>COUNTIF('School-Details'!U:U,C26)</f>
+        <v>10</v>
+      </c>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
       <c r="I26" s="31"/>
       <c r="K26" s="33"/>
       <c r="L26" s="14" t="s">
@@ -3562,16 +3575,18 @@
       <c r="R26" s="31"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B27" s="33" t="s">
-        <v>273</v>
-      </c>
+      <c r="B27" s="14"/>
       <c r="C27" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="14">
         <f>COUNTIF('School-Details'!U:U,C27)</f>
-        <v>10</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
       <c r="I27" s="31"/>
       <c r="K27" s="33" t="s">
         <v>278</v>
@@ -3586,14 +3601,18 @@
       <c r="R27" s="31"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B28" s="33"/>
-      <c r="C28" s="14">
-        <v>1</v>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14" t="s">
+        <v>276</v>
       </c>
       <c r="D28" s="14">
-        <f>COUNTIF('School-Details'!U:U,C28)</f>
-        <v>0</v>
-      </c>
+        <f>SUM(D26:D27)</f>
+        <v>10</v>
+      </c>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
       <c r="I28" s="31"/>
       <c r="K28" s="33"/>
       <c r="L28" s="14" t="s">
@@ -3606,14 +3625,18 @@
       <c r="R28" s="31"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B29" s="33"/>
-      <c r="C29" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="D29" s="14">
-        <f>SUM(D27:D28)</f>
-        <v>10</v>
-      </c>
+      <c r="B29" s="14"/>
+      <c r="C29" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D29" s="16">
+        <f>D23+D25+D28</f>
+        <v>125</v>
+      </c>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
       <c r="I29" s="31"/>
       <c r="K29" s="33" t="s">
         <v>273</v>
@@ -3628,14 +3651,9 @@
       <c r="R29" s="31"/>
     </row>
     <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="55"/>
-      <c r="C30" s="56" t="s">
-        <v>244</v>
-      </c>
-      <c r="D30" s="56">
-        <f>D24+D26+D29</f>
-        <v>125</v>
-      </c>
+      <c r="B30" s="34"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
       <c r="E30" s="35"/>
       <c r="F30" s="35"/>
       <c r="G30" s="35"/>
@@ -3699,11 +3717,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D137" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="N120" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F144" sqref="F144"/>
+      <selection pane="bottomRight" activeCell="V120" sqref="V120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4181,7 +4199,7 @@
       <c r="G10" s="40" t="s">
         <v>471</v>
       </c>
-      <c r="H10" s="62" t="s">
+      <c r="H10" s="60" t="s">
         <v>472</v>
       </c>
       <c r="O10" s="10">
@@ -4451,10 +4469,10 @@
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="61" t="s">
         <v>482</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="61" t="s">
         <v>483</v>
       </c>
       <c r="F16" s="7" t="s">
@@ -4497,7 +4515,7 @@
       <c r="D17" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="E17" s="64" t="s">
+      <c r="E17" s="62" t="s">
         <v>485</v>
       </c>
       <c r="F17" s="7" t="s">
@@ -5465,7 +5483,7 @@
       <c r="C39" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="65" t="s">
+      <c r="D39" s="63" t="s">
         <v>491</v>
       </c>
       <c r="F39" s="9">
@@ -5683,7 +5701,7 @@
       <c r="C44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D44" s="66" t="s">
+      <c r="D44" s="64" t="s">
         <v>492</v>
       </c>
       <c r="F44" s="7">
@@ -7767,10 +7785,10 @@
       <c r="C92" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D92" s="67" t="s">
+      <c r="D92" s="65" t="s">
         <v>500</v>
       </c>
-      <c r="E92" s="67" t="s">
+      <c r="E92" s="65" t="s">
         <v>501</v>
       </c>
       <c r="F92" s="7">
@@ -9263,7 +9281,7 @@
       <c r="D130" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="F130" s="62" t="s">
+      <c r="F130" s="60" t="s">
         <v>519</v>
       </c>
       <c r="G130" s="40" t="s">
@@ -9286,7 +9304,7 @@
       <c r="D131" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="F131" s="75" t="s">
+      <c r="F131" s="66" t="s">
         <v>524</v>
       </c>
       <c r="G131" s="40" t="s">
@@ -13308,12 +13326,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="60" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" style="58" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="59" t="s">
         <v>248</v>
       </c>
       <c r="B1" s="21" t="s">
@@ -13407,36 +13425,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="58" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="56" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="38">
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="55" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="58" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="56" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="38">
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="55" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="58" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="56" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="57" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update AI workshop for schools & colleges
Update AI workshop for schools & colleges
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2A18BC-EDB9-4D8F-B5ED-FF02DB8968B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -22,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'School-Details'!$A$1:$V$124</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,13 +42,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
     <author>User</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M28" authorId="1" shapeId="0">
+    <comment ref="M28" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -90,12 +91,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>del</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -2358,7 +2359,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="36">
     <font>
       <sz val="11"/>
@@ -2995,16 +2996,16 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3034,6 +3035,12 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3054,12 +3061,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3341,7 +3342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3369,23 +3370,23 @@
     <row r="2" spans="2:18" ht="34.200000000000003" thickBot="1">
       <c r="B2" s="27"/>
       <c r="C2" s="28"/>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="93" t="s">
         <v>293</v>
       </c>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="93"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="95"/>
       <c r="I2" s="29"/>
       <c r="K2" s="27"/>
       <c r="L2" s="28"/>
-      <c r="M2" s="94" t="s">
+      <c r="M2" s="96" t="s">
         <v>374</v>
       </c>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="96"/>
+      <c r="N2" s="97"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="98"/>
       <c r="R2" s="29"/>
     </row>
     <row r="3" spans="2:18">
@@ -3614,17 +3615,17 @@
         <v>34</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="90" t="s">
+      <c r="G11" s="92" t="s">
         <v>210</v>
       </c>
-      <c r="H11" s="90"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="31"/>
       <c r="K11" s="30"/>
       <c r="O11" s="14"/>
-      <c r="P11" s="90" t="s">
+      <c r="P11" s="92" t="s">
         <v>210</v>
       </c>
-      <c r="Q11" s="90"/>
+      <c r="Q11" s="92"/>
       <c r="R11" s="31"/>
     </row>
     <row r="12" spans="2:18">
@@ -4295,7 +4296,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12959,156 +12960,156 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V124"/>
+  <autoFilter ref="A1:V124" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Initial,Potential,Customer,Workshp Fixed,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1"/>
-    <hyperlink ref="D32" r:id="rId2"/>
-    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp"/>
-    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w"/>
-    <hyperlink ref="D22" r:id="rId5"/>
-    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com"/>
-    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in"/>
-    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com"/>
-    <hyperlink ref="D30" r:id="rId9"/>
-    <hyperlink ref="D33" r:id="rId10"/>
-    <hyperlink ref="D35" r:id="rId11"/>
-    <hyperlink ref="D37" r:id="rId12"/>
-    <hyperlink ref="D41" r:id="rId13"/>
-    <hyperlink ref="D42" r:id="rId14"/>
-    <hyperlink ref="D43" r:id="rId15"/>
-    <hyperlink ref="D47" r:id="rId16"/>
-    <hyperlink ref="D48" r:id="rId17"/>
-    <hyperlink ref="D49" r:id="rId18"/>
-    <hyperlink ref="D51" r:id="rId19"/>
-    <hyperlink ref="D52" r:id="rId20"/>
-    <hyperlink ref="D53" r:id="rId21"/>
-    <hyperlink ref="D54" r:id="rId22"/>
-    <hyperlink ref="D55" r:id="rId23"/>
-    <hyperlink ref="D56" r:id="rId24"/>
-    <hyperlink ref="D57" r:id="rId25"/>
-    <hyperlink ref="D58" r:id="rId26"/>
-    <hyperlink ref="D59" r:id="rId27"/>
-    <hyperlink ref="D60" r:id="rId28"/>
-    <hyperlink ref="D61" r:id="rId29"/>
-    <hyperlink ref="D62" r:id="rId30"/>
-    <hyperlink ref="D63" r:id="rId31"/>
-    <hyperlink ref="D64" r:id="rId32"/>
-    <hyperlink ref="D65" r:id="rId33"/>
-    <hyperlink ref="D66" r:id="rId34"/>
-    <hyperlink ref="D67" r:id="rId35"/>
-    <hyperlink ref="D68" r:id="rId36"/>
-    <hyperlink ref="D69" r:id="rId37"/>
-    <hyperlink ref="D70" r:id="rId38"/>
-    <hyperlink ref="D71" r:id="rId39"/>
-    <hyperlink ref="D72" r:id="rId40"/>
-    <hyperlink ref="D73" r:id="rId41"/>
-    <hyperlink ref="D75" r:id="rId42"/>
-    <hyperlink ref="D78" r:id="rId43"/>
-    <hyperlink ref="D79" r:id="rId44"/>
-    <hyperlink ref="D80" r:id="rId45"/>
-    <hyperlink ref="D81" r:id="rId46"/>
-    <hyperlink ref="D85" r:id="rId47"/>
-    <hyperlink ref="D88" r:id="rId48"/>
-    <hyperlink ref="D89" r:id="rId49"/>
-    <hyperlink ref="D91" r:id="rId50"/>
-    <hyperlink ref="D2" r:id="rId51"/>
-    <hyperlink ref="D28" r:id="rId52"/>
-    <hyperlink ref="E2" r:id="rId53"/>
-    <hyperlink ref="D3" r:id="rId54"/>
-    <hyperlink ref="D4" r:id="rId55"/>
-    <hyperlink ref="E4" r:id="rId56"/>
-    <hyperlink ref="D5" r:id="rId57"/>
-    <hyperlink ref="D7" r:id="rId58"/>
-    <hyperlink ref="D6" r:id="rId59"/>
-    <hyperlink ref="E6" r:id="rId60"/>
-    <hyperlink ref="D8" r:id="rId61"/>
-    <hyperlink ref="E8" r:id="rId62"/>
-    <hyperlink ref="D9" r:id="rId63"/>
-    <hyperlink ref="D10" r:id="rId64"/>
-    <hyperlink ref="D12" r:id="rId65"/>
-    <hyperlink ref="D13" r:id="rId66"/>
-    <hyperlink ref="E13" r:id="rId67"/>
-    <hyperlink ref="D14" r:id="rId68"/>
-    <hyperlink ref="E14" r:id="rId69"/>
-    <hyperlink ref="D15" r:id="rId70"/>
-    <hyperlink ref="D17" r:id="rId71"/>
-    <hyperlink ref="D18" r:id="rId72"/>
-    <hyperlink ref="E18" r:id="rId73"/>
-    <hyperlink ref="D19" r:id="rId74"/>
-    <hyperlink ref="D38" r:id="rId75"/>
-    <hyperlink ref="D40" r:id="rId76"/>
-    <hyperlink ref="D44" r:id="rId77"/>
-    <hyperlink ref="D45" r:id="rId78"/>
-    <hyperlink ref="D82" r:id="rId79"/>
-    <hyperlink ref="D83" r:id="rId80"/>
-    <hyperlink ref="D84" r:id="rId81"/>
-    <hyperlink ref="D86" r:id="rId82"/>
-    <hyperlink ref="D87" r:id="rId83"/>
-    <hyperlink ref="D90" r:id="rId84"/>
-    <hyperlink ref="D127" r:id="rId85"/>
-    <hyperlink ref="D128" r:id="rId86"/>
-    <hyperlink ref="D129" r:id="rId87"/>
-    <hyperlink ref="D130" r:id="rId88"/>
-    <hyperlink ref="D131" r:id="rId89"/>
-    <hyperlink ref="D132" r:id="rId90"/>
-    <hyperlink ref="D133" r:id="rId91"/>
-    <hyperlink ref="D134" r:id="rId92"/>
-    <hyperlink ref="D135" r:id="rId93"/>
-    <hyperlink ref="D136" r:id="rId94"/>
-    <hyperlink ref="D137" r:id="rId95"/>
-    <hyperlink ref="D138" r:id="rId96"/>
-    <hyperlink ref="D139" r:id="rId97"/>
-    <hyperlink ref="D140" r:id="rId98"/>
-    <hyperlink ref="D141" r:id="rId99"/>
-    <hyperlink ref="D142" r:id="rId100"/>
-    <hyperlink ref="D143" r:id="rId101"/>
-    <hyperlink ref="D144" r:id="rId102"/>
-    <hyperlink ref="D145" r:id="rId103"/>
-    <hyperlink ref="D146" r:id="rId104"/>
-    <hyperlink ref="D147" r:id="rId105"/>
-    <hyperlink ref="D149" r:id="rId106"/>
-    <hyperlink ref="D150" r:id="rId107"/>
-    <hyperlink ref="D152" r:id="rId108"/>
-    <hyperlink ref="D153" r:id="rId109"/>
-    <hyperlink ref="D154" r:id="rId110"/>
-    <hyperlink ref="E151" r:id="rId111"/>
-    <hyperlink ref="D156" r:id="rId112"/>
-    <hyperlink ref="D157" r:id="rId113"/>
-    <hyperlink ref="D159" r:id="rId114"/>
-    <hyperlink ref="D160" r:id="rId115"/>
-    <hyperlink ref="D163" r:id="rId116"/>
-    <hyperlink ref="D166" r:id="rId117"/>
-    <hyperlink ref="D167" r:id="rId118"/>
-    <hyperlink ref="D168" r:id="rId119"/>
-    <hyperlink ref="D169" r:id="rId120"/>
-    <hyperlink ref="D170" r:id="rId121"/>
-    <hyperlink ref="D171" r:id="rId122"/>
-    <hyperlink ref="D175" r:id="rId123"/>
-    <hyperlink ref="D176" r:id="rId124"/>
-    <hyperlink ref="D177" r:id="rId125"/>
-    <hyperlink ref="F177" r:id="rId126" display="tel:9038724147"/>
-    <hyperlink ref="D178" r:id="rId127"/>
-    <hyperlink ref="D179" r:id="rId128"/>
-    <hyperlink ref="D181" r:id="rId129"/>
-    <hyperlink ref="D182" r:id="rId130"/>
-    <hyperlink ref="D184" r:id="rId131"/>
-    <hyperlink ref="D185" r:id="rId132"/>
-    <hyperlink ref="D186" r:id="rId133"/>
-    <hyperlink ref="D187" r:id="rId134"/>
-    <hyperlink ref="D188" r:id="rId135"/>
-    <hyperlink ref="D189" r:id="rId136"/>
-    <hyperlink ref="D192" r:id="rId137"/>
-    <hyperlink ref="D193" r:id="rId138"/>
-    <hyperlink ref="D195" r:id="rId139"/>
-    <hyperlink ref="D196" r:id="rId140"/>
+    <hyperlink ref="D31" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D32" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="F8" r:id="rId4" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D22" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D25" r:id="rId6" display="mailto:official@younghorizonsschool.com" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="D26" r:id="rId7" display="mailto:iwanttojoin@siskol.edu.in" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="D27" r:id="rId8" display="mailto:lcgvm2012@gmail.com" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="D30" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D33" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="D35" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="D37" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="D41" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="D42" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="D43" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="D47" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D48" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="D49" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="D51" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="D53" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="D54" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="D55" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="D56" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="D57" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="D58" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="D59" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="D60" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="D61" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="D62" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="D63" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="D64" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="D65" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="D66" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="D67" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="D68" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="D69" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="D70" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="D71" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="D72" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="D73" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="D75" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="D78" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="D79" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="D80" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="D81" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="D85" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="D88" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="D89" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="D91" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="D2" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="D28" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="E2" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="D3" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="D4" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="E4" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="D5" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="D7" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="D6" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="E6" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="D8" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="E8" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="D9" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="D10" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="D12" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="D13" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="E13" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="D14" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="E14" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="D15" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="D17" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="D18" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="E18" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="D19" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="D38" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="D40" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="D44" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="D45" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="D82" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="D83" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="D84" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="D86" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="D87" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="D90" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="D127" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="D128" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="D129" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="D130" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="D131" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="D132" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="D133" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="D134" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="D135" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="D136" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="D137" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="D138" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="D139" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="D140" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="D141" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="D142" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="D143" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="D144" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="D145" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="D146" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="D147" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="D149" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="D150" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="D152" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="D153" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="D154" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="E151" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="D156" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="D157" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="D159" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
+    <hyperlink ref="D160" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
+    <hyperlink ref="D163" r:id="rId116" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
+    <hyperlink ref="D166" r:id="rId117" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
+    <hyperlink ref="D167" r:id="rId118" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
+    <hyperlink ref="D168" r:id="rId119" xr:uid="{00000000-0004-0000-0100-000076000000}"/>
+    <hyperlink ref="D169" r:id="rId120" xr:uid="{00000000-0004-0000-0100-000077000000}"/>
+    <hyperlink ref="D170" r:id="rId121" xr:uid="{00000000-0004-0000-0100-000078000000}"/>
+    <hyperlink ref="D171" r:id="rId122" xr:uid="{00000000-0004-0000-0100-000079000000}"/>
+    <hyperlink ref="D175" r:id="rId123" xr:uid="{00000000-0004-0000-0100-00007A000000}"/>
+    <hyperlink ref="D176" r:id="rId124" xr:uid="{00000000-0004-0000-0100-00007B000000}"/>
+    <hyperlink ref="D177" r:id="rId125" xr:uid="{00000000-0004-0000-0100-00007C000000}"/>
+    <hyperlink ref="F177" r:id="rId126" display="tel:9038724147" xr:uid="{00000000-0004-0000-0100-00007D000000}"/>
+    <hyperlink ref="D178" r:id="rId127" xr:uid="{00000000-0004-0000-0100-00007E000000}"/>
+    <hyperlink ref="D179" r:id="rId128" xr:uid="{00000000-0004-0000-0100-00007F000000}"/>
+    <hyperlink ref="D181" r:id="rId129" xr:uid="{00000000-0004-0000-0100-000080000000}"/>
+    <hyperlink ref="D182" r:id="rId130" xr:uid="{00000000-0004-0000-0100-000081000000}"/>
+    <hyperlink ref="D184" r:id="rId131" xr:uid="{00000000-0004-0000-0100-000082000000}"/>
+    <hyperlink ref="D185" r:id="rId132" xr:uid="{00000000-0004-0000-0100-000083000000}"/>
+    <hyperlink ref="D186" r:id="rId133" xr:uid="{00000000-0004-0000-0100-000084000000}"/>
+    <hyperlink ref="D187" r:id="rId134" xr:uid="{00000000-0004-0000-0100-000085000000}"/>
+    <hyperlink ref="D188" r:id="rId135" xr:uid="{00000000-0004-0000-0100-000086000000}"/>
+    <hyperlink ref="D189" r:id="rId136" xr:uid="{00000000-0004-0000-0100-000087000000}"/>
+    <hyperlink ref="D192" r:id="rId137" xr:uid="{00000000-0004-0000-0100-000088000000}"/>
+    <hyperlink ref="D193" r:id="rId138" xr:uid="{00000000-0004-0000-0100-000089000000}"/>
+    <hyperlink ref="D195" r:id="rId139" xr:uid="{00000000-0004-0000-0100-00008A000000}"/>
+    <hyperlink ref="D196" r:id="rId140" xr:uid="{00000000-0004-0000-0100-00008B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId141"/>
@@ -13117,11 +13118,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S57" sqref="S57"/>
+    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13248,6 +13249,7 @@
         <v>5</v>
       </c>
       <c r="T2" s="10">
+        <f>SUM(O2:S2)</f>
         <v>19</v>
       </c>
       <c r="U2" s="10">
@@ -13291,10 +13293,11 @@
         <v>5</v>
       </c>
       <c r="T3" s="10">
-        <v>19</v>
+        <f t="shared" ref="T3:T54" si="0">SUM(O3:S3)</f>
+        <v>21</v>
       </c>
       <c r="U3" s="10">
-        <f t="shared" ref="U3:U35" si="0">ROUND(T3/5,0)</f>
+        <f t="shared" ref="U3:U54" si="1">ROUND(T3/5,0)</f>
         <v>4</v>
       </c>
       <c r="V3" s="10" t="s">
@@ -13334,10 +13337,11 @@
         <v>5</v>
       </c>
       <c r="T4" s="10">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="U4" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="V4" s="10" t="s">
@@ -13377,10 +13381,11 @@
         <v>4</v>
       </c>
       <c r="T5" s="10">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="U5" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="V5" s="10" t="s">
@@ -13420,10 +13425,11 @@
         <v>5</v>
       </c>
       <c r="T6" s="10">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="U6" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="V6" s="10" t="s">
@@ -13463,10 +13469,11 @@
         <v>4</v>
       </c>
       <c r="T7" s="10">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="U7" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="V7" s="10" t="s">
@@ -13506,10 +13513,11 @@
         <v>3</v>
       </c>
       <c r="T8" s="10">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="U8" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V8" s="10" t="s">
@@ -13546,10 +13554,11 @@
         <v>0</v>
       </c>
       <c r="T9" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U9" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V9" s="10" t="s">
@@ -13586,10 +13595,11 @@
         <v>0</v>
       </c>
       <c r="T10" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U10" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V10" s="10" t="s">
@@ -13627,10 +13637,11 @@
         <v>0</v>
       </c>
       <c r="T11" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U11" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V11" s="10" t="s">
@@ -13667,10 +13678,11 @@
         <v>0</v>
       </c>
       <c r="T12" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U12" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V12" s="10" t="s">
@@ -13707,10 +13719,11 @@
         <v>0</v>
       </c>
       <c r="T13" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U13" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V13" s="10" t="s">
@@ -13747,10 +13760,11 @@
         <v>0</v>
       </c>
       <c r="T14" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U14" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V14" s="10" t="s">
@@ -13787,10 +13801,11 @@
         <v>0</v>
       </c>
       <c r="T15" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U15" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V15" s="10" t="s">
@@ -13827,10 +13842,11 @@
         <v>0</v>
       </c>
       <c r="T16" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U16" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V16" s="10" t="s">
@@ -13867,10 +13883,11 @@
         <v>0</v>
       </c>
       <c r="T17" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U17" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V17" s="10" t="s">
@@ -13907,10 +13924,11 @@
         <v>0</v>
       </c>
       <c r="T18" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U18" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V18" s="10" t="s">
@@ -13947,10 +13965,11 @@
         <v>0</v>
       </c>
       <c r="T19" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U19" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V19" s="10" t="s">
@@ -13968,7 +13987,7 @@
       <c r="D20" s="43" t="s">
         <v>336</v>
       </c>
-      <c r="K20" s="97" t="s">
+      <c r="K20" s="90" t="s">
         <v>367</v>
       </c>
       <c r="L20" s="10"/>
@@ -13988,10 +14007,11 @@
         <v>0</v>
       </c>
       <c r="T20" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U20" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V20" s="10" t="s">
@@ -14029,10 +14049,11 @@
         <v>0</v>
       </c>
       <c r="T21" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U21" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V21" s="10" t="s">
@@ -14069,10 +14090,11 @@
         <v>0</v>
       </c>
       <c r="T22" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U22" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V22" s="10" t="s">
@@ -14110,10 +14132,11 @@
         <v>0</v>
       </c>
       <c r="T23" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U23" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V23" s="10" t="s">
@@ -14151,10 +14174,11 @@
         <v>0</v>
       </c>
       <c r="T24" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U24" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V24" s="10" t="s">
@@ -14192,10 +14216,11 @@
         <v>0</v>
       </c>
       <c r="T25" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U25" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V25" s="10" t="s">
@@ -14233,10 +14258,11 @@
         <v>0</v>
       </c>
       <c r="T26" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U26" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V26" s="10" t="s">
@@ -14273,10 +14299,11 @@
         <v>0</v>
       </c>
       <c r="T27" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U27" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V27" s="10" t="s">
@@ -14313,10 +14340,11 @@
         <v>0</v>
       </c>
       <c r="T28" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U28" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V28" s="10" t="s">
@@ -14354,10 +14382,11 @@
         <v>0</v>
       </c>
       <c r="T29" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U29" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V29" s="10" t="s">
@@ -14395,10 +14424,11 @@
         <v>0</v>
       </c>
       <c r="T30" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U30" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V30" s="10" t="s">
@@ -14436,10 +14466,11 @@
         <v>0</v>
       </c>
       <c r="T31" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U31" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V31" s="10" t="s">
@@ -14476,10 +14507,11 @@
         <v>0</v>
       </c>
       <c r="T32" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U32" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V32" s="10" t="s">
@@ -14516,10 +14548,11 @@
         <v>0</v>
       </c>
       <c r="T33" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U33" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V33" s="10" t="s">
@@ -14556,10 +14589,11 @@
         <v>0</v>
       </c>
       <c r="T34" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U34" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V34" s="10" t="s">
@@ -14596,10 +14630,11 @@
         <v>0</v>
       </c>
       <c r="T35" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U35" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V35" s="10" t="s">
@@ -14642,10 +14677,11 @@
         <v>4</v>
       </c>
       <c r="T36" s="10">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="U36" s="10">
-        <f t="shared" ref="U36:U54" si="1">ROUND(T36/5,0)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="V36" s="10" t="s">
@@ -14688,6 +14724,7 @@
         <v>4</v>
       </c>
       <c r="T37" s="10">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="U37" s="10">
@@ -14731,6 +14768,7 @@
         <v>3</v>
       </c>
       <c r="T38" s="10">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="U38" s="10">
@@ -14774,6 +14812,7 @@
         <v>5</v>
       </c>
       <c r="T39" s="10">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="U39" s="10">
@@ -14817,6 +14856,7 @@
         <v>5</v>
       </c>
       <c r="T40" s="10">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="U40" s="10">
@@ -14860,6 +14900,7 @@
         <v>0</v>
       </c>
       <c r="T41" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U41" s="10">
@@ -14903,6 +14944,7 @@
         <v>0</v>
       </c>
       <c r="T42" s="10">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="U42" s="10">
@@ -14949,6 +14991,7 @@
         <v>4</v>
       </c>
       <c r="T43" s="10">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="U43" s="10">
@@ -14992,6 +15035,7 @@
         <v>3</v>
       </c>
       <c r="T44" s="10">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="U44" s="10">
@@ -15035,6 +15079,7 @@
         <v>5</v>
       </c>
       <c r="T45" s="10">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="U45" s="10">
@@ -15078,6 +15123,7 @@
         <v>3</v>
       </c>
       <c r="T46" s="10">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="U46" s="10">
@@ -15092,7 +15138,7 @@
       <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="98" t="s">
+      <c r="B47" s="91" t="s">
         <v>733</v>
       </c>
       <c r="D47" s="45" t="s">
@@ -15121,6 +15167,7 @@
         <v>5</v>
       </c>
       <c r="T47" s="10">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="U47" s="10">
@@ -15164,9 +15211,11 @@
         <v>5</v>
       </c>
       <c r="T48" s="10">
-        <v>21</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="U48" s="10">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="V48" s="10" t="s">
@@ -15209,7 +15258,8 @@
         <v>5</v>
       </c>
       <c r="T49" s="10">
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="U49" s="10">
         <f t="shared" si="1"/>
@@ -15252,6 +15302,7 @@
         <v>3</v>
       </c>
       <c r="T50" s="10">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="U50" s="10">
@@ -15295,6 +15346,7 @@
         <v>5</v>
       </c>
       <c r="T51" s="10">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="U51" s="10">
@@ -15338,6 +15390,7 @@
         <v>5</v>
       </c>
       <c r="T52" s="10">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="U52" s="10">
@@ -15381,6 +15434,7 @@
         <v>5</v>
       </c>
       <c r="T53" s="10">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="U53" s="10">
@@ -15424,6 +15478,7 @@
         <v>5</v>
       </c>
       <c r="T54" s="10">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="U54" s="10">
@@ -16561,23 +16616,23 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Initial,Potential,Customer,Workshop Fixed,Reject,Not-Contacted,Ex-Customer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Rahul Dutta,Sayan Basak,Anirban Chakraborty,Debashish Nath"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Technical,Non-Technical"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C36" r:id="rId1"/>
-    <hyperlink ref="C37" r:id="rId2"/>
-    <hyperlink ref="D41" r:id="rId3" display="https://www.google.com/search?sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;tbs=lf:1,lf_ui:2&amp;tbm=lcl&amp;sxsrf=ACQVn0-yjBygfThguW8-plBveMrMzDiPGw:1704870884151&amp;q=engineering+colleges+in+south+calcutta&amp;rflfq=1&amp;num=10&amp;sa=X&amp;ved=2ahUKEwjQ47_7otKDAxUve2wGHY_pCzEQjGp6BAgXEAE&amp;biw=1536&amp;bih=730&amp;dpr=1.25"/>
-    <hyperlink ref="C43" r:id="rId4"/>
-    <hyperlink ref="D47" r:id="rId5" display="https://www.google.com/search?q=engineering+colleges+kolkata&amp;sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;biw=1536&amp;bih=730&amp;tbm=lcl&amp;sxsrf=ACQVn09cs4SfDApVNizAZQHyNbKrHkG1kw%3A1704870889163&amp;ei=6UOeZYunCcqWseMP2bOt0A4&amp;ved=0ahUKEwjLv_H9otKDAxVKS2wGHdlZC-oQ4dUDCAk&amp;uact=5&amp;oq=engineering+colleges+kolkata&amp;gs_lp=Eg1nd3Mtd2l6LWxvY2FsIhxlbmdpbmVlcmluZyBjb2xsZWdlcyBrb2xrYXRhMgUQABiABDIGEAAYFhgeMgYQABgWGB4yCBAAGBYYHhgPMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeSPErUNUEWOgmcAF4AJABAZgBqwGgAb0XqgEEMC4yM7gBA8gBAPgBAcICCxAAGIAEGIoFGIYDwgIEECMYJ8ICCxAAGIAEGIoFGJECwgIKEAAYgAQYFBiHAsICDhAAGIAEGIoFGJECGMkDiAYB&amp;sclient=gws-wiz-local"/>
-    <hyperlink ref="C49" r:id="rId6"/>
+    <hyperlink ref="C36" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C37" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D41" r:id="rId3" display="https://www.google.com/search?sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;tbs=lf:1,lf_ui:2&amp;tbm=lcl&amp;sxsrf=ACQVn0-yjBygfThguW8-plBveMrMzDiPGw:1704870884151&amp;q=engineering+colleges+in+south+calcutta&amp;rflfq=1&amp;num=10&amp;sa=X&amp;ved=2ahUKEwjQ47_7otKDAxUve2wGHY_pCzEQjGp6BAgXEAE&amp;biw=1536&amp;bih=730&amp;dpr=1.25" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C43" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="D47" r:id="rId5" display="https://www.google.com/search?q=engineering+colleges+kolkata&amp;sca_esv=597127733&amp;rlz=1C1CHBF_enAU1047AU1047&amp;biw=1536&amp;bih=730&amp;tbm=lcl&amp;sxsrf=ACQVn09cs4SfDApVNizAZQHyNbKrHkG1kw%3A1704870889163&amp;ei=6UOeZYunCcqWseMP2bOt0A4&amp;ved=0ahUKEwjLv_H9otKDAxVKS2wGHdlZC-oQ4dUDCAk&amp;uact=5&amp;oq=engineering+colleges+kolkata&amp;gs_lp=Eg1nd3Mtd2l6LWxvY2FsIhxlbmdpbmVlcmluZyBjb2xsZWdlcyBrb2xrYXRhMgUQABiABDIGEAAYFhgeMgYQABgWGB4yCBAAGBYYHhgPMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeMgYQABgWGB4yBhAAGBYYHjIGEAAYFhgeSPErUNUEWOgmcAF4AJABAZgBqwGgAb0XqgEEMC4yM7gBA8gBAPgBAcICCxAAGIAEGIoFGIYDwgIEECMYJ8ICCxAAGIAEGIoFGJECwgIKEAAYgAQYFBiHAsICDhAAGIAEGIoFGJECGMkDiAYB&amp;sclient=gws-wiz-local" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="C49" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -16586,7 +16641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16708,7 +16763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16791,7 +16846,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
@@ -18028,8 +18083,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp"/>
-    <hyperlink ref="C6" r:id="rId2" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w"/>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.google.com/search?q=panchasayar+siksha+niketan&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKnlKkWvrpmDIvMzNnJR8ZC_8s6gNQ%3A1703524925488&amp;ei=PbqJZaauHY2KnesPo--TuAo&amp;gs_ssp=eJzj4tFP1zc0MqnMzTa1TDNgtFI1qDBONDAyNzRPNU1LM0xOTkuyAgqZpJmZmJgnGZgZGSWnpSV5SRUk5iVnJBYnViYWKRRnZhdnJCrkZWanliTmAQC7Qxln&amp;oq=panchasayar+s&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDXBhbmNoYXNheWFyIHMqAggAMhQQLhivARjHARimAxioAxiABBiOBTIFEAAYgAQyBRAAGIAEMgsQLhiABBioAxidAzIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgAQyCBAAGIAEGMsBMggQABiABBjLATIjEC4YrwEYxwEYpgMYqAMYgAQYjgUYlwUY3AQY3gQY4ATYAQNIuzhQmhhYmCVwAXgBkAEAmAGvAqAB1gSqAQUyLTEuMbgBAcgBAPgBAcICChAAGEcY1gQYsAPCAg0QABiABBiKBRhDGLADwgIcEC4YgAQYigUYQxjHARivARjIAxiwAxiOBdgBAcICGRAuGIAEGIoFGEMYxwEYrwEYyAMYsAPYAQHCAg4QABjkAhjWBBiwA9gBAsICEBAuGEMYnQMYqAMYgAQYigXCAhAQLhiABBiKBRhDGKgDGJ0DwgIWEC4YQxivARjHARimAxioAxiABBiKBcICChAAGIAEGBQYhwLCAh8QLhhDGJ0DGKgDGIAEGIoFGJcFGNwEGN4EGOAE2AED4gMEGAAgQYgGAZAGDroGBggBEAEYCLoGBggCEAEYCboGBggDEAEYFA&amp;sclient=gws-wiz-serp" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId2" display="https://www.google.com/search?q=miranda+high+school&amp;sca_esv=593615924&amp;rlz=1C1CHBF_enAU1047AU1047&amp;sxsrf=AM9HkKmR8dFtasrVNGZkMFIxGz5Wq06ZjA%3A1703525037148&amp;ei=rbqJZczSCOCWjuMPsMy_8AM&amp;oq=miranda+high+&amp;gs_lp=Egxnd3Mtd2l6LXNlcnAiDW1pcmFuZGEgaGlnaCAqAggAMg0QABiABBgUGIcCGMkDMgUQABiABDILEAAYgAQYigUYkgMyBRAAGIAEMgUQABiABDIKEAAYgAQYFBiHAjIFEAAYgAQyBRAAGIAEMgUQABiABDIFEAAYgARI7RNQ6AZY6AZwAXgAkAEAmAH0BqABuAyqAQM2LTK4AQHIAQD4AQHCAgoQABhHGNYEGLAD4gMEGAAgQYgGAZAGCA&amp;sclient=gws-wiz-serp&amp;lqi=ChNtaXJhbmRhIGhpZ2ggc2Nob29sSN-07OW4roCACForEAAQARACGAAYARgCIhNtaXJhbmRhIGhpZ2ggc2Nob29sKggIAhAAEAEQApIBBnNjaG9vbJoBI0NoWkRTVWhOTUc5blMwVkpRMEZuU1VOUGNqUnVSbVZuRUFFqgE7EAEyHhABIhpTQ3iPFiqMHHb-9vGb0lli1Rpc5Z8xE87GgDIXEAIiE21pcmFuZGEgaGlnaCBzY2hvb2w" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update AI Schools & Colleges
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
+++ b/Offline/BusinessManagement/Marketing/AI marketing/AI Workshop Schools-Colleges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Marketing\AI marketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68691FBD-0EC5-429B-AF44-B314A083C816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FC42C8-0EB8-45C5-8ED1-23A342F7B011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="506" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -3350,7 +3350,7 @@
   <dimension ref="B1:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3616,7 +3616,7 @@
       </c>
       <c r="D11" s="11">
         <f>COUNTIF('School-Details'!V:V,C11)</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="87" t="s">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="D16" s="11">
         <f>COUNTIF('School-Details'!V:V,C16)</f>
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F16" s="19">
         <v>45383</v>
@@ -4303,11 +4303,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V196"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F183" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3:M196"/>
+      <selection pane="bottomRight" activeCell="V67" sqref="V67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -7323,7 +7323,7 @@
         <v>4</v>
       </c>
       <c r="V67" s="7" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="68" spans="1:22" ht="14.4" customHeight="1">
@@ -7411,7 +7411,7 @@
         <v>4</v>
       </c>
       <c r="V69" s="7" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:22" ht="14.4" customHeight="1">
@@ -16852,7 +16852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+    <sheetView topLeftCell="A162" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>

</xml_diff>